<commit_message>
Going through Alt1 in detail
</commit_message>
<xml_diff>
--- a/CH-130 FIFO.xlsx
+++ b/CH-130 FIFO.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD323AAE-CB30-44DA-8905-00A223AA7C30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{053A694F-D78A-4A05-AB11-064323AD78F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Original" sheetId="1" r:id="rId1"/>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="23">
   <si>
     <t>Question</t>
   </si>
@@ -125,6 +125,15 @@
   </si>
   <si>
     <t>https://www.linkedin.com/feed/update/urn:li:activity:7253147842951696385/</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>g</t>
+  </si>
+  <si>
+    <t>e</t>
   </si>
 </sst>
 </file>
@@ -1602,7 +1611,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4C65EB1-3462-4A10-A150-765232CDCA14}">
   <dimension ref="A1:O36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView topLeftCell="A12" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
@@ -2223,10 +2232,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CBB5195-1E8A-4CD7-99EA-F5B23BFB852F}">
-  <dimension ref="A1:O36"/>
+  <dimension ref="A1:O301"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17:E25"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17:G301"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -2597,6 +2606,15 @@
       <c r="E16" s="7" t="s">
         <v>4</v>
       </c>
+      <c r="G16" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="I16" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="K16" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="17" spans="1:15" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
@@ -2623,6 +2641,54 @@
       <c r="E17" s="7">
         <v>27</v>
       </c>
+      <c r="G17" s="5" cm="1">
+        <f t="array" ref="G17:G301">_xlfn.LET(
+    _xlpm.a, B3:B13,
+    _xlpm.b, C3:C13,
+    _xlpm.c, D3:D13,
+    _xlpm.d, _xlfn._xlws.FILTER(_xlfn.HSTACK(_xlpm.a, _xlpm.c), _xlpm.b = "Input"),
+    _xlpm.e, --_xlfn.TEXTSPLIT(_xlfn.CONCAT(REPT(_xlfn.TAKE(_xlpm.d, , 1) &amp; " ", _xlfn.TAKE(_xlpm.d, , -1))), , " ", 1),
+    _xlpm.f, _xlfn._xlws.FILTER(_xlfn.HSTACK(_xlpm.a &amp; "-" &amp; RIGHT(_xlpm.b), _xlpm.c), _xlpm.b &lt;&gt; "Input"),
+    _xlpm.g, _xlfn.TEXTSPLIT(_xlfn.CONCAT(REPT(_xlfn.TAKE(_xlpm.f, , 1) &amp; " ", _xlfn.TAKE(_xlpm.f, , -1))), "-", " ", 1),
+    _xlpm.h, --_xlfn.TAKE(_xlpm.g, , 1),
+    _xlpm.e
+)</f>
+        <v>45455</v>
+      </c>
+      <c r="I17" s="5" t="str" cm="1">
+        <f t="array" ref="I17:J21">_xlfn.LET(
+    _xlpm.a, B3:B13,
+    _xlpm.b, C3:C13,
+    _xlpm.c, D3:D13,
+    _xlpm.d, _xlfn._xlws.FILTER(_xlfn.HSTACK(_xlpm.a, _xlpm.c), _xlpm.b = "Input"),
+    _xlpm.e, --_xlfn.TEXTSPLIT(_xlfn.CONCAT(REPT(_xlfn.TAKE(_xlpm.d, , 1) &amp; " ", _xlfn.TAKE(_xlpm.d, , -1))), , " ", 1),
+    _xlpm.f, _xlfn._xlws.FILTER(_xlfn.HSTACK(_xlpm.a &amp; "-" &amp; RIGHT(_xlpm.b), _xlpm.c), _xlpm.b &lt;&gt; "Input"),
+    _xlpm.g, _xlfn.TEXTSPLIT(_xlfn.CONCAT(REPT(_xlfn.TAKE(_xlpm.f, , 1) &amp; " ", _xlfn.TAKE(_xlpm.f, , -1))), "-", " ", 1),
+    _xlpm.h, --_xlfn.TAKE(_xlpm.g, , 1),
+    _xlpm.f
+)</f>
+        <v>45457-A</v>
+      </c>
+      <c r="J17">
+        <v>27</v>
+      </c>
+      <c r="K17" s="5" t="str" cm="1">
+        <f t="array" ref="K17:L198">_xlfn.LET(
+    _xlpm.a, B3:B13,
+    _xlpm.b, C3:C13,
+    _xlpm.c, D3:D13,
+    _xlpm.d, _xlfn._xlws.FILTER(_xlfn.HSTACK(_xlpm.a, _xlpm.c), _xlpm.b = "Input"),
+    _xlpm.e, --_xlfn.TEXTSPLIT(_xlfn.CONCAT(REPT(_xlfn.TAKE(_xlpm.d, , 1) &amp; " ", _xlfn.TAKE(_xlpm.d, , -1))), , " ", 1),
+    _xlpm.f, _xlfn._xlws.FILTER(_xlfn.HSTACK(_xlpm.a &amp; "-" &amp; RIGHT(_xlpm.b), _xlpm.c), _xlpm.b &lt;&gt; "Input"),
+    _xlpm.g, _xlfn.TEXTSPLIT(_xlfn.CONCAT(REPT(_xlfn.TAKE(_xlpm.f, , 1) &amp; " ", _xlfn.TAKE(_xlpm.f, , -1))), "-", " ", 1),
+    _xlpm.h, --_xlfn.TAKE(_xlpm.g, , 1),
+    _xlpm.g
+)</f>
+        <v>45457</v>
+      </c>
+      <c r="L17" t="str">
+        <v>A</v>
+      </c>
       <c r="O17" s="2"/>
     </row>
     <row r="18" spans="1:15" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
@@ -2639,6 +2705,21 @@
       <c r="E18" s="7">
         <v>51</v>
       </c>
+      <c r="G18" s="5">
+        <v>45455</v>
+      </c>
+      <c r="I18" s="5" t="str">
+        <v>45487-B</v>
+      </c>
+      <c r="J18">
+        <v>58</v>
+      </c>
+      <c r="K18" s="5" t="str">
+        <v>45457</v>
+      </c>
+      <c r="L18" t="str">
+        <v>A</v>
+      </c>
       <c r="O18" s="2"/>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
@@ -2654,6 +2735,21 @@
       </c>
       <c r="E19" s="7">
         <v>7</v>
+      </c>
+      <c r="G19" s="5">
+        <v>45455</v>
+      </c>
+      <c r="I19" s="5" t="str">
+        <v>45489-C</v>
+      </c>
+      <c r="J19">
+        <v>32</v>
+      </c>
+      <c r="K19" s="5" t="str">
+        <v>45457</v>
+      </c>
+      <c r="L19" t="str">
+        <v>A</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
@@ -2670,6 +2766,21 @@
       <c r="E20" s="7">
         <v>20</v>
       </c>
+      <c r="G20" s="5">
+        <v>45455</v>
+      </c>
+      <c r="I20" s="5" t="str">
+        <v>45520-D</v>
+      </c>
+      <c r="J20">
+        <v>42</v>
+      </c>
+      <c r="K20" s="5" t="str">
+        <v>45457</v>
+      </c>
+      <c r="L20" t="str">
+        <v>A</v>
+      </c>
       <c r="O20" s="2"/>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
@@ -2686,6 +2797,21 @@
       <c r="E21" s="7">
         <v>12</v>
       </c>
+      <c r="G21" s="5">
+        <v>45455</v>
+      </c>
+      <c r="I21" s="5" t="str">
+        <v>45523-E</v>
+      </c>
+      <c r="J21">
+        <v>23</v>
+      </c>
+      <c r="K21" s="5" t="str">
+        <v>45457</v>
+      </c>
+      <c r="L21" t="str">
+        <v>A</v>
+      </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
@@ -2701,6 +2827,16 @@
       <c r="E22" s="7">
         <v>3</v>
       </c>
+      <c r="G22" s="5">
+        <v>45455</v>
+      </c>
+      <c r="I22" s="5"/>
+      <c r="K22" s="5" t="str">
+        <v>45457</v>
+      </c>
+      <c r="L22" t="str">
+        <v>A</v>
+      </c>
       <c r="O22" s="2"/>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
@@ -2717,6 +2853,16 @@
       <c r="E23" s="7">
         <v>38</v>
       </c>
+      <c r="G23" s="5">
+        <v>45455</v>
+      </c>
+      <c r="I23" s="5"/>
+      <c r="K23" s="5" t="str">
+        <v>45457</v>
+      </c>
+      <c r="L23" t="str">
+        <v>A</v>
+      </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B24" s="7" t="str">
@@ -2731,6 +2877,16 @@
       <c r="E24" s="7">
         <v>1</v>
       </c>
+      <c r="G24" s="5">
+        <v>45455</v>
+      </c>
+      <c r="I24" s="5"/>
+      <c r="K24" s="5" t="str">
+        <v>45457</v>
+      </c>
+      <c r="L24" t="str">
+        <v>A</v>
+      </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B25" s="7" t="str">
@@ -2744,46 +2900,2629 @@
       </c>
       <c r="E25" s="7">
         <v>23</v>
+      </c>
+      <c r="G25" s="5">
+        <v>45455</v>
+      </c>
+      <c r="I25" s="5"/>
+      <c r="K25" s="5" t="str">
+        <v>45457</v>
+      </c>
+      <c r="L25" t="str">
+        <v>A</v>
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B26" s="7"/>
       <c r="C26" s="7"/>
       <c r="E26" s="7"/>
+      <c r="G26" s="5">
+        <v>45455</v>
+      </c>
+      <c r="I26" s="5"/>
+      <c r="K26" s="5" t="str">
+        <v>45457</v>
+      </c>
+      <c r="L26" t="str">
+        <v>A</v>
+      </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B27" s="7"/>
       <c r="D27" s="7"/>
+      <c r="G27" s="5">
+        <v>45455</v>
+      </c>
+      <c r="I27" s="5"/>
+      <c r="K27" s="5" t="str">
+        <v>45457</v>
+      </c>
+      <c r="L27" t="str">
+        <v>A</v>
+      </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B28" s="7"/>
       <c r="D28" s="7"/>
+      <c r="G28" s="5">
+        <v>45455</v>
+      </c>
+      <c r="I28" s="5"/>
+      <c r="K28" s="5" t="str">
+        <v>45457</v>
+      </c>
+      <c r="L28" t="str">
+        <v>A</v>
+      </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B29" s="7"/>
+      <c r="G29" s="5">
+        <v>45455</v>
+      </c>
+      <c r="I29" s="5"/>
+      <c r="K29" s="5" t="str">
+        <v>45457</v>
+      </c>
+      <c r="L29" t="str">
+        <v>A</v>
+      </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B30" s="7"/>
       <c r="D30" s="7"/>
+      <c r="G30" s="5">
+        <v>45455</v>
+      </c>
+      <c r="I30" s="5"/>
+      <c r="K30" s="5" t="str">
+        <v>45457</v>
+      </c>
+      <c r="L30" t="str">
+        <v>A</v>
+      </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B31" s="7"/>
       <c r="D31" s="7"/>
+      <c r="G31" s="5">
+        <v>45455</v>
+      </c>
+      <c r="I31" s="5"/>
+      <c r="K31" s="5" t="str">
+        <v>45457</v>
+      </c>
+      <c r="L31" t="str">
+        <v>A</v>
+      </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B32" s="7"/>
-    </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="G32" s="5">
+        <v>45455</v>
+      </c>
+      <c r="I32" s="5"/>
+      <c r="K32" s="5" t="str">
+        <v>45457</v>
+      </c>
+      <c r="L32" t="str">
+        <v>A</v>
+      </c>
+    </row>
+    <row r="33" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B33" s="7"/>
-    </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="G33" s="5">
+        <v>45455</v>
+      </c>
+      <c r="I33" s="5"/>
+      <c r="K33" s="5" t="str">
+        <v>45457</v>
+      </c>
+      <c r="L33" t="str">
+        <v>A</v>
+      </c>
+    </row>
+    <row r="34" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B34" s="7"/>
-    </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="G34" s="5">
+        <v>45455</v>
+      </c>
+      <c r="I34" s="5"/>
+      <c r="K34" s="5" t="str">
+        <v>45457</v>
+      </c>
+      <c r="L34" t="str">
+        <v>A</v>
+      </c>
+    </row>
+    <row r="35" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B35" s="7"/>
-    </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="G35" s="5">
+        <v>45455</v>
+      </c>
+      <c r="I35" s="5"/>
+      <c r="K35" s="5" t="str">
+        <v>45457</v>
+      </c>
+      <c r="L35" t="str">
+        <v>A</v>
+      </c>
+    </row>
+    <row r="36" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B36" s="7"/>
+      <c r="G36" s="5">
+        <v>45455</v>
+      </c>
+      <c r="I36" s="5"/>
+      <c r="K36" s="5" t="str">
+        <v>45457</v>
+      </c>
+      <c r="L36" t="str">
+        <v>A</v>
+      </c>
+    </row>
+    <row r="37" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="G37" s="5">
+        <v>45455</v>
+      </c>
+      <c r="I37" s="5"/>
+      <c r="K37" s="5" t="str">
+        <v>45457</v>
+      </c>
+      <c r="L37" t="str">
+        <v>A</v>
+      </c>
+    </row>
+    <row r="38" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="G38" s="5">
+        <v>45455</v>
+      </c>
+      <c r="I38" s="5"/>
+      <c r="K38" s="5" t="str">
+        <v>45457</v>
+      </c>
+      <c r="L38" t="str">
+        <v>A</v>
+      </c>
+    </row>
+    <row r="39" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="G39" s="5">
+        <v>45455</v>
+      </c>
+      <c r="I39" s="5"/>
+      <c r="K39" s="5" t="str">
+        <v>45457</v>
+      </c>
+      <c r="L39" t="str">
+        <v>A</v>
+      </c>
+    </row>
+    <row r="40" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="G40" s="5">
+        <v>45455</v>
+      </c>
+      <c r="I40" s="5"/>
+      <c r="K40" s="5" t="str">
+        <v>45457</v>
+      </c>
+      <c r="L40" t="str">
+        <v>A</v>
+      </c>
+    </row>
+    <row r="41" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="G41" s="5">
+        <v>45455</v>
+      </c>
+      <c r="I41" s="5"/>
+      <c r="K41" s="5" t="str">
+        <v>45457</v>
+      </c>
+      <c r="L41" t="str">
+        <v>A</v>
+      </c>
+    </row>
+    <row r="42" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="G42" s="5">
+        <v>45455</v>
+      </c>
+      <c r="I42" s="5"/>
+      <c r="K42" s="5" t="str">
+        <v>45457</v>
+      </c>
+      <c r="L42" t="str">
+        <v>A</v>
+      </c>
+    </row>
+    <row r="43" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="G43" s="5">
+        <v>45455</v>
+      </c>
+      <c r="I43" s="5"/>
+      <c r="K43" s="5" t="str">
+        <v>45457</v>
+      </c>
+      <c r="L43" t="str">
+        <v>A</v>
+      </c>
+    </row>
+    <row r="44" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="G44" s="5">
+        <v>45455</v>
+      </c>
+      <c r="I44" s="5"/>
+      <c r="K44" s="5" t="str">
+        <v>45487</v>
+      </c>
+      <c r="L44" t="str">
+        <v>B</v>
+      </c>
+    </row>
+    <row r="45" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="G45" s="5">
+        <v>45455</v>
+      </c>
+      <c r="I45" s="5"/>
+      <c r="K45" s="5" t="str">
+        <v>45487</v>
+      </c>
+      <c r="L45" t="str">
+        <v>B</v>
+      </c>
+    </row>
+    <row r="46" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="G46" s="5">
+        <v>45455</v>
+      </c>
+      <c r="I46" s="5"/>
+      <c r="K46" s="5" t="str">
+        <v>45487</v>
+      </c>
+      <c r="L46" t="str">
+        <v>B</v>
+      </c>
+    </row>
+    <row r="47" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="G47" s="5">
+        <v>45455</v>
+      </c>
+      <c r="I47" s="5"/>
+      <c r="K47" s="5" t="str">
+        <v>45487</v>
+      </c>
+      <c r="L47" t="str">
+        <v>B</v>
+      </c>
+    </row>
+    <row r="48" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="G48" s="5">
+        <v>45455</v>
+      </c>
+      <c r="I48" s="5"/>
+      <c r="K48" s="5" t="str">
+        <v>45487</v>
+      </c>
+      <c r="L48" t="str">
+        <v>B</v>
+      </c>
+    </row>
+    <row r="49" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G49" s="5">
+        <v>45455</v>
+      </c>
+      <c r="I49" s="5"/>
+      <c r="K49" s="5" t="str">
+        <v>45487</v>
+      </c>
+      <c r="L49" t="str">
+        <v>B</v>
+      </c>
+    </row>
+    <row r="50" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G50" s="5">
+        <v>45455</v>
+      </c>
+      <c r="I50" s="5"/>
+      <c r="K50" s="5" t="str">
+        <v>45487</v>
+      </c>
+      <c r="L50" t="str">
+        <v>B</v>
+      </c>
+    </row>
+    <row r="51" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G51" s="5">
+        <v>45455</v>
+      </c>
+      <c r="I51" s="5"/>
+      <c r="K51" s="5" t="str">
+        <v>45487</v>
+      </c>
+      <c r="L51" t="str">
+        <v>B</v>
+      </c>
+    </row>
+    <row r="52" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G52" s="5">
+        <v>45455</v>
+      </c>
+      <c r="I52" s="5"/>
+      <c r="K52" s="5" t="str">
+        <v>45487</v>
+      </c>
+      <c r="L52" t="str">
+        <v>B</v>
+      </c>
+    </row>
+    <row r="53" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G53" s="5">
+        <v>45455</v>
+      </c>
+      <c r="I53" s="5"/>
+      <c r="K53" s="5" t="str">
+        <v>45487</v>
+      </c>
+      <c r="L53" t="str">
+        <v>B</v>
+      </c>
+    </row>
+    <row r="54" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G54" s="5">
+        <v>45455</v>
+      </c>
+      <c r="I54" s="5"/>
+      <c r="K54" s="5" t="str">
+        <v>45487</v>
+      </c>
+      <c r="L54" t="str">
+        <v>B</v>
+      </c>
+    </row>
+    <row r="55" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G55" s="5">
+        <v>45455</v>
+      </c>
+      <c r="I55" s="5"/>
+      <c r="K55" s="5" t="str">
+        <v>45487</v>
+      </c>
+      <c r="L55" t="str">
+        <v>B</v>
+      </c>
+    </row>
+    <row r="56" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G56" s="5">
+        <v>45455</v>
+      </c>
+      <c r="I56" s="5"/>
+      <c r="K56" s="5" t="str">
+        <v>45487</v>
+      </c>
+      <c r="L56" t="str">
+        <v>B</v>
+      </c>
+    </row>
+    <row r="57" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G57" s="5">
+        <v>45455</v>
+      </c>
+      <c r="I57" s="5"/>
+      <c r="K57" s="5" t="str">
+        <v>45487</v>
+      </c>
+      <c r="L57" t="str">
+        <v>B</v>
+      </c>
+    </row>
+    <row r="58" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G58" s="5">
+        <v>45455</v>
+      </c>
+      <c r="I58" s="5"/>
+      <c r="K58" s="5" t="str">
+        <v>45487</v>
+      </c>
+      <c r="L58" t="str">
+        <v>B</v>
+      </c>
+    </row>
+    <row r="59" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G59" s="5">
+        <v>45455</v>
+      </c>
+      <c r="I59" s="5"/>
+      <c r="K59" s="5" t="str">
+        <v>45487</v>
+      </c>
+      <c r="L59" t="str">
+        <v>B</v>
+      </c>
+    </row>
+    <row r="60" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G60" s="5">
+        <v>45455</v>
+      </c>
+      <c r="I60" s="5"/>
+      <c r="K60" s="5" t="str">
+        <v>45487</v>
+      </c>
+      <c r="L60" t="str">
+        <v>B</v>
+      </c>
+    </row>
+    <row r="61" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G61" s="5">
+        <v>45455</v>
+      </c>
+      <c r="I61" s="5"/>
+      <c r="K61" s="5" t="str">
+        <v>45487</v>
+      </c>
+      <c r="L61" t="str">
+        <v>B</v>
+      </c>
+    </row>
+    <row r="62" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G62" s="5">
+        <v>45455</v>
+      </c>
+      <c r="I62" s="5"/>
+      <c r="K62" s="5" t="str">
+        <v>45487</v>
+      </c>
+      <c r="L62" t="str">
+        <v>B</v>
+      </c>
+    </row>
+    <row r="63" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G63" s="5">
+        <v>45455</v>
+      </c>
+      <c r="I63" s="5"/>
+      <c r="K63" s="5" t="str">
+        <v>45487</v>
+      </c>
+      <c r="L63" t="str">
+        <v>B</v>
+      </c>
+    </row>
+    <row r="64" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G64" s="5">
+        <v>45455</v>
+      </c>
+      <c r="I64" s="5"/>
+      <c r="K64" s="5" t="str">
+        <v>45487</v>
+      </c>
+      <c r="L64" t="str">
+        <v>B</v>
+      </c>
+    </row>
+    <row r="65" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G65" s="5">
+        <v>45455</v>
+      </c>
+      <c r="I65" s="5"/>
+      <c r="K65" s="5" t="str">
+        <v>45487</v>
+      </c>
+      <c r="L65" t="str">
+        <v>B</v>
+      </c>
+    </row>
+    <row r="66" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G66" s="5">
+        <v>45455</v>
+      </c>
+      <c r="I66" s="5"/>
+      <c r="K66" s="5" t="str">
+        <v>45487</v>
+      </c>
+      <c r="L66" t="str">
+        <v>B</v>
+      </c>
+    </row>
+    <row r="67" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G67" s="5">
+        <v>45455</v>
+      </c>
+      <c r="I67" s="5"/>
+      <c r="K67" s="5" t="str">
+        <v>45487</v>
+      </c>
+      <c r="L67" t="str">
+        <v>B</v>
+      </c>
+    </row>
+    <row r="68" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G68" s="5">
+        <v>45455</v>
+      </c>
+      <c r="I68" s="5"/>
+      <c r="K68" s="5" t="str">
+        <v>45487</v>
+      </c>
+      <c r="L68" t="str">
+        <v>B</v>
+      </c>
+    </row>
+    <row r="69" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G69" s="5">
+        <v>45455</v>
+      </c>
+      <c r="I69" s="5"/>
+      <c r="K69" s="5" t="str">
+        <v>45487</v>
+      </c>
+      <c r="L69" t="str">
+        <v>B</v>
+      </c>
+    </row>
+    <row r="70" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G70" s="5">
+        <v>45455</v>
+      </c>
+      <c r="I70" s="5"/>
+      <c r="K70" s="5" t="str">
+        <v>45487</v>
+      </c>
+      <c r="L70" t="str">
+        <v>B</v>
+      </c>
+    </row>
+    <row r="71" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G71" s="5">
+        <v>45455</v>
+      </c>
+      <c r="I71" s="5"/>
+      <c r="K71" s="5" t="str">
+        <v>45487</v>
+      </c>
+      <c r="L71" t="str">
+        <v>B</v>
+      </c>
+    </row>
+    <row r="72" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G72" s="5">
+        <v>45455</v>
+      </c>
+      <c r="I72" s="5"/>
+      <c r="K72" s="5" t="str">
+        <v>45487</v>
+      </c>
+      <c r="L72" t="str">
+        <v>B</v>
+      </c>
+    </row>
+    <row r="73" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G73" s="5">
+        <v>45455</v>
+      </c>
+      <c r="I73" s="5"/>
+      <c r="K73" s="5" t="str">
+        <v>45487</v>
+      </c>
+      <c r="L73" t="str">
+        <v>B</v>
+      </c>
+    </row>
+    <row r="74" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G74" s="5">
+        <v>45455</v>
+      </c>
+      <c r="I74" s="5"/>
+      <c r="K74" s="5" t="str">
+        <v>45487</v>
+      </c>
+      <c r="L74" t="str">
+        <v>B</v>
+      </c>
+    </row>
+    <row r="75" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G75" s="5">
+        <v>45455</v>
+      </c>
+      <c r="I75" s="5"/>
+      <c r="K75" s="5" t="str">
+        <v>45487</v>
+      </c>
+      <c r="L75" t="str">
+        <v>B</v>
+      </c>
+    </row>
+    <row r="76" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G76" s="5">
+        <v>45455</v>
+      </c>
+      <c r="I76" s="5"/>
+      <c r="K76" s="5" t="str">
+        <v>45487</v>
+      </c>
+      <c r="L76" t="str">
+        <v>B</v>
+      </c>
+    </row>
+    <row r="77" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G77" s="5">
+        <v>45455</v>
+      </c>
+      <c r="I77" s="5"/>
+      <c r="K77" s="5" t="str">
+        <v>45487</v>
+      </c>
+      <c r="L77" t="str">
+        <v>B</v>
+      </c>
+    </row>
+    <row r="78" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G78" s="5">
+        <v>45455</v>
+      </c>
+      <c r="I78" s="5"/>
+      <c r="K78" s="5" t="str">
+        <v>45487</v>
+      </c>
+      <c r="L78" t="str">
+        <v>B</v>
+      </c>
+    </row>
+    <row r="79" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G79" s="5">
+        <v>45455</v>
+      </c>
+      <c r="I79" s="5"/>
+      <c r="K79" s="5" t="str">
+        <v>45487</v>
+      </c>
+      <c r="L79" t="str">
+        <v>B</v>
+      </c>
+    </row>
+    <row r="80" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G80" s="5">
+        <v>45455</v>
+      </c>
+      <c r="I80" s="5"/>
+      <c r="K80" s="5" t="str">
+        <v>45487</v>
+      </c>
+      <c r="L80" t="str">
+        <v>B</v>
+      </c>
+    </row>
+    <row r="81" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G81" s="5">
+        <v>45455</v>
+      </c>
+      <c r="I81" s="5"/>
+      <c r="K81" s="5" t="str">
+        <v>45487</v>
+      </c>
+      <c r="L81" t="str">
+        <v>B</v>
+      </c>
+    </row>
+    <row r="82" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G82" s="5">
+        <v>45455</v>
+      </c>
+      <c r="I82" s="5"/>
+      <c r="K82" s="5" t="str">
+        <v>45487</v>
+      </c>
+      <c r="L82" t="str">
+        <v>B</v>
+      </c>
+    </row>
+    <row r="83" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G83" s="5">
+        <v>45455</v>
+      </c>
+      <c r="I83" s="5"/>
+      <c r="K83" s="5" t="str">
+        <v>45487</v>
+      </c>
+      <c r="L83" t="str">
+        <v>B</v>
+      </c>
+    </row>
+    <row r="84" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G84" s="5">
+        <v>45455</v>
+      </c>
+      <c r="I84" s="5"/>
+      <c r="K84" s="5" t="str">
+        <v>45487</v>
+      </c>
+      <c r="L84" t="str">
+        <v>B</v>
+      </c>
+    </row>
+    <row r="85" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G85" s="5">
+        <v>45455</v>
+      </c>
+      <c r="I85" s="5"/>
+      <c r="K85" s="5" t="str">
+        <v>45487</v>
+      </c>
+      <c r="L85" t="str">
+        <v>B</v>
+      </c>
+    </row>
+    <row r="86" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G86" s="5">
+        <v>45455</v>
+      </c>
+      <c r="I86" s="5"/>
+      <c r="K86" s="5" t="str">
+        <v>45487</v>
+      </c>
+      <c r="L86" t="str">
+        <v>B</v>
+      </c>
+    </row>
+    <row r="87" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G87" s="5">
+        <v>45455</v>
+      </c>
+      <c r="I87" s="5"/>
+      <c r="K87" s="5" t="str">
+        <v>45487</v>
+      </c>
+      <c r="L87" t="str">
+        <v>B</v>
+      </c>
+    </row>
+    <row r="88" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G88" s="5">
+        <v>45455</v>
+      </c>
+      <c r="I88" s="5"/>
+      <c r="K88" s="5" t="str">
+        <v>45487</v>
+      </c>
+      <c r="L88" t="str">
+        <v>B</v>
+      </c>
+    </row>
+    <row r="89" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G89" s="5">
+        <v>45455</v>
+      </c>
+      <c r="I89" s="5"/>
+      <c r="K89" s="5" t="str">
+        <v>45487</v>
+      </c>
+      <c r="L89" t="str">
+        <v>B</v>
+      </c>
+    </row>
+    <row r="90" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G90" s="5">
+        <v>45455</v>
+      </c>
+      <c r="I90" s="5"/>
+      <c r="K90" s="5" t="str">
+        <v>45487</v>
+      </c>
+      <c r="L90" t="str">
+        <v>B</v>
+      </c>
+    </row>
+    <row r="91" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G91" s="5">
+        <v>45455</v>
+      </c>
+      <c r="I91" s="5"/>
+      <c r="K91" s="5" t="str">
+        <v>45487</v>
+      </c>
+      <c r="L91" t="str">
+        <v>B</v>
+      </c>
+    </row>
+    <row r="92" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G92" s="5">
+        <v>45455</v>
+      </c>
+      <c r="I92" s="5"/>
+      <c r="K92" s="5" t="str">
+        <v>45487</v>
+      </c>
+      <c r="L92" t="str">
+        <v>B</v>
+      </c>
+    </row>
+    <row r="93" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G93" s="5">
+        <v>45455</v>
+      </c>
+      <c r="I93" s="5"/>
+      <c r="K93" s="5" t="str">
+        <v>45487</v>
+      </c>
+      <c r="L93" t="str">
+        <v>B</v>
+      </c>
+    </row>
+    <row r="94" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G94" s="5">
+        <v>45455</v>
+      </c>
+      <c r="I94" s="5"/>
+      <c r="K94" s="5" t="str">
+        <v>45487</v>
+      </c>
+      <c r="L94" t="str">
+        <v>B</v>
+      </c>
+    </row>
+    <row r="95" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G95" s="5">
+        <v>45456</v>
+      </c>
+      <c r="I95" s="5"/>
+      <c r="K95" s="5" t="str">
+        <v>45487</v>
+      </c>
+      <c r="L95" t="str">
+        <v>B</v>
+      </c>
+    </row>
+    <row r="96" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G96" s="5">
+        <v>45456</v>
+      </c>
+      <c r="I96" s="5"/>
+      <c r="K96" s="5" t="str">
+        <v>45487</v>
+      </c>
+      <c r="L96" t="str">
+        <v>B</v>
+      </c>
+    </row>
+    <row r="97" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G97" s="5">
+        <v>45456</v>
+      </c>
+      <c r="I97" s="5"/>
+      <c r="K97" s="5" t="str">
+        <v>45487</v>
+      </c>
+      <c r="L97" t="str">
+        <v>B</v>
+      </c>
+    </row>
+    <row r="98" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G98" s="5">
+        <v>45456</v>
+      </c>
+      <c r="I98" s="5"/>
+      <c r="K98" s="5" t="str">
+        <v>45487</v>
+      </c>
+      <c r="L98" t="str">
+        <v>B</v>
+      </c>
+    </row>
+    <row r="99" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G99" s="5">
+        <v>45456</v>
+      </c>
+      <c r="I99" s="5"/>
+      <c r="K99" s="5" t="str">
+        <v>45487</v>
+      </c>
+      <c r="L99" t="str">
+        <v>B</v>
+      </c>
+    </row>
+    <row r="100" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G100" s="5">
+        <v>45456</v>
+      </c>
+      <c r="I100" s="5"/>
+      <c r="K100" s="5" t="str">
+        <v>45487</v>
+      </c>
+      <c r="L100" t="str">
+        <v>B</v>
+      </c>
+    </row>
+    <row r="101" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G101" s="5">
+        <v>45456</v>
+      </c>
+      <c r="I101" s="5"/>
+      <c r="K101" s="5" t="str">
+        <v>45487</v>
+      </c>
+      <c r="L101" t="str">
+        <v>B</v>
+      </c>
+    </row>
+    <row r="102" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G102" s="5">
+        <v>45456</v>
+      </c>
+      <c r="I102" s="5"/>
+      <c r="K102" s="5" t="str">
+        <v>45489</v>
+      </c>
+      <c r="L102" t="str">
+        <v>C</v>
+      </c>
+    </row>
+    <row r="103" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G103" s="5">
+        <v>45456</v>
+      </c>
+      <c r="I103" s="5"/>
+      <c r="K103" s="5" t="str">
+        <v>45489</v>
+      </c>
+      <c r="L103" t="str">
+        <v>C</v>
+      </c>
+    </row>
+    <row r="104" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G104" s="5">
+        <v>45456</v>
+      </c>
+      <c r="I104" s="5"/>
+      <c r="K104" s="5" t="str">
+        <v>45489</v>
+      </c>
+      <c r="L104" t="str">
+        <v>C</v>
+      </c>
+    </row>
+    <row r="105" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G105" s="5">
+        <v>45456</v>
+      </c>
+      <c r="I105" s="5"/>
+      <c r="K105" s="5" t="str">
+        <v>45489</v>
+      </c>
+      <c r="L105" t="str">
+        <v>C</v>
+      </c>
+    </row>
+    <row r="106" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G106" s="5">
+        <v>45456</v>
+      </c>
+      <c r="I106" s="5"/>
+      <c r="K106" s="5" t="str">
+        <v>45489</v>
+      </c>
+      <c r="L106" t="str">
+        <v>C</v>
+      </c>
+    </row>
+    <row r="107" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G107" s="5">
+        <v>45456</v>
+      </c>
+      <c r="I107" s="5"/>
+      <c r="K107" s="5" t="str">
+        <v>45489</v>
+      </c>
+      <c r="L107" t="str">
+        <v>C</v>
+      </c>
+    </row>
+    <row r="108" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G108" s="5">
+        <v>45456</v>
+      </c>
+      <c r="I108" s="5"/>
+      <c r="K108" s="5" t="str">
+        <v>45489</v>
+      </c>
+      <c r="L108" t="str">
+        <v>C</v>
+      </c>
+    </row>
+    <row r="109" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G109" s="5">
+        <v>45456</v>
+      </c>
+      <c r="I109" s="5"/>
+      <c r="K109" s="5" t="str">
+        <v>45489</v>
+      </c>
+      <c r="L109" t="str">
+        <v>C</v>
+      </c>
+    </row>
+    <row r="110" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G110" s="5">
+        <v>45456</v>
+      </c>
+      <c r="I110" s="5"/>
+      <c r="K110" s="5" t="str">
+        <v>45489</v>
+      </c>
+      <c r="L110" t="str">
+        <v>C</v>
+      </c>
+    </row>
+    <row r="111" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G111" s="5">
+        <v>45456</v>
+      </c>
+      <c r="I111" s="5"/>
+      <c r="K111" s="5" t="str">
+        <v>45489</v>
+      </c>
+      <c r="L111" t="str">
+        <v>C</v>
+      </c>
+    </row>
+    <row r="112" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G112" s="5">
+        <v>45456</v>
+      </c>
+      <c r="I112" s="5"/>
+      <c r="K112" s="5" t="str">
+        <v>45489</v>
+      </c>
+      <c r="L112" t="str">
+        <v>C</v>
+      </c>
+    </row>
+    <row r="113" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G113" s="5">
+        <v>45456</v>
+      </c>
+      <c r="I113" s="5"/>
+      <c r="K113" s="5" t="str">
+        <v>45489</v>
+      </c>
+      <c r="L113" t="str">
+        <v>C</v>
+      </c>
+    </row>
+    <row r="114" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G114" s="5">
+        <v>45456</v>
+      </c>
+      <c r="I114" s="5"/>
+      <c r="K114" s="5" t="str">
+        <v>45489</v>
+      </c>
+      <c r="L114" t="str">
+        <v>C</v>
+      </c>
+    </row>
+    <row r="115" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G115" s="5">
+        <v>45456</v>
+      </c>
+      <c r="I115" s="5"/>
+      <c r="K115" s="5" t="str">
+        <v>45489</v>
+      </c>
+      <c r="L115" t="str">
+        <v>C</v>
+      </c>
+    </row>
+    <row r="116" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G116" s="5">
+        <v>45456</v>
+      </c>
+      <c r="I116" s="5"/>
+      <c r="K116" s="5" t="str">
+        <v>45489</v>
+      </c>
+      <c r="L116" t="str">
+        <v>C</v>
+      </c>
+    </row>
+    <row r="117" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G117" s="5">
+        <v>45456</v>
+      </c>
+      <c r="I117" s="5"/>
+      <c r="K117" s="5" t="str">
+        <v>45489</v>
+      </c>
+      <c r="L117" t="str">
+        <v>C</v>
+      </c>
+    </row>
+    <row r="118" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G118" s="5">
+        <v>45456</v>
+      </c>
+      <c r="I118" s="5"/>
+      <c r="K118" s="5" t="str">
+        <v>45489</v>
+      </c>
+      <c r="L118" t="str">
+        <v>C</v>
+      </c>
+    </row>
+    <row r="119" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G119" s="5">
+        <v>45456</v>
+      </c>
+      <c r="I119" s="5"/>
+      <c r="K119" s="5" t="str">
+        <v>45489</v>
+      </c>
+      <c r="L119" t="str">
+        <v>C</v>
+      </c>
+    </row>
+    <row r="120" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G120" s="5">
+        <v>45456</v>
+      </c>
+      <c r="I120" s="5"/>
+      <c r="K120" s="5" t="str">
+        <v>45489</v>
+      </c>
+      <c r="L120" t="str">
+        <v>C</v>
+      </c>
+    </row>
+    <row r="121" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G121" s="5">
+        <v>45456</v>
+      </c>
+      <c r="I121" s="5"/>
+      <c r="K121" s="5" t="str">
+        <v>45489</v>
+      </c>
+      <c r="L121" t="str">
+        <v>C</v>
+      </c>
+    </row>
+    <row r="122" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G122" s="5">
+        <v>45464</v>
+      </c>
+      <c r="I122" s="5"/>
+      <c r="K122" s="5" t="str">
+        <v>45489</v>
+      </c>
+      <c r="L122" t="str">
+        <v>C</v>
+      </c>
+    </row>
+    <row r="123" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G123" s="5">
+        <v>45464</v>
+      </c>
+      <c r="I123" s="5"/>
+      <c r="K123" s="5" t="str">
+        <v>45489</v>
+      </c>
+      <c r="L123" t="str">
+        <v>C</v>
+      </c>
+    </row>
+    <row r="124" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G124" s="5">
+        <v>45464</v>
+      </c>
+      <c r="I124" s="5"/>
+      <c r="K124" s="5" t="str">
+        <v>45489</v>
+      </c>
+      <c r="L124" t="str">
+        <v>C</v>
+      </c>
+    </row>
+    <row r="125" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G125" s="5">
+        <v>45464</v>
+      </c>
+      <c r="I125" s="5"/>
+      <c r="K125" s="5" t="str">
+        <v>45489</v>
+      </c>
+      <c r="L125" t="str">
+        <v>C</v>
+      </c>
+    </row>
+    <row r="126" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G126" s="5">
+        <v>45464</v>
+      </c>
+      <c r="I126" s="5"/>
+      <c r="K126" s="5" t="str">
+        <v>45489</v>
+      </c>
+      <c r="L126" t="str">
+        <v>C</v>
+      </c>
+    </row>
+    <row r="127" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G127" s="5">
+        <v>45464</v>
+      </c>
+      <c r="I127" s="5"/>
+      <c r="K127" s="5" t="str">
+        <v>45489</v>
+      </c>
+      <c r="L127" t="str">
+        <v>C</v>
+      </c>
+    </row>
+    <row r="128" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G128" s="5">
+        <v>45464</v>
+      </c>
+      <c r="I128" s="5"/>
+      <c r="K128" s="5" t="str">
+        <v>45489</v>
+      </c>
+      <c r="L128" t="str">
+        <v>C</v>
+      </c>
+    </row>
+    <row r="129" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G129" s="5">
+        <v>45464</v>
+      </c>
+      <c r="I129" s="5"/>
+      <c r="K129" s="5" t="str">
+        <v>45489</v>
+      </c>
+      <c r="L129" t="str">
+        <v>C</v>
+      </c>
+    </row>
+    <row r="130" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G130" s="5">
+        <v>45464</v>
+      </c>
+      <c r="I130" s="5"/>
+      <c r="K130" s="5" t="str">
+        <v>45489</v>
+      </c>
+      <c r="L130" t="str">
+        <v>C</v>
+      </c>
+    </row>
+    <row r="131" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G131" s="5">
+        <v>45464</v>
+      </c>
+      <c r="I131" s="5"/>
+      <c r="K131" s="5" t="str">
+        <v>45489</v>
+      </c>
+      <c r="L131" t="str">
+        <v>C</v>
+      </c>
+    </row>
+    <row r="132" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G132" s="5">
+        <v>45464</v>
+      </c>
+      <c r="I132" s="5"/>
+      <c r="K132" s="5" t="str">
+        <v>45489</v>
+      </c>
+      <c r="L132" t="str">
+        <v>C</v>
+      </c>
+    </row>
+    <row r="133" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G133" s="5">
+        <v>45464</v>
+      </c>
+      <c r="I133" s="5"/>
+      <c r="K133" s="5" t="str">
+        <v>45489</v>
+      </c>
+      <c r="L133" t="str">
+        <v>C</v>
+      </c>
+    </row>
+    <row r="134" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G134" s="5">
+        <v>45464</v>
+      </c>
+      <c r="I134" s="5"/>
+      <c r="K134" s="5" t="str">
+        <v>45520</v>
+      </c>
+      <c r="L134" t="str">
+        <v>D</v>
+      </c>
+    </row>
+    <row r="135" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G135" s="5">
+        <v>45464</v>
+      </c>
+      <c r="I135" s="5"/>
+      <c r="K135" s="5" t="str">
+        <v>45520</v>
+      </c>
+      <c r="L135" t="str">
+        <v>D</v>
+      </c>
+    </row>
+    <row r="136" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G136" s="5">
+        <v>45464</v>
+      </c>
+      <c r="I136" s="5"/>
+      <c r="K136" s="5" t="str">
+        <v>45520</v>
+      </c>
+      <c r="L136" t="str">
+        <v>D</v>
+      </c>
+    </row>
+    <row r="137" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G137" s="5">
+        <v>45486</v>
+      </c>
+      <c r="I137" s="5"/>
+      <c r="K137" s="5" t="str">
+        <v>45520</v>
+      </c>
+      <c r="L137" t="str">
+        <v>D</v>
+      </c>
+    </row>
+    <row r="138" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G138" s="5">
+        <v>45486</v>
+      </c>
+      <c r="I138" s="5"/>
+      <c r="K138" s="5" t="str">
+        <v>45520</v>
+      </c>
+      <c r="L138" t="str">
+        <v>D</v>
+      </c>
+    </row>
+    <row r="139" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G139" s="5">
+        <v>45486</v>
+      </c>
+      <c r="I139" s="5"/>
+      <c r="K139" s="5" t="str">
+        <v>45520</v>
+      </c>
+      <c r="L139" t="str">
+        <v>D</v>
+      </c>
+    </row>
+    <row r="140" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G140" s="5">
+        <v>45486</v>
+      </c>
+      <c r="I140" s="5"/>
+      <c r="K140" s="5" t="str">
+        <v>45520</v>
+      </c>
+      <c r="L140" t="str">
+        <v>D</v>
+      </c>
+    </row>
+    <row r="141" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G141" s="5">
+        <v>45486</v>
+      </c>
+      <c r="I141" s="5"/>
+      <c r="K141" s="5" t="str">
+        <v>45520</v>
+      </c>
+      <c r="L141" t="str">
+        <v>D</v>
+      </c>
+    </row>
+    <row r="142" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G142" s="5">
+        <v>45486</v>
+      </c>
+      <c r="I142" s="5"/>
+      <c r="K142" s="5" t="str">
+        <v>45520</v>
+      </c>
+      <c r="L142" t="str">
+        <v>D</v>
+      </c>
+    </row>
+    <row r="143" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G143" s="5">
+        <v>45486</v>
+      </c>
+      <c r="I143" s="5"/>
+      <c r="K143" s="5" t="str">
+        <v>45520</v>
+      </c>
+      <c r="L143" t="str">
+        <v>D</v>
+      </c>
+    </row>
+    <row r="144" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G144" s="5">
+        <v>45486</v>
+      </c>
+      <c r="I144" s="5"/>
+      <c r="K144" s="5" t="str">
+        <v>45520</v>
+      </c>
+      <c r="L144" t="str">
+        <v>D</v>
+      </c>
+    </row>
+    <row r="145" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G145" s="5">
+        <v>45486</v>
+      </c>
+      <c r="I145" s="5"/>
+      <c r="K145" s="5" t="str">
+        <v>45520</v>
+      </c>
+      <c r="L145" t="str">
+        <v>D</v>
+      </c>
+    </row>
+    <row r="146" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G146" s="5">
+        <v>45486</v>
+      </c>
+      <c r="I146" s="5"/>
+      <c r="K146" s="5" t="str">
+        <v>45520</v>
+      </c>
+      <c r="L146" t="str">
+        <v>D</v>
+      </c>
+    </row>
+    <row r="147" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G147" s="5">
+        <v>45486</v>
+      </c>
+      <c r="I147" s="5"/>
+      <c r="K147" s="5" t="str">
+        <v>45520</v>
+      </c>
+      <c r="L147" t="str">
+        <v>D</v>
+      </c>
+    </row>
+    <row r="148" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G148" s="5">
+        <v>45486</v>
+      </c>
+      <c r="I148" s="5"/>
+      <c r="K148" s="5" t="str">
+        <v>45520</v>
+      </c>
+      <c r="L148" t="str">
+        <v>D</v>
+      </c>
+    </row>
+    <row r="149" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G149" s="5">
+        <v>45486</v>
+      </c>
+      <c r="I149" s="5"/>
+      <c r="K149" s="5" t="str">
+        <v>45520</v>
+      </c>
+      <c r="L149" t="str">
+        <v>D</v>
+      </c>
+    </row>
+    <row r="150" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G150" s="5">
+        <v>45486</v>
+      </c>
+      <c r="I150" s="5"/>
+      <c r="K150" s="5" t="str">
+        <v>45520</v>
+      </c>
+      <c r="L150" t="str">
+        <v>D</v>
+      </c>
+    </row>
+    <row r="151" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G151" s="5">
+        <v>45486</v>
+      </c>
+      <c r="I151" s="5"/>
+      <c r="K151" s="5" t="str">
+        <v>45520</v>
+      </c>
+      <c r="L151" t="str">
+        <v>D</v>
+      </c>
+    </row>
+    <row r="152" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G152" s="5">
+        <v>45486</v>
+      </c>
+      <c r="I152" s="5"/>
+      <c r="K152" s="5" t="str">
+        <v>45520</v>
+      </c>
+      <c r="L152" t="str">
+        <v>D</v>
+      </c>
+    </row>
+    <row r="153" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G153" s="5">
+        <v>45486</v>
+      </c>
+      <c r="I153" s="5"/>
+      <c r="K153" s="5" t="str">
+        <v>45520</v>
+      </c>
+      <c r="L153" t="str">
+        <v>D</v>
+      </c>
+    </row>
+    <row r="154" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G154" s="5">
+        <v>45486</v>
+      </c>
+      <c r="I154" s="5"/>
+      <c r="K154" s="5" t="str">
+        <v>45520</v>
+      </c>
+      <c r="L154" t="str">
+        <v>D</v>
+      </c>
+    </row>
+    <row r="155" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G155" s="5">
+        <v>45486</v>
+      </c>
+      <c r="I155" s="5"/>
+      <c r="K155" s="5" t="str">
+        <v>45520</v>
+      </c>
+      <c r="L155" t="str">
+        <v>D</v>
+      </c>
+    </row>
+    <row r="156" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G156" s="5">
+        <v>45486</v>
+      </c>
+      <c r="I156" s="5"/>
+      <c r="K156" s="5" t="str">
+        <v>45520</v>
+      </c>
+      <c r="L156" t="str">
+        <v>D</v>
+      </c>
+    </row>
+    <row r="157" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G157" s="5">
+        <v>45486</v>
+      </c>
+      <c r="I157" s="5"/>
+      <c r="K157" s="5" t="str">
+        <v>45520</v>
+      </c>
+      <c r="L157" t="str">
+        <v>D</v>
+      </c>
+    </row>
+    <row r="158" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G158" s="5">
+        <v>45486</v>
+      </c>
+      <c r="I158" s="5"/>
+      <c r="K158" s="5" t="str">
+        <v>45520</v>
+      </c>
+      <c r="L158" t="str">
+        <v>D</v>
+      </c>
+    </row>
+    <row r="159" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G159" s="5">
+        <v>45486</v>
+      </c>
+      <c r="I159" s="5"/>
+      <c r="K159" s="5" t="str">
+        <v>45520</v>
+      </c>
+      <c r="L159" t="str">
+        <v>D</v>
+      </c>
+    </row>
+    <row r="160" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G160" s="5">
+        <v>45486</v>
+      </c>
+      <c r="I160" s="5"/>
+      <c r="K160" s="5" t="str">
+        <v>45520</v>
+      </c>
+      <c r="L160" t="str">
+        <v>D</v>
+      </c>
+    </row>
+    <row r="161" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G161" s="5">
+        <v>45486</v>
+      </c>
+      <c r="I161" s="5"/>
+      <c r="K161" s="5" t="str">
+        <v>45520</v>
+      </c>
+      <c r="L161" t="str">
+        <v>D</v>
+      </c>
+    </row>
+    <row r="162" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G162" s="5">
+        <v>45486</v>
+      </c>
+      <c r="I162" s="5"/>
+      <c r="K162" s="5" t="str">
+        <v>45520</v>
+      </c>
+      <c r="L162" t="str">
+        <v>D</v>
+      </c>
+    </row>
+    <row r="163" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G163" s="5">
+        <v>45486</v>
+      </c>
+      <c r="I163" s="5"/>
+      <c r="K163" s="5" t="str">
+        <v>45520</v>
+      </c>
+      <c r="L163" t="str">
+        <v>D</v>
+      </c>
+    </row>
+    <row r="164" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G164" s="5">
+        <v>45486</v>
+      </c>
+      <c r="I164" s="5"/>
+      <c r="K164" s="5" t="str">
+        <v>45520</v>
+      </c>
+      <c r="L164" t="str">
+        <v>D</v>
+      </c>
+    </row>
+    <row r="165" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G165" s="5">
+        <v>45486</v>
+      </c>
+      <c r="I165" s="5"/>
+      <c r="K165" s="5" t="str">
+        <v>45520</v>
+      </c>
+      <c r="L165" t="str">
+        <v>D</v>
+      </c>
+    </row>
+    <row r="166" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G166" s="5">
+        <v>45486</v>
+      </c>
+      <c r="I166" s="5"/>
+      <c r="K166" s="5" t="str">
+        <v>45520</v>
+      </c>
+      <c r="L166" t="str">
+        <v>D</v>
+      </c>
+    </row>
+    <row r="167" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G167" s="5">
+        <v>45486</v>
+      </c>
+      <c r="I167" s="5"/>
+      <c r="K167" s="5" t="str">
+        <v>45520</v>
+      </c>
+      <c r="L167" t="str">
+        <v>D</v>
+      </c>
+    </row>
+    <row r="168" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G168" s="5">
+        <v>45486</v>
+      </c>
+      <c r="I168" s="5"/>
+      <c r="K168" s="5" t="str">
+        <v>45520</v>
+      </c>
+      <c r="L168" t="str">
+        <v>D</v>
+      </c>
+    </row>
+    <row r="169" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G169" s="5">
+        <v>45486</v>
+      </c>
+      <c r="I169" s="5"/>
+      <c r="K169" s="5" t="str">
+        <v>45520</v>
+      </c>
+      <c r="L169" t="str">
+        <v>D</v>
+      </c>
+    </row>
+    <row r="170" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G170" s="5">
+        <v>45486</v>
+      </c>
+      <c r="I170" s="5"/>
+      <c r="K170" s="5" t="str">
+        <v>45520</v>
+      </c>
+      <c r="L170" t="str">
+        <v>D</v>
+      </c>
+    </row>
+    <row r="171" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G171" s="5">
+        <v>45486</v>
+      </c>
+      <c r="I171" s="5"/>
+      <c r="K171" s="5" t="str">
+        <v>45520</v>
+      </c>
+      <c r="L171" t="str">
+        <v>D</v>
+      </c>
+    </row>
+    <row r="172" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G172" s="5">
+        <v>45486</v>
+      </c>
+      <c r="I172" s="5"/>
+      <c r="K172" s="5" t="str">
+        <v>45520</v>
+      </c>
+      <c r="L172" t="str">
+        <v>D</v>
+      </c>
+    </row>
+    <row r="173" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G173" s="5">
+        <v>45486</v>
+      </c>
+      <c r="I173" s="5"/>
+      <c r="K173" s="5" t="str">
+        <v>45520</v>
+      </c>
+      <c r="L173" t="str">
+        <v>D</v>
+      </c>
+    </row>
+    <row r="174" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G174" s="5">
+        <v>45486</v>
+      </c>
+      <c r="I174" s="5"/>
+      <c r="K174" s="5" t="str">
+        <v>45520</v>
+      </c>
+      <c r="L174" t="str">
+        <v>D</v>
+      </c>
+    </row>
+    <row r="175" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G175" s="5">
+        <v>45502</v>
+      </c>
+      <c r="I175" s="5"/>
+      <c r="K175" s="5" t="str">
+        <v>45520</v>
+      </c>
+      <c r="L175" t="str">
+        <v>D</v>
+      </c>
+    </row>
+    <row r="176" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G176" s="5">
+        <v>45502</v>
+      </c>
+      <c r="I176" s="5"/>
+      <c r="K176" s="5" t="str">
+        <v>45523</v>
+      </c>
+      <c r="L176" t="str">
+        <v>E</v>
+      </c>
+    </row>
+    <row r="177" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G177" s="5">
+        <v>45502</v>
+      </c>
+      <c r="I177" s="5"/>
+      <c r="K177" s="5" t="str">
+        <v>45523</v>
+      </c>
+      <c r="L177" t="str">
+        <v>E</v>
+      </c>
+    </row>
+    <row r="178" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G178" s="5">
+        <v>45502</v>
+      </c>
+      <c r="I178" s="5"/>
+      <c r="K178" s="5" t="str">
+        <v>45523</v>
+      </c>
+      <c r="L178" t="str">
+        <v>E</v>
+      </c>
+    </row>
+    <row r="179" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G179" s="5">
+        <v>45502</v>
+      </c>
+      <c r="I179" s="5"/>
+      <c r="K179" s="5" t="str">
+        <v>45523</v>
+      </c>
+      <c r="L179" t="str">
+        <v>E</v>
+      </c>
+    </row>
+    <row r="180" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G180" s="5">
+        <v>45502</v>
+      </c>
+      <c r="I180" s="5"/>
+      <c r="K180" s="5" t="str">
+        <v>45523</v>
+      </c>
+      <c r="L180" t="str">
+        <v>E</v>
+      </c>
+    </row>
+    <row r="181" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G181" s="5">
+        <v>45502</v>
+      </c>
+      <c r="I181" s="5"/>
+      <c r="K181" s="5" t="str">
+        <v>45523</v>
+      </c>
+      <c r="L181" t="str">
+        <v>E</v>
+      </c>
+    </row>
+    <row r="182" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G182" s="5">
+        <v>45502</v>
+      </c>
+      <c r="I182" s="5"/>
+      <c r="K182" s="5" t="str">
+        <v>45523</v>
+      </c>
+      <c r="L182" t="str">
+        <v>E</v>
+      </c>
+    </row>
+    <row r="183" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G183" s="5">
+        <v>45502</v>
+      </c>
+      <c r="I183" s="5"/>
+      <c r="K183" s="5" t="str">
+        <v>45523</v>
+      </c>
+      <c r="L183" t="str">
+        <v>E</v>
+      </c>
+    </row>
+    <row r="184" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G184" s="5">
+        <v>45502</v>
+      </c>
+      <c r="I184" s="5"/>
+      <c r="K184" s="5" t="str">
+        <v>45523</v>
+      </c>
+      <c r="L184" t="str">
+        <v>E</v>
+      </c>
+    </row>
+    <row r="185" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G185" s="5">
+        <v>45502</v>
+      </c>
+      <c r="I185" s="5"/>
+      <c r="K185" s="5" t="str">
+        <v>45523</v>
+      </c>
+      <c r="L185" t="str">
+        <v>E</v>
+      </c>
+    </row>
+    <row r="186" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G186" s="5">
+        <v>45502</v>
+      </c>
+      <c r="I186" s="5"/>
+      <c r="K186" s="5" t="str">
+        <v>45523</v>
+      </c>
+      <c r="L186" t="str">
+        <v>E</v>
+      </c>
+    </row>
+    <row r="187" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G187" s="5">
+        <v>45502</v>
+      </c>
+      <c r="I187" s="5"/>
+      <c r="K187" s="5" t="str">
+        <v>45523</v>
+      </c>
+      <c r="L187" t="str">
+        <v>E</v>
+      </c>
+    </row>
+    <row r="188" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G188" s="5">
+        <v>45502</v>
+      </c>
+      <c r="I188" s="5"/>
+      <c r="K188" s="5" t="str">
+        <v>45523</v>
+      </c>
+      <c r="L188" t="str">
+        <v>E</v>
+      </c>
+    </row>
+    <row r="189" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G189" s="5">
+        <v>45502</v>
+      </c>
+      <c r="I189" s="5"/>
+      <c r="K189" s="5" t="str">
+        <v>45523</v>
+      </c>
+      <c r="L189" t="str">
+        <v>E</v>
+      </c>
+    </row>
+    <row r="190" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G190" s="5">
+        <v>45502</v>
+      </c>
+      <c r="I190" s="5"/>
+      <c r="K190" s="5" t="str">
+        <v>45523</v>
+      </c>
+      <c r="L190" t="str">
+        <v>E</v>
+      </c>
+    </row>
+    <row r="191" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G191" s="5">
+        <v>45502</v>
+      </c>
+      <c r="I191" s="5"/>
+      <c r="K191" s="5" t="str">
+        <v>45523</v>
+      </c>
+      <c r="L191" t="str">
+        <v>E</v>
+      </c>
+    </row>
+    <row r="192" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G192" s="5">
+        <v>45502</v>
+      </c>
+      <c r="I192" s="5"/>
+      <c r="K192" s="5" t="str">
+        <v>45523</v>
+      </c>
+      <c r="L192" t="str">
+        <v>E</v>
+      </c>
+    </row>
+    <row r="193" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G193" s="5">
+        <v>45502</v>
+      </c>
+      <c r="I193" s="5"/>
+      <c r="K193" s="5" t="str">
+        <v>45523</v>
+      </c>
+      <c r="L193" t="str">
+        <v>E</v>
+      </c>
+    </row>
+    <row r="194" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G194" s="5">
+        <v>45502</v>
+      </c>
+      <c r="I194" s="5"/>
+      <c r="K194" s="5" t="str">
+        <v>45523</v>
+      </c>
+      <c r="L194" t="str">
+        <v>E</v>
+      </c>
+    </row>
+    <row r="195" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G195" s="5">
+        <v>45502</v>
+      </c>
+      <c r="I195" s="5"/>
+      <c r="K195" s="5" t="str">
+        <v>45523</v>
+      </c>
+      <c r="L195" t="str">
+        <v>E</v>
+      </c>
+    </row>
+    <row r="196" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G196" s="5">
+        <v>45502</v>
+      </c>
+      <c r="I196" s="5"/>
+      <c r="K196" s="5" t="str">
+        <v>45523</v>
+      </c>
+      <c r="L196" t="str">
+        <v>E</v>
+      </c>
+    </row>
+    <row r="197" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G197" s="5">
+        <v>45502</v>
+      </c>
+      <c r="I197" s="5"/>
+      <c r="K197" s="5" t="str">
+        <v>45523</v>
+      </c>
+      <c r="L197" t="str">
+        <v>E</v>
+      </c>
+    </row>
+    <row r="198" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G198" s="5">
+        <v>45502</v>
+      </c>
+      <c r="I198" s="5"/>
+      <c r="K198" s="5" t="str">
+        <v>45523</v>
+      </c>
+      <c r="L198" t="str">
+        <v>E</v>
+      </c>
+    </row>
+    <row r="199" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G199" s="5">
+        <v>45502</v>
+      </c>
+      <c r="I199" s="5"/>
+    </row>
+    <row r="200" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G200" s="5">
+        <v>45502</v>
+      </c>
+      <c r="I200" s="5"/>
+    </row>
+    <row r="201" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G201" s="5">
+        <v>45502</v>
+      </c>
+      <c r="I201" s="5"/>
+    </row>
+    <row r="202" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G202" s="5">
+        <v>45502</v>
+      </c>
+      <c r="I202" s="5"/>
+    </row>
+    <row r="203" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G203" s="5">
+        <v>45502</v>
+      </c>
+    </row>
+    <row r="204" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G204" s="5">
+        <v>45502</v>
+      </c>
+    </row>
+    <row r="205" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G205" s="5">
+        <v>45502</v>
+      </c>
+    </row>
+    <row r="206" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G206" s="5">
+        <v>45502</v>
+      </c>
+    </row>
+    <row r="207" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G207" s="5">
+        <v>45502</v>
+      </c>
+    </row>
+    <row r="208" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G208" s="5">
+        <v>45502</v>
+      </c>
+    </row>
+    <row r="209" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G209" s="5">
+        <v>45502</v>
+      </c>
+    </row>
+    <row r="210" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G210" s="5">
+        <v>45502</v>
+      </c>
+    </row>
+    <row r="211" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G211" s="5">
+        <v>45502</v>
+      </c>
+    </row>
+    <row r="212" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G212" s="5">
+        <v>45502</v>
+      </c>
+    </row>
+    <row r="213" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G213" s="5">
+        <v>45502</v>
+      </c>
+    </row>
+    <row r="214" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G214" s="5">
+        <v>45502</v>
+      </c>
+    </row>
+    <row r="215" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G215" s="5">
+        <v>45502</v>
+      </c>
+    </row>
+    <row r="216" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G216" s="5">
+        <v>45502</v>
+      </c>
+    </row>
+    <row r="217" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G217" s="5">
+        <v>45502</v>
+      </c>
+    </row>
+    <row r="218" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G218" s="5">
+        <v>45502</v>
+      </c>
+    </row>
+    <row r="219" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G219" s="5">
+        <v>45502</v>
+      </c>
+    </row>
+    <row r="220" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G220" s="5">
+        <v>45502</v>
+      </c>
+    </row>
+    <row r="221" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G221" s="5">
+        <v>45502</v>
+      </c>
+    </row>
+    <row r="222" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G222" s="5">
+        <v>45502</v>
+      </c>
+    </row>
+    <row r="223" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G223" s="5">
+        <v>45502</v>
+      </c>
+    </row>
+    <row r="224" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G224" s="5">
+        <v>45502</v>
+      </c>
+    </row>
+    <row r="225" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G225" s="5">
+        <v>45502</v>
+      </c>
+    </row>
+    <row r="226" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G226" s="5">
+        <v>45502</v>
+      </c>
+    </row>
+    <row r="227" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G227" s="5">
+        <v>45502</v>
+      </c>
+    </row>
+    <row r="228" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G228" s="5">
+        <v>45502</v>
+      </c>
+    </row>
+    <row r="229" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G229" s="5">
+        <v>45502</v>
+      </c>
+    </row>
+    <row r="230" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G230" s="5">
+        <v>45502</v>
+      </c>
+    </row>
+    <row r="231" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G231" s="5">
+        <v>45502</v>
+      </c>
+    </row>
+    <row r="232" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G232" s="5">
+        <v>45502</v>
+      </c>
+    </row>
+    <row r="233" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G233" s="5">
+        <v>45502</v>
+      </c>
+    </row>
+    <row r="234" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G234" s="5">
+        <v>45502</v>
+      </c>
+    </row>
+    <row r="235" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G235" s="5">
+        <v>45502</v>
+      </c>
+    </row>
+    <row r="236" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G236" s="5">
+        <v>45502</v>
+      </c>
+    </row>
+    <row r="237" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G237" s="5">
+        <v>45502</v>
+      </c>
+    </row>
+    <row r="238" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G238" s="5">
+        <v>45502</v>
+      </c>
+    </row>
+    <row r="239" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G239" s="5">
+        <v>45502</v>
+      </c>
+    </row>
+    <row r="240" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G240" s="5">
+        <v>45502</v>
+      </c>
+    </row>
+    <row r="241" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G241" s="5">
+        <v>45502</v>
+      </c>
+    </row>
+    <row r="242" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G242" s="5">
+        <v>45502</v>
+      </c>
+    </row>
+    <row r="243" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G243" s="5">
+        <v>45502</v>
+      </c>
+    </row>
+    <row r="244" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G244" s="5">
+        <v>45502</v>
+      </c>
+    </row>
+    <row r="245" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G245" s="5">
+        <v>45502</v>
+      </c>
+    </row>
+    <row r="246" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G246" s="5">
+        <v>45502</v>
+      </c>
+    </row>
+    <row r="247" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G247" s="5">
+        <v>45502</v>
+      </c>
+    </row>
+    <row r="248" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G248" s="5">
+        <v>45502</v>
+      </c>
+    </row>
+    <row r="249" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G249" s="5">
+        <v>45502</v>
+      </c>
+    </row>
+    <row r="250" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G250" s="5">
+        <v>45502</v>
+      </c>
+    </row>
+    <row r="251" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G251" s="5">
+        <v>45502</v>
+      </c>
+    </row>
+    <row r="252" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G252" s="5">
+        <v>45502</v>
+      </c>
+    </row>
+    <row r="253" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G253" s="5">
+        <v>45502</v>
+      </c>
+    </row>
+    <row r="254" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G254" s="5">
+        <v>45502</v>
+      </c>
+    </row>
+    <row r="255" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G255" s="5">
+        <v>45502</v>
+      </c>
+    </row>
+    <row r="256" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G256" s="5">
+        <v>45502</v>
+      </c>
+    </row>
+    <row r="257" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G257" s="5">
+        <v>45502</v>
+      </c>
+    </row>
+    <row r="258" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G258" s="5">
+        <v>45502</v>
+      </c>
+    </row>
+    <row r="259" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G259" s="5">
+        <v>45502</v>
+      </c>
+    </row>
+    <row r="260" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G260" s="5">
+        <v>45502</v>
+      </c>
+    </row>
+    <row r="261" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G261" s="5">
+        <v>45502</v>
+      </c>
+    </row>
+    <row r="262" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G262" s="5">
+        <v>45502</v>
+      </c>
+    </row>
+    <row r="263" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G263" s="5">
+        <v>45502</v>
+      </c>
+    </row>
+    <row r="264" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G264" s="5">
+        <v>45502</v>
+      </c>
+    </row>
+    <row r="265" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G265" s="5">
+        <v>45502</v>
+      </c>
+    </row>
+    <row r="266" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G266" s="5">
+        <v>45502</v>
+      </c>
+    </row>
+    <row r="267" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G267" s="5">
+        <v>45502</v>
+      </c>
+    </row>
+    <row r="268" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G268" s="5">
+        <v>45502</v>
+      </c>
+    </row>
+    <row r="269" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G269" s="5">
+        <v>45502</v>
+      </c>
+    </row>
+    <row r="270" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G270" s="5">
+        <v>45502</v>
+      </c>
+    </row>
+    <row r="271" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G271" s="5">
+        <v>45502</v>
+      </c>
+    </row>
+    <row r="272" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G272" s="5">
+        <v>45502</v>
+      </c>
+    </row>
+    <row r="273" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G273" s="5">
+        <v>45502</v>
+      </c>
+    </row>
+    <row r="274" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G274" s="5">
+        <v>45502</v>
+      </c>
+    </row>
+    <row r="275" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G275" s="5">
+        <v>45502</v>
+      </c>
+    </row>
+    <row r="276" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G276" s="5">
+        <v>45502</v>
+      </c>
+    </row>
+    <row r="277" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G277" s="5">
+        <v>45502</v>
+      </c>
+    </row>
+    <row r="278" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G278" s="5">
+        <v>45502</v>
+      </c>
+    </row>
+    <row r="279" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G279" s="5">
+        <v>45502</v>
+      </c>
+    </row>
+    <row r="280" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G280" s="5">
+        <v>45502</v>
+      </c>
+    </row>
+    <row r="281" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G281" s="5">
+        <v>45502</v>
+      </c>
+    </row>
+    <row r="282" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G282" s="5">
+        <v>45502</v>
+      </c>
+    </row>
+    <row r="283" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G283" s="5">
+        <v>45502</v>
+      </c>
+    </row>
+    <row r="284" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G284" s="5">
+        <v>45502</v>
+      </c>
+    </row>
+    <row r="285" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G285" s="5">
+        <v>45502</v>
+      </c>
+    </row>
+    <row r="286" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G286" s="5">
+        <v>45502</v>
+      </c>
+    </row>
+    <row r="287" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G287" s="5">
+        <v>45502</v>
+      </c>
+    </row>
+    <row r="288" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G288" s="5">
+        <v>45502</v>
+      </c>
+    </row>
+    <row r="289" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G289" s="5">
+        <v>45502</v>
+      </c>
+    </row>
+    <row r="290" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G290" s="5">
+        <v>45502</v>
+      </c>
+    </row>
+    <row r="291" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G291" s="5">
+        <v>45502</v>
+      </c>
+    </row>
+    <row r="292" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G292" s="5">
+        <v>45502</v>
+      </c>
+    </row>
+    <row r="293" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G293" s="5">
+        <v>45502</v>
+      </c>
+    </row>
+    <row r="294" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G294" s="5">
+        <v>45502</v>
+      </c>
+    </row>
+    <row r="295" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G295" s="5">
+        <v>45502</v>
+      </c>
+    </row>
+    <row r="296" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G296" s="5">
+        <v>45502</v>
+      </c>
+    </row>
+    <row r="297" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G297" s="5">
+        <v>45502</v>
+      </c>
+    </row>
+    <row r="298" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G298" s="5">
+        <v>45502</v>
+      </c>
+    </row>
+    <row r="299" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G299" s="5">
+        <v>45502</v>
+      </c>
+    </row>
+    <row r="300" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G300" s="5">
+        <v>45502</v>
+      </c>
+    </row>
+    <row r="301" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G301" s="5">
+        <v>45502</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
Completed a multi-stage solution
</commit_message>
<xml_diff>
--- a/CH-130 FIFO.xlsx
+++ b/CH-130 FIFO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38F76307-E418-4EA5-84E8-6062FE9FC945}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C85B50C-C3D7-4B59-8D3E-3235C9B05211}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="25">
   <si>
     <t>Question</t>
   </si>
@@ -135,12 +135,18 @@
   <si>
     <t>e</t>
   </si>
+  <si>
+    <t>h</t>
+  </si>
+  <si>
+    <t>GROUPBY(HSTACK(TAKE(g, , -1), h, TAKE(e, ROWS(g))), h, COUNT, , 0)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -168,8 +174,14 @@
       <family val="1"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -179,6 +191,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -467,7 +485,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -536,6 +554,9 @@
     <xf numFmtId="3" fontId="2" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="4" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -551,9 +572,12 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="4" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1113,6 +1137,9 @@
   <we:bindings/>
   <we:snapshot xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
   <we:extLst>
+    <a:ext xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" uri="{D87F86FE-615C-45B5-9D79-34F1136793EB}">
+      <we:containsCustomFunctions/>
+    </a:ext>
     <a:ext xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" uri="{7C84B067-C214-45C3-A712-C9D94CD141B2}">
       <we:customFunctionIdList>
         <we:customFunctionIds>_xldudf_LABS_GENERATIVEAI</we:customFunctionIds>
@@ -1143,17 +1170,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" s="6" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="27"/>
-      <c r="D1" s="28"/>
-      <c r="F1" s="29" t="s">
+      <c r="C1" s="28"/>
+      <c r="D1" s="29"/>
+      <c r="F1" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="30"/>
-      <c r="H1" s="30"/>
-      <c r="I1" s="30"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
       <c r="K1" s="6" t="s">
         <v>19</v>
       </c>
@@ -1628,17 +1655,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" s="6" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="27"/>
-      <c r="D1" s="28"/>
-      <c r="F1" s="29" t="s">
+      <c r="C1" s="28"/>
+      <c r="D1" s="29"/>
+      <c r="F1" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="30"/>
-      <c r="H1" s="30"/>
-      <c r="I1" s="30"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
       <c r="K1" s="6" t="s">
         <v>19</v>
       </c>
@@ -2232,10 +2259,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CBB5195-1E8A-4CD7-99EA-F5B23BFB852F}">
-  <dimension ref="A1:O301"/>
+  <dimension ref="A1:U301"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+    <sheetView tabSelected="1" topLeftCell="D12" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -2248,25 +2275,27 @@
     <col min="7" max="7" width="12.3984375" style="5" customWidth="1"/>
     <col min="8" max="8" width="11.5" customWidth="1"/>
     <col min="9" max="9" width="8.8984375" customWidth="1"/>
+    <col min="14" max="14" width="10.8984375" customWidth="1"/>
+    <col min="15" max="15" width="10.3984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="6" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="26" t="s">
+    <row r="1" spans="1:18" s="6" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="27"/>
-      <c r="D1" s="28"/>
-      <c r="F1" s="29" t="s">
+      <c r="C1" s="28"/>
+      <c r="D1" s="29"/>
+      <c r="F1" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="30"/>
-      <c r="H1" s="30"/>
-      <c r="I1" s="30"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
       <c r="K1" s="6" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B2" s="9" t="s">
         <v>5</v>
       </c>
@@ -2290,7 +2319,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B3" s="14">
         <v>45455</v>
       </c>
@@ -2319,7 +2348,7 @@
       <c r="M3" s="8"/>
       <c r="N3" s="7"/>
     </row>
-    <row r="4" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B4" s="14">
         <v>45456</v>
       </c>
@@ -2348,7 +2377,7 @@
       <c r="M4" s="8"/>
       <c r="N4" s="7"/>
     </row>
-    <row r="5" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B5" s="14">
         <v>45457</v>
       </c>
@@ -2377,7 +2406,7 @@
       <c r="M5" s="8"/>
       <c r="N5" s="7"/>
     </row>
-    <row r="6" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B6" s="14">
         <v>45464</v>
       </c>
@@ -2406,7 +2435,7 @@
       <c r="M6" s="8"/>
       <c r="N6" s="7"/>
     </row>
-    <row r="7" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B7" s="14">
         <v>45486</v>
       </c>
@@ -2430,7 +2459,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B8" s="14">
         <v>45487</v>
       </c>
@@ -2459,7 +2488,7 @@
       <c r="M8"/>
       <c r="N8"/>
     </row>
-    <row r="9" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B9" s="14">
         <v>45489</v>
       </c>
@@ -2489,7 +2518,7 @@
       <c r="M9"/>
       <c r="N9"/>
     </row>
-    <row r="10" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B10" s="14">
         <v>45502</v>
       </c>
@@ -2512,11 +2541,13 @@
       <c r="I10" s="25">
         <v>1</v>
       </c>
-      <c r="K10"/>
+      <c r="K10" s="34" t="s">
+        <v>24</v>
+      </c>
       <c r="M10"/>
       <c r="N10"/>
     </row>
-    <row r="11" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B11" s="14">
         <v>45502</v>
       </c>
@@ -2544,7 +2575,7 @@
       <c r="M11"/>
       <c r="N11"/>
     </row>
-    <row r="12" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B12" s="14">
         <v>45520</v>
       </c>
@@ -2564,7 +2595,7 @@
       <c r="M12"/>
       <c r="N12"/>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B13" s="14">
         <v>45523</v>
       </c>
@@ -2577,22 +2608,28 @@
       <c r="E13" s="7"/>
       <c r="L13" s="2"/>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B14" s="7"/>
       <c r="C14" s="7"/>
       <c r="D14" s="7"/>
       <c r="E14" s="7"/>
+      <c r="K14" s="33" t="s">
+        <v>23</v>
+      </c>
       <c r="L14" s="2"/>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="7"/>
       <c r="C15" s="7"/>
       <c r="D15" s="7"/>
       <c r="E15" s="7"/>
       <c r="L15" s="2"/>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="R15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="7" t="s">
         <v>3</v>
@@ -2615,10 +2652,23 @@
       <c r="K16" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="17" spans="1:15" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M16" s="9" t="str" cm="1">
+        <f t="array" ref="M16:P16">F2:I2</f>
+        <v>Output</v>
+      </c>
+      <c r="N16" s="17" t="str">
+        <v>Registered Date</v>
+      </c>
+      <c r="O16" s="10" t="str">
+        <v>Source Date</v>
+      </c>
+      <c r="P16" s="11" t="str">
+        <v>Quantity</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1"/>
-      <c r="B17" s="31" t="str" cm="1">
+      <c r="B17" s="26" t="str" cm="1">
         <f t="array" ref="B17:E25">_xlfn.LET(
     _xlpm.a, B3:B13,
     _xlpm.b, C3:C13,
@@ -2672,7 +2722,7 @@
       <c r="J17">
         <v>27</v>
       </c>
-      <c r="K17" s="5" t="str" cm="1">
+      <c r="K17" s="32" cm="1">
         <f t="array" ref="K17:L198">_xlfn.LET(
     _xlpm.a, B3:B13,
     _xlpm.b, C3:C13,
@@ -2682,16 +2732,33 @@
     _xlpm.f, _xlfn._xlws.FILTER(_xlfn.HSTACK(_xlpm.a &amp; "-" &amp; RIGHT(_xlpm.b), _xlpm.c), _xlpm.b &lt;&gt; "Input"),
     _xlpm.g, _xlfn.TEXTSPLIT(_xlfn.CONCAT(REPT(_xlfn.TAKE(_xlpm.f, , 1) &amp; " ", _xlfn.TAKE(_xlpm.f, , -1))), "-", " ", 1),
     _xlpm.h, --_xlfn.TAKE(_xlpm.g, , 1),
-    _xlpm.g
+    _xlfn.HSTACK(_xlfn.CHOOSECOLS(_xlpm.g,1)+0,_xlfn.CHOOSECOLS(_xlpm.g,2))
 )</f>
         <v>45457</v>
       </c>
       <c r="L17" t="str">
         <v>A</v>
       </c>
-      <c r="O17" s="2"/>
-    </row>
-    <row r="18" spans="1:15" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M17" s="12" t="str" cm="1">
+        <f t="array" ref="M17:P25">_xlfn.GROUPBY(_xlfn.HSTACK(L17:L198,K17:K198,_xlfn.TAKE(_xlfn.ANCHORARRAY(G17),ROWS(L17:L198))),K17:K198,_xleta.COUNTA,,0)</f>
+        <v>A</v>
+      </c>
+      <c r="N17" s="18">
+        <v>45457</v>
+      </c>
+      <c r="O17" s="14">
+        <v>45455</v>
+      </c>
+      <c r="P17" s="22">
+        <v>27</v>
+      </c>
+      <c r="Q17" s="35"/>
+      <c r="R17" s="35"/>
+      <c r="S17" s="35"/>
+      <c r="T17" s="35"/>
+      <c r="U17" s="35"/>
+    </row>
+    <row r="18" spans="1:21" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1"/>
       <c r="B18" s="7" t="str">
         <v>B</v>
@@ -2714,15 +2781,31 @@
       <c r="J18">
         <v>58</v>
       </c>
-      <c r="K18" s="5" t="str">
+      <c r="K18" s="32">
         <v>45457</v>
       </c>
       <c r="L18" t="str">
         <v>A</v>
       </c>
-      <c r="O18" s="2"/>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="M18" s="12" t="str">
+        <v>B</v>
+      </c>
+      <c r="N18" s="18">
+        <v>45487</v>
+      </c>
+      <c r="O18" s="14">
+        <v>45455</v>
+      </c>
+      <c r="P18" s="22">
+        <v>51</v>
+      </c>
+      <c r="Q18" s="35"/>
+      <c r="R18" s="35"/>
+      <c r="S18" s="35"/>
+      <c r="T18" s="35"/>
+      <c r="U18" s="35"/>
+    </row>
+    <row r="19" spans="1:21" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A19" s="1"/>
       <c r="B19" s="7" t="str">
         <v>B</v>
@@ -2745,14 +2828,31 @@
       <c r="J19">
         <v>32</v>
       </c>
-      <c r="K19" s="5" t="str">
+      <c r="K19" s="32">
         <v>45457</v>
       </c>
       <c r="L19" t="str">
         <v>A</v>
       </c>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="M19" s="12" t="str">
+        <v>B</v>
+      </c>
+      <c r="N19" s="18">
+        <v>45487</v>
+      </c>
+      <c r="O19" s="19">
+        <v>45456</v>
+      </c>
+      <c r="P19" s="22">
+        <v>7</v>
+      </c>
+      <c r="Q19" s="35"/>
+      <c r="R19" s="35"/>
+      <c r="S19" s="35"/>
+      <c r="T19" s="35"/>
+      <c r="U19" s="35"/>
+    </row>
+    <row r="20" spans="1:21" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A20" s="1"/>
       <c r="B20" s="7" t="str">
         <v>C</v>
@@ -2775,15 +2875,31 @@
       <c r="J20">
         <v>42</v>
       </c>
-      <c r="K20" s="5" t="str">
+      <c r="K20" s="32">
         <v>45457</v>
       </c>
       <c r="L20" t="str">
         <v>A</v>
       </c>
-      <c r="O20" s="2"/>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="M20" s="12" t="str">
+        <v>C</v>
+      </c>
+      <c r="N20" s="18">
+        <v>45489</v>
+      </c>
+      <c r="O20" s="19">
+        <v>45456</v>
+      </c>
+      <c r="P20" s="22">
+        <v>20</v>
+      </c>
+      <c r="Q20" s="35"/>
+      <c r="R20" s="35"/>
+      <c r="S20" s="35"/>
+      <c r="T20" s="35"/>
+      <c r="U20" s="35"/>
+    </row>
+    <row r="21" spans="1:21" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A21" s="1"/>
       <c r="B21" s="7" t="str">
         <v>C</v>
@@ -2806,14 +2922,31 @@
       <c r="J21">
         <v>23</v>
       </c>
-      <c r="K21" s="5" t="str">
+      <c r="K21" s="32">
         <v>45457</v>
       </c>
       <c r="L21" t="str">
         <v>A</v>
       </c>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="M21" s="12" t="str">
+        <v>C</v>
+      </c>
+      <c r="N21" s="18">
+        <v>45489</v>
+      </c>
+      <c r="O21" s="19">
+        <v>45464</v>
+      </c>
+      <c r="P21" s="22">
+        <v>12</v>
+      </c>
+      <c r="Q21" s="35"/>
+      <c r="R21" s="35"/>
+      <c r="S21" s="35"/>
+      <c r="T21" s="35"/>
+      <c r="U21" s="35"/>
+    </row>
+    <row r="22" spans="1:21" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A22" s="1"/>
       <c r="B22" s="7" t="str">
         <v>D</v>
@@ -2831,15 +2964,31 @@
         <v>45455</v>
       </c>
       <c r="I22" s="5"/>
-      <c r="K22" s="5" t="str">
+      <c r="K22" s="32">
         <v>45457</v>
       </c>
       <c r="L22" t="str">
         <v>A</v>
       </c>
-      <c r="O22" s="2"/>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="M22" s="12" t="str">
+        <v>D</v>
+      </c>
+      <c r="N22" s="18">
+        <v>45520</v>
+      </c>
+      <c r="O22" s="19">
+        <v>45464</v>
+      </c>
+      <c r="P22" s="22">
+        <v>3</v>
+      </c>
+      <c r="Q22" s="35"/>
+      <c r="R22" s="35"/>
+      <c r="S22" s="35"/>
+      <c r="T22" s="35"/>
+      <c r="U22" s="35"/>
+    </row>
+    <row r="23" spans="1:21" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A23" s="1"/>
       <c r="B23" s="7" t="str">
         <v>D</v>
@@ -2857,14 +3006,31 @@
         <v>45455</v>
       </c>
       <c r="I23" s="5"/>
-      <c r="K23" s="5" t="str">
+      <c r="K23" s="32">
         <v>45457</v>
       </c>
       <c r="L23" t="str">
         <v>A</v>
       </c>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="M23" s="12" t="str">
+        <v>D</v>
+      </c>
+      <c r="N23" s="18">
+        <v>45520</v>
+      </c>
+      <c r="O23" s="19">
+        <v>45486</v>
+      </c>
+      <c r="P23" s="25">
+        <v>38</v>
+      </c>
+      <c r="Q23" s="35"/>
+      <c r="R23" s="35"/>
+      <c r="S23" s="35"/>
+      <c r="T23" s="35"/>
+      <c r="U23" s="35"/>
+    </row>
+    <row r="24" spans="1:21" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B24" s="7" t="str">
         <v>D</v>
       </c>
@@ -2881,14 +3047,31 @@
         <v>45455</v>
       </c>
       <c r="I24" s="5"/>
-      <c r="K24" s="5" t="str">
+      <c r="K24" s="32">
         <v>45457</v>
       </c>
       <c r="L24" t="str">
         <v>A</v>
       </c>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="M24" s="12" t="str">
+        <v>D</v>
+      </c>
+      <c r="N24" s="18">
+        <v>45520</v>
+      </c>
+      <c r="O24" s="24">
+        <v>45502</v>
+      </c>
+      <c r="P24" s="25">
+        <v>1</v>
+      </c>
+      <c r="Q24" s="35"/>
+      <c r="R24" s="35"/>
+      <c r="S24" s="35"/>
+      <c r="T24" s="35"/>
+      <c r="U24" s="35"/>
+    </row>
+    <row r="25" spans="1:21" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B25" s="7" t="str">
         <v>E</v>
       </c>
@@ -2905,14 +3088,31 @@
         <v>45455</v>
       </c>
       <c r="I25" s="5"/>
-      <c r="K25" s="5" t="str">
+      <c r="K25" s="32">
         <v>45457</v>
       </c>
       <c r="L25" t="str">
         <v>A</v>
       </c>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="M25" s="13" t="str">
+        <v>E</v>
+      </c>
+      <c r="N25" s="20">
+        <v>45523</v>
+      </c>
+      <c r="O25" s="21">
+        <v>45502</v>
+      </c>
+      <c r="P25" s="23">
+        <v>23</v>
+      </c>
+      <c r="Q25" s="35"/>
+      <c r="R25" s="35"/>
+      <c r="S25" s="35"/>
+      <c r="T25" s="35"/>
+      <c r="U25" s="35"/>
+    </row>
+    <row r="26" spans="1:21" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B26" s="7"/>
       <c r="C26" s="7"/>
       <c r="E26" s="7"/>
@@ -2920,89 +3120,98 @@
         <v>45455</v>
       </c>
       <c r="I26" s="5"/>
-      <c r="K26" s="5" t="str">
+      <c r="K26" s="32">
         <v>45457</v>
       </c>
       <c r="L26" t="str">
         <v>A</v>
       </c>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="M26" s="35"/>
+      <c r="N26" s="35"/>
+      <c r="O26" s="35"/>
+      <c r="P26" s="35"/>
+      <c r="Q26" s="35"/>
+      <c r="R26" s="35"/>
+      <c r="S26" s="35"/>
+      <c r="T26" s="35"/>
+      <c r="U26" s="35"/>
+    </row>
+    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B27" s="7"/>
       <c r="D27" s="7"/>
       <c r="G27" s="5">
         <v>45455</v>
       </c>
       <c r="I27" s="5"/>
-      <c r="K27" s="5" t="str">
+      <c r="K27" s="32">
         <v>45457</v>
       </c>
       <c r="L27" t="str">
         <v>A</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B28" s="7"/>
       <c r="D28" s="7"/>
       <c r="G28" s="5">
         <v>45455</v>
       </c>
       <c r="I28" s="5"/>
-      <c r="K28" s="5" t="str">
+      <c r="K28" s="32">
         <v>45457</v>
       </c>
       <c r="L28" t="str">
         <v>A</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B29" s="7"/>
       <c r="G29" s="5">
         <v>45455</v>
       </c>
       <c r="I29" s="5"/>
-      <c r="K29" s="5" t="str">
+      <c r="K29" s="32">
         <v>45457</v>
       </c>
       <c r="L29" t="str">
         <v>A</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B30" s="7"/>
       <c r="D30" s="7"/>
       <c r="G30" s="5">
         <v>45455</v>
       </c>
       <c r="I30" s="5"/>
-      <c r="K30" s="5" t="str">
+      <c r="K30" s="32">
         <v>45457</v>
       </c>
       <c r="L30" t="str">
         <v>A</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B31" s="7"/>
       <c r="D31" s="7"/>
       <c r="G31" s="5">
         <v>45455</v>
       </c>
       <c r="I31" s="5"/>
-      <c r="K31" s="5" t="str">
+      <c r="K31" s="32">
         <v>45457</v>
       </c>
       <c r="L31" t="str">
         <v>A</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B32" s="7"/>
       <c r="G32" s="5">
         <v>45455</v>
       </c>
       <c r="I32" s="5"/>
-      <c r="K32" s="5" t="str">
+      <c r="K32" s="32">
         <v>45457</v>
       </c>
       <c r="L32" t="str">
@@ -3015,7 +3224,7 @@
         <v>45455</v>
       </c>
       <c r="I33" s="5"/>
-      <c r="K33" s="5" t="str">
+      <c r="K33" s="32">
         <v>45457</v>
       </c>
       <c r="L33" t="str">
@@ -3028,7 +3237,7 @@
         <v>45455</v>
       </c>
       <c r="I34" s="5"/>
-      <c r="K34" s="5" t="str">
+      <c r="K34" s="32">
         <v>45457</v>
       </c>
       <c r="L34" t="str">
@@ -3041,7 +3250,7 @@
         <v>45455</v>
       </c>
       <c r="I35" s="5"/>
-      <c r="K35" s="5" t="str">
+      <c r="K35" s="32">
         <v>45457</v>
       </c>
       <c r="L35" t="str">
@@ -3054,7 +3263,7 @@
         <v>45455</v>
       </c>
       <c r="I36" s="5"/>
-      <c r="K36" s="5" t="str">
+      <c r="K36" s="32">
         <v>45457</v>
       </c>
       <c r="L36" t="str">
@@ -3066,7 +3275,7 @@
         <v>45455</v>
       </c>
       <c r="I37" s="5"/>
-      <c r="K37" s="5" t="str">
+      <c r="K37" s="32">
         <v>45457</v>
       </c>
       <c r="L37" t="str">
@@ -3078,7 +3287,7 @@
         <v>45455</v>
       </c>
       <c r="I38" s="5"/>
-      <c r="K38" s="5" t="str">
+      <c r="K38" s="32">
         <v>45457</v>
       </c>
       <c r="L38" t="str">
@@ -3090,7 +3299,7 @@
         <v>45455</v>
       </c>
       <c r="I39" s="5"/>
-      <c r="K39" s="5" t="str">
+      <c r="K39" s="32">
         <v>45457</v>
       </c>
       <c r="L39" t="str">
@@ -3102,7 +3311,7 @@
         <v>45455</v>
       </c>
       <c r="I40" s="5"/>
-      <c r="K40" s="5" t="str">
+      <c r="K40" s="32">
         <v>45457</v>
       </c>
       <c r="L40" t="str">
@@ -3114,7 +3323,7 @@
         <v>45455</v>
       </c>
       <c r="I41" s="5"/>
-      <c r="K41" s="5" t="str">
+      <c r="K41" s="32">
         <v>45457</v>
       </c>
       <c r="L41" t="str">
@@ -3126,7 +3335,7 @@
         <v>45455</v>
       </c>
       <c r="I42" s="5"/>
-      <c r="K42" s="5" t="str">
+      <c r="K42" s="32">
         <v>45457</v>
       </c>
       <c r="L42" t="str">
@@ -3138,7 +3347,7 @@
         <v>45455</v>
       </c>
       <c r="I43" s="5"/>
-      <c r="K43" s="5" t="str">
+      <c r="K43" s="32">
         <v>45457</v>
       </c>
       <c r="L43" t="str">
@@ -3150,7 +3359,7 @@
         <v>45455</v>
       </c>
       <c r="I44" s="5"/>
-      <c r="K44" s="5" t="str">
+      <c r="K44" s="32">
         <v>45487</v>
       </c>
       <c r="L44" t="str">
@@ -3162,7 +3371,7 @@
         <v>45455</v>
       </c>
       <c r="I45" s="5"/>
-      <c r="K45" s="5" t="str">
+      <c r="K45" s="32">
         <v>45487</v>
       </c>
       <c r="L45" t="str">
@@ -3174,7 +3383,7 @@
         <v>45455</v>
       </c>
       <c r="I46" s="5"/>
-      <c r="K46" s="5" t="str">
+      <c r="K46" s="32">
         <v>45487</v>
       </c>
       <c r="L46" t="str">
@@ -3186,7 +3395,7 @@
         <v>45455</v>
       </c>
       <c r="I47" s="5"/>
-      <c r="K47" s="5" t="str">
+      <c r="K47" s="32">
         <v>45487</v>
       </c>
       <c r="L47" t="str">
@@ -3198,7 +3407,7 @@
         <v>45455</v>
       </c>
       <c r="I48" s="5"/>
-      <c r="K48" s="5" t="str">
+      <c r="K48" s="32">
         <v>45487</v>
       </c>
       <c r="L48" t="str">
@@ -3210,7 +3419,7 @@
         <v>45455</v>
       </c>
       <c r="I49" s="5"/>
-      <c r="K49" s="5" t="str">
+      <c r="K49" s="32">
         <v>45487</v>
       </c>
       <c r="L49" t="str">
@@ -3222,7 +3431,7 @@
         <v>45455</v>
       </c>
       <c r="I50" s="5"/>
-      <c r="K50" s="5" t="str">
+      <c r="K50" s="32">
         <v>45487</v>
       </c>
       <c r="L50" t="str">
@@ -3234,7 +3443,7 @@
         <v>45455</v>
       </c>
       <c r="I51" s="5"/>
-      <c r="K51" s="5" t="str">
+      <c r="K51" s="32">
         <v>45487</v>
       </c>
       <c r="L51" t="str">
@@ -3246,7 +3455,7 @@
         <v>45455</v>
       </c>
       <c r="I52" s="5"/>
-      <c r="K52" s="5" t="str">
+      <c r="K52" s="32">
         <v>45487</v>
       </c>
       <c r="L52" t="str">
@@ -3258,7 +3467,7 @@
         <v>45455</v>
       </c>
       <c r="I53" s="5"/>
-      <c r="K53" s="5" t="str">
+      <c r="K53" s="32">
         <v>45487</v>
       </c>
       <c r="L53" t="str">
@@ -3270,7 +3479,7 @@
         <v>45455</v>
       </c>
       <c r="I54" s="5"/>
-      <c r="K54" s="5" t="str">
+      <c r="K54" s="32">
         <v>45487</v>
       </c>
       <c r="L54" t="str">
@@ -3282,7 +3491,7 @@
         <v>45455</v>
       </c>
       <c r="I55" s="5"/>
-      <c r="K55" s="5" t="str">
+      <c r="K55" s="32">
         <v>45487</v>
       </c>
       <c r="L55" t="str">
@@ -3294,7 +3503,7 @@
         <v>45455</v>
       </c>
       <c r="I56" s="5"/>
-      <c r="K56" s="5" t="str">
+      <c r="K56" s="32">
         <v>45487</v>
       </c>
       <c r="L56" t="str">
@@ -3306,7 +3515,7 @@
         <v>45455</v>
       </c>
       <c r="I57" s="5"/>
-      <c r="K57" s="5" t="str">
+      <c r="K57" s="32">
         <v>45487</v>
       </c>
       <c r="L57" t="str">
@@ -3318,7 +3527,7 @@
         <v>45455</v>
       </c>
       <c r="I58" s="5"/>
-      <c r="K58" s="5" t="str">
+      <c r="K58" s="32">
         <v>45487</v>
       </c>
       <c r="L58" t="str">
@@ -3330,7 +3539,7 @@
         <v>45455</v>
       </c>
       <c r="I59" s="5"/>
-      <c r="K59" s="5" t="str">
+      <c r="K59" s="32">
         <v>45487</v>
       </c>
       <c r="L59" t="str">
@@ -3342,7 +3551,7 @@
         <v>45455</v>
       </c>
       <c r="I60" s="5"/>
-      <c r="K60" s="5" t="str">
+      <c r="K60" s="32">
         <v>45487</v>
       </c>
       <c r="L60" t="str">
@@ -3354,7 +3563,7 @@
         <v>45455</v>
       </c>
       <c r="I61" s="5"/>
-      <c r="K61" s="5" t="str">
+      <c r="K61" s="32">
         <v>45487</v>
       </c>
       <c r="L61" t="str">
@@ -3366,7 +3575,7 @@
         <v>45455</v>
       </c>
       <c r="I62" s="5"/>
-      <c r="K62" s="5" t="str">
+      <c r="K62" s="32">
         <v>45487</v>
       </c>
       <c r="L62" t="str">
@@ -3378,7 +3587,7 @@
         <v>45455</v>
       </c>
       <c r="I63" s="5"/>
-      <c r="K63" s="5" t="str">
+      <c r="K63" s="32">
         <v>45487</v>
       </c>
       <c r="L63" t="str">
@@ -3390,7 +3599,7 @@
         <v>45455</v>
       </c>
       <c r="I64" s="5"/>
-      <c r="K64" s="5" t="str">
+      <c r="K64" s="32">
         <v>45487</v>
       </c>
       <c r="L64" t="str">
@@ -3402,7 +3611,7 @@
         <v>45455</v>
       </c>
       <c r="I65" s="5"/>
-      <c r="K65" s="5" t="str">
+      <c r="K65" s="32">
         <v>45487</v>
       </c>
       <c r="L65" t="str">
@@ -3414,7 +3623,7 @@
         <v>45455</v>
       </c>
       <c r="I66" s="5"/>
-      <c r="K66" s="5" t="str">
+      <c r="K66" s="32">
         <v>45487</v>
       </c>
       <c r="L66" t="str">
@@ -3426,7 +3635,7 @@
         <v>45455</v>
       </c>
       <c r="I67" s="5"/>
-      <c r="K67" s="5" t="str">
+      <c r="K67" s="32">
         <v>45487</v>
       </c>
       <c r="L67" t="str">
@@ -3438,7 +3647,7 @@
         <v>45455</v>
       </c>
       <c r="I68" s="5"/>
-      <c r="K68" s="5" t="str">
+      <c r="K68" s="32">
         <v>45487</v>
       </c>
       <c r="L68" t="str">
@@ -3450,7 +3659,7 @@
         <v>45455</v>
       </c>
       <c r="I69" s="5"/>
-      <c r="K69" s="5" t="str">
+      <c r="K69" s="32">
         <v>45487</v>
       </c>
       <c r="L69" t="str">
@@ -3462,7 +3671,7 @@
         <v>45455</v>
       </c>
       <c r="I70" s="5"/>
-      <c r="K70" s="5" t="str">
+      <c r="K70" s="32">
         <v>45487</v>
       </c>
       <c r="L70" t="str">
@@ -3474,7 +3683,7 @@
         <v>45455</v>
       </c>
       <c r="I71" s="5"/>
-      <c r="K71" s="5" t="str">
+      <c r="K71" s="32">
         <v>45487</v>
       </c>
       <c r="L71" t="str">
@@ -3486,7 +3695,7 @@
         <v>45455</v>
       </c>
       <c r="I72" s="5"/>
-      <c r="K72" s="5" t="str">
+      <c r="K72" s="32">
         <v>45487</v>
       </c>
       <c r="L72" t="str">
@@ -3498,7 +3707,7 @@
         <v>45455</v>
       </c>
       <c r="I73" s="5"/>
-      <c r="K73" s="5" t="str">
+      <c r="K73" s="32">
         <v>45487</v>
       </c>
       <c r="L73" t="str">
@@ -3510,7 +3719,7 @@
         <v>45455</v>
       </c>
       <c r="I74" s="5"/>
-      <c r="K74" s="5" t="str">
+      <c r="K74" s="32">
         <v>45487</v>
       </c>
       <c r="L74" t="str">
@@ -3522,7 +3731,7 @@
         <v>45455</v>
       </c>
       <c r="I75" s="5"/>
-      <c r="K75" s="5" t="str">
+      <c r="K75" s="32">
         <v>45487</v>
       </c>
       <c r="L75" t="str">
@@ -3534,7 +3743,7 @@
         <v>45455</v>
       </c>
       <c r="I76" s="5"/>
-      <c r="K76" s="5" t="str">
+      <c r="K76" s="32">
         <v>45487</v>
       </c>
       <c r="L76" t="str">
@@ -3546,7 +3755,7 @@
         <v>45455</v>
       </c>
       <c r="I77" s="5"/>
-      <c r="K77" s="5" t="str">
+      <c r="K77" s="32">
         <v>45487</v>
       </c>
       <c r="L77" t="str">
@@ -3558,7 +3767,7 @@
         <v>45455</v>
       </c>
       <c r="I78" s="5"/>
-      <c r="K78" s="5" t="str">
+      <c r="K78" s="32">
         <v>45487</v>
       </c>
       <c r="L78" t="str">
@@ -3570,7 +3779,7 @@
         <v>45455</v>
       </c>
       <c r="I79" s="5"/>
-      <c r="K79" s="5" t="str">
+      <c r="K79" s="32">
         <v>45487</v>
       </c>
       <c r="L79" t="str">
@@ -3582,7 +3791,7 @@
         <v>45455</v>
       </c>
       <c r="I80" s="5"/>
-      <c r="K80" s="5" t="str">
+      <c r="K80" s="32">
         <v>45487</v>
       </c>
       <c r="L80" t="str">
@@ -3594,7 +3803,7 @@
         <v>45455</v>
       </c>
       <c r="I81" s="5"/>
-      <c r="K81" s="5" t="str">
+      <c r="K81" s="32">
         <v>45487</v>
       </c>
       <c r="L81" t="str">
@@ -3606,7 +3815,7 @@
         <v>45455</v>
       </c>
       <c r="I82" s="5"/>
-      <c r="K82" s="5" t="str">
+      <c r="K82" s="32">
         <v>45487</v>
       </c>
       <c r="L82" t="str">
@@ -3618,7 +3827,7 @@
         <v>45455</v>
       </c>
       <c r="I83" s="5"/>
-      <c r="K83" s="5" t="str">
+      <c r="K83" s="32">
         <v>45487</v>
       </c>
       <c r="L83" t="str">
@@ -3630,7 +3839,7 @@
         <v>45455</v>
       </c>
       <c r="I84" s="5"/>
-      <c r="K84" s="5" t="str">
+      <c r="K84" s="32">
         <v>45487</v>
       </c>
       <c r="L84" t="str">
@@ -3642,7 +3851,7 @@
         <v>45455</v>
       </c>
       <c r="I85" s="5"/>
-      <c r="K85" s="5" t="str">
+      <c r="K85" s="32">
         <v>45487</v>
       </c>
       <c r="L85" t="str">
@@ -3654,7 +3863,7 @@
         <v>45455</v>
       </c>
       <c r="I86" s="5"/>
-      <c r="K86" s="5" t="str">
+      <c r="K86" s="32">
         <v>45487</v>
       </c>
       <c r="L86" t="str">
@@ -3666,7 +3875,7 @@
         <v>45455</v>
       </c>
       <c r="I87" s="5"/>
-      <c r="K87" s="5" t="str">
+      <c r="K87" s="32">
         <v>45487</v>
       </c>
       <c r="L87" t="str">
@@ -3678,7 +3887,7 @@
         <v>45455</v>
       </c>
       <c r="I88" s="5"/>
-      <c r="K88" s="5" t="str">
+      <c r="K88" s="32">
         <v>45487</v>
       </c>
       <c r="L88" t="str">
@@ -3690,7 +3899,7 @@
         <v>45455</v>
       </c>
       <c r="I89" s="5"/>
-      <c r="K89" s="5" t="str">
+      <c r="K89" s="32">
         <v>45487</v>
       </c>
       <c r="L89" t="str">
@@ -3702,7 +3911,7 @@
         <v>45455</v>
       </c>
       <c r="I90" s="5"/>
-      <c r="K90" s="5" t="str">
+      <c r="K90" s="32">
         <v>45487</v>
       </c>
       <c r="L90" t="str">
@@ -3714,7 +3923,7 @@
         <v>45455</v>
       </c>
       <c r="I91" s="5"/>
-      <c r="K91" s="5" t="str">
+      <c r="K91" s="32">
         <v>45487</v>
       </c>
       <c r="L91" t="str">
@@ -3726,7 +3935,7 @@
         <v>45455</v>
       </c>
       <c r="I92" s="5"/>
-      <c r="K92" s="5" t="str">
+      <c r="K92" s="32">
         <v>45487</v>
       </c>
       <c r="L92" t="str">
@@ -3738,7 +3947,7 @@
         <v>45455</v>
       </c>
       <c r="I93" s="5"/>
-      <c r="K93" s="5" t="str">
+      <c r="K93" s="32">
         <v>45487</v>
       </c>
       <c r="L93" t="str">
@@ -3750,7 +3959,7 @@
         <v>45455</v>
       </c>
       <c r="I94" s="5"/>
-      <c r="K94" s="5" t="str">
+      <c r="K94" s="32">
         <v>45487</v>
       </c>
       <c r="L94" t="str">
@@ -3762,7 +3971,7 @@
         <v>45456</v>
       </c>
       <c r="I95" s="5"/>
-      <c r="K95" s="5" t="str">
+      <c r="K95" s="32">
         <v>45487</v>
       </c>
       <c r="L95" t="str">
@@ -3774,7 +3983,7 @@
         <v>45456</v>
       </c>
       <c r="I96" s="5"/>
-      <c r="K96" s="5" t="str">
+      <c r="K96" s="32">
         <v>45487</v>
       </c>
       <c r="L96" t="str">
@@ -3786,7 +3995,7 @@
         <v>45456</v>
       </c>
       <c r="I97" s="5"/>
-      <c r="K97" s="5" t="str">
+      <c r="K97" s="32">
         <v>45487</v>
       </c>
       <c r="L97" t="str">
@@ -3798,7 +4007,7 @@
         <v>45456</v>
       </c>
       <c r="I98" s="5"/>
-      <c r="K98" s="5" t="str">
+      <c r="K98" s="32">
         <v>45487</v>
       </c>
       <c r="L98" t="str">
@@ -3810,7 +4019,7 @@
         <v>45456</v>
       </c>
       <c r="I99" s="5"/>
-      <c r="K99" s="5" t="str">
+      <c r="K99" s="32">
         <v>45487</v>
       </c>
       <c r="L99" t="str">
@@ -3822,7 +4031,7 @@
         <v>45456</v>
       </c>
       <c r="I100" s="5"/>
-      <c r="K100" s="5" t="str">
+      <c r="K100" s="32">
         <v>45487</v>
       </c>
       <c r="L100" t="str">
@@ -3834,7 +4043,7 @@
         <v>45456</v>
       </c>
       <c r="I101" s="5"/>
-      <c r="K101" s="5" t="str">
+      <c r="K101" s="32">
         <v>45487</v>
       </c>
       <c r="L101" t="str">
@@ -3846,7 +4055,7 @@
         <v>45456</v>
       </c>
       <c r="I102" s="5"/>
-      <c r="K102" s="5" t="str">
+      <c r="K102" s="32">
         <v>45489</v>
       </c>
       <c r="L102" t="str">
@@ -3858,7 +4067,7 @@
         <v>45456</v>
       </c>
       <c r="I103" s="5"/>
-      <c r="K103" s="5" t="str">
+      <c r="K103" s="32">
         <v>45489</v>
       </c>
       <c r="L103" t="str">
@@ -3870,7 +4079,7 @@
         <v>45456</v>
       </c>
       <c r="I104" s="5"/>
-      <c r="K104" s="5" t="str">
+      <c r="K104" s="32">
         <v>45489</v>
       </c>
       <c r="L104" t="str">
@@ -3882,7 +4091,7 @@
         <v>45456</v>
       </c>
       <c r="I105" s="5"/>
-      <c r="K105" s="5" t="str">
+      <c r="K105" s="32">
         <v>45489</v>
       </c>
       <c r="L105" t="str">
@@ -3894,7 +4103,7 @@
         <v>45456</v>
       </c>
       <c r="I106" s="5"/>
-      <c r="K106" s="5" t="str">
+      <c r="K106" s="32">
         <v>45489</v>
       </c>
       <c r="L106" t="str">
@@ -3906,7 +4115,7 @@
         <v>45456</v>
       </c>
       <c r="I107" s="5"/>
-      <c r="K107" s="5" t="str">
+      <c r="K107" s="32">
         <v>45489</v>
       </c>
       <c r="L107" t="str">
@@ -3918,7 +4127,7 @@
         <v>45456</v>
       </c>
       <c r="I108" s="5"/>
-      <c r="K108" s="5" t="str">
+      <c r="K108" s="32">
         <v>45489</v>
       </c>
       <c r="L108" t="str">
@@ -3930,7 +4139,7 @@
         <v>45456</v>
       </c>
       <c r="I109" s="5"/>
-      <c r="K109" s="5" t="str">
+      <c r="K109" s="32">
         <v>45489</v>
       </c>
       <c r="L109" t="str">
@@ -3942,7 +4151,7 @@
         <v>45456</v>
       </c>
       <c r="I110" s="5"/>
-      <c r="K110" s="5" t="str">
+      <c r="K110" s="32">
         <v>45489</v>
       </c>
       <c r="L110" t="str">
@@ -3954,7 +4163,7 @@
         <v>45456</v>
       </c>
       <c r="I111" s="5"/>
-      <c r="K111" s="5" t="str">
+      <c r="K111" s="32">
         <v>45489</v>
       </c>
       <c r="L111" t="str">
@@ -3966,7 +4175,7 @@
         <v>45456</v>
       </c>
       <c r="I112" s="5"/>
-      <c r="K112" s="5" t="str">
+      <c r="K112" s="32">
         <v>45489</v>
       </c>
       <c r="L112" t="str">
@@ -3978,7 +4187,7 @@
         <v>45456</v>
       </c>
       <c r="I113" s="5"/>
-      <c r="K113" s="5" t="str">
+      <c r="K113" s="32">
         <v>45489</v>
       </c>
       <c r="L113" t="str">
@@ -3990,7 +4199,7 @@
         <v>45456</v>
       </c>
       <c r="I114" s="5"/>
-      <c r="K114" s="5" t="str">
+      <c r="K114" s="32">
         <v>45489</v>
       </c>
       <c r="L114" t="str">
@@ -4002,7 +4211,7 @@
         <v>45456</v>
       </c>
       <c r="I115" s="5"/>
-      <c r="K115" s="5" t="str">
+      <c r="K115" s="32">
         <v>45489</v>
       </c>
       <c r="L115" t="str">
@@ -4014,7 +4223,7 @@
         <v>45456</v>
       </c>
       <c r="I116" s="5"/>
-      <c r="K116" s="5" t="str">
+      <c r="K116" s="32">
         <v>45489</v>
       </c>
       <c r="L116" t="str">
@@ -4026,7 +4235,7 @@
         <v>45456</v>
       </c>
       <c r="I117" s="5"/>
-      <c r="K117" s="5" t="str">
+      <c r="K117" s="32">
         <v>45489</v>
       </c>
       <c r="L117" t="str">
@@ -4038,7 +4247,7 @@
         <v>45456</v>
       </c>
       <c r="I118" s="5"/>
-      <c r="K118" s="5" t="str">
+      <c r="K118" s="32">
         <v>45489</v>
       </c>
       <c r="L118" t="str">
@@ -4050,7 +4259,7 @@
         <v>45456</v>
       </c>
       <c r="I119" s="5"/>
-      <c r="K119" s="5" t="str">
+      <c r="K119" s="32">
         <v>45489</v>
       </c>
       <c r="L119" t="str">
@@ -4062,7 +4271,7 @@
         <v>45456</v>
       </c>
       <c r="I120" s="5"/>
-      <c r="K120" s="5" t="str">
+      <c r="K120" s="32">
         <v>45489</v>
       </c>
       <c r="L120" t="str">
@@ -4074,7 +4283,7 @@
         <v>45456</v>
       </c>
       <c r="I121" s="5"/>
-      <c r="K121" s="5" t="str">
+      <c r="K121" s="32">
         <v>45489</v>
       </c>
       <c r="L121" t="str">
@@ -4086,7 +4295,7 @@
         <v>45464</v>
       </c>
       <c r="I122" s="5"/>
-      <c r="K122" s="5" t="str">
+      <c r="K122" s="32">
         <v>45489</v>
       </c>
       <c r="L122" t="str">
@@ -4098,7 +4307,7 @@
         <v>45464</v>
       </c>
       <c r="I123" s="5"/>
-      <c r="K123" s="5" t="str">
+      <c r="K123" s="32">
         <v>45489</v>
       </c>
       <c r="L123" t="str">
@@ -4110,7 +4319,7 @@
         <v>45464</v>
       </c>
       <c r="I124" s="5"/>
-      <c r="K124" s="5" t="str">
+      <c r="K124" s="32">
         <v>45489</v>
       </c>
       <c r="L124" t="str">
@@ -4122,7 +4331,7 @@
         <v>45464</v>
       </c>
       <c r="I125" s="5"/>
-      <c r="K125" s="5" t="str">
+      <c r="K125" s="32">
         <v>45489</v>
       </c>
       <c r="L125" t="str">
@@ -4134,7 +4343,7 @@
         <v>45464</v>
       </c>
       <c r="I126" s="5"/>
-      <c r="K126" s="5" t="str">
+      <c r="K126" s="32">
         <v>45489</v>
       </c>
       <c r="L126" t="str">
@@ -4146,7 +4355,7 @@
         <v>45464</v>
       </c>
       <c r="I127" s="5"/>
-      <c r="K127" s="5" t="str">
+      <c r="K127" s="32">
         <v>45489</v>
       </c>
       <c r="L127" t="str">
@@ -4158,7 +4367,7 @@
         <v>45464</v>
       </c>
       <c r="I128" s="5"/>
-      <c r="K128" s="5" t="str">
+      <c r="K128" s="32">
         <v>45489</v>
       </c>
       <c r="L128" t="str">
@@ -4170,7 +4379,7 @@
         <v>45464</v>
       </c>
       <c r="I129" s="5"/>
-      <c r="K129" s="5" t="str">
+      <c r="K129" s="32">
         <v>45489</v>
       </c>
       <c r="L129" t="str">
@@ -4182,7 +4391,7 @@
         <v>45464</v>
       </c>
       <c r="I130" s="5"/>
-      <c r="K130" s="5" t="str">
+      <c r="K130" s="32">
         <v>45489</v>
       </c>
       <c r="L130" t="str">
@@ -4194,7 +4403,7 @@
         <v>45464</v>
       </c>
       <c r="I131" s="5"/>
-      <c r="K131" s="5" t="str">
+      <c r="K131" s="32">
         <v>45489</v>
       </c>
       <c r="L131" t="str">
@@ -4206,7 +4415,7 @@
         <v>45464</v>
       </c>
       <c r="I132" s="5"/>
-      <c r="K132" s="5" t="str">
+      <c r="K132" s="32">
         <v>45489</v>
       </c>
       <c r="L132" t="str">
@@ -4218,7 +4427,7 @@
         <v>45464</v>
       </c>
       <c r="I133" s="5"/>
-      <c r="K133" s="5" t="str">
+      <c r="K133" s="32">
         <v>45489</v>
       </c>
       <c r="L133" t="str">
@@ -4230,7 +4439,7 @@
         <v>45464</v>
       </c>
       <c r="I134" s="5"/>
-      <c r="K134" s="5" t="str">
+      <c r="K134" s="32">
         <v>45520</v>
       </c>
       <c r="L134" t="str">
@@ -4242,7 +4451,7 @@
         <v>45464</v>
       </c>
       <c r="I135" s="5"/>
-      <c r="K135" s="5" t="str">
+      <c r="K135" s="32">
         <v>45520</v>
       </c>
       <c r="L135" t="str">
@@ -4254,7 +4463,7 @@
         <v>45464</v>
       </c>
       <c r="I136" s="5"/>
-      <c r="K136" s="5" t="str">
+      <c r="K136" s="32">
         <v>45520</v>
       </c>
       <c r="L136" t="str">
@@ -4266,7 +4475,7 @@
         <v>45486</v>
       </c>
       <c r="I137" s="5"/>
-      <c r="K137" s="5" t="str">
+      <c r="K137" s="32">
         <v>45520</v>
       </c>
       <c r="L137" t="str">
@@ -4278,7 +4487,7 @@
         <v>45486</v>
       </c>
       <c r="I138" s="5"/>
-      <c r="K138" s="5" t="str">
+      <c r="K138" s="32">
         <v>45520</v>
       </c>
       <c r="L138" t="str">
@@ -4290,7 +4499,7 @@
         <v>45486</v>
       </c>
       <c r="I139" s="5"/>
-      <c r="K139" s="5" t="str">
+      <c r="K139" s="32">
         <v>45520</v>
       </c>
       <c r="L139" t="str">
@@ -4302,7 +4511,7 @@
         <v>45486</v>
       </c>
       <c r="I140" s="5"/>
-      <c r="K140" s="5" t="str">
+      <c r="K140" s="32">
         <v>45520</v>
       </c>
       <c r="L140" t="str">
@@ -4314,7 +4523,7 @@
         <v>45486</v>
       </c>
       <c r="I141" s="5"/>
-      <c r="K141" s="5" t="str">
+      <c r="K141" s="32">
         <v>45520</v>
       </c>
       <c r="L141" t="str">
@@ -4326,7 +4535,7 @@
         <v>45486</v>
       </c>
       <c r="I142" s="5"/>
-      <c r="K142" s="5" t="str">
+      <c r="K142" s="32">
         <v>45520</v>
       </c>
       <c r="L142" t="str">
@@ -4338,7 +4547,7 @@
         <v>45486</v>
       </c>
       <c r="I143" s="5"/>
-      <c r="K143" s="5" t="str">
+      <c r="K143" s="32">
         <v>45520</v>
       </c>
       <c r="L143" t="str">
@@ -4350,7 +4559,7 @@
         <v>45486</v>
       </c>
       <c r="I144" s="5"/>
-      <c r="K144" s="5" t="str">
+      <c r="K144" s="32">
         <v>45520</v>
       </c>
       <c r="L144" t="str">
@@ -4362,7 +4571,7 @@
         <v>45486</v>
       </c>
       <c r="I145" s="5"/>
-      <c r="K145" s="5" t="str">
+      <c r="K145" s="32">
         <v>45520</v>
       </c>
       <c r="L145" t="str">
@@ -4374,7 +4583,7 @@
         <v>45486</v>
       </c>
       <c r="I146" s="5"/>
-      <c r="K146" s="5" t="str">
+      <c r="K146" s="32">
         <v>45520</v>
       </c>
       <c r="L146" t="str">
@@ -4386,7 +4595,7 @@
         <v>45486</v>
       </c>
       <c r="I147" s="5"/>
-      <c r="K147" s="5" t="str">
+      <c r="K147" s="32">
         <v>45520</v>
       </c>
       <c r="L147" t="str">
@@ -4398,7 +4607,7 @@
         <v>45486</v>
       </c>
       <c r="I148" s="5"/>
-      <c r="K148" s="5" t="str">
+      <c r="K148" s="32">
         <v>45520</v>
       </c>
       <c r="L148" t="str">
@@ -4410,7 +4619,7 @@
         <v>45486</v>
       </c>
       <c r="I149" s="5"/>
-      <c r="K149" s="5" t="str">
+      <c r="K149" s="32">
         <v>45520</v>
       </c>
       <c r="L149" t="str">
@@ -4422,7 +4631,7 @@
         <v>45486</v>
       </c>
       <c r="I150" s="5"/>
-      <c r="K150" s="5" t="str">
+      <c r="K150" s="32">
         <v>45520</v>
       </c>
       <c r="L150" t="str">
@@ -4434,7 +4643,7 @@
         <v>45486</v>
       </c>
       <c r="I151" s="5"/>
-      <c r="K151" s="5" t="str">
+      <c r="K151" s="32">
         <v>45520</v>
       </c>
       <c r="L151" t="str">
@@ -4446,7 +4655,7 @@
         <v>45486</v>
       </c>
       <c r="I152" s="5"/>
-      <c r="K152" s="5" t="str">
+      <c r="K152" s="32">
         <v>45520</v>
       </c>
       <c r="L152" t="str">
@@ -4458,7 +4667,7 @@
         <v>45486</v>
       </c>
       <c r="I153" s="5"/>
-      <c r="K153" s="5" t="str">
+      <c r="K153" s="32">
         <v>45520</v>
       </c>
       <c r="L153" t="str">
@@ -4470,7 +4679,7 @@
         <v>45486</v>
       </c>
       <c r="I154" s="5"/>
-      <c r="K154" s="5" t="str">
+      <c r="K154" s="32">
         <v>45520</v>
       </c>
       <c r="L154" t="str">
@@ -4482,7 +4691,7 @@
         <v>45486</v>
       </c>
       <c r="I155" s="5"/>
-      <c r="K155" s="5" t="str">
+      <c r="K155" s="32">
         <v>45520</v>
       </c>
       <c r="L155" t="str">
@@ -4494,7 +4703,7 @@
         <v>45486</v>
       </c>
       <c r="I156" s="5"/>
-      <c r="K156" s="5" t="str">
+      <c r="K156" s="32">
         <v>45520</v>
       </c>
       <c r="L156" t="str">
@@ -4506,7 +4715,7 @@
         <v>45486</v>
       </c>
       <c r="I157" s="5"/>
-      <c r="K157" s="5" t="str">
+      <c r="K157" s="32">
         <v>45520</v>
       </c>
       <c r="L157" t="str">
@@ -4518,7 +4727,7 @@
         <v>45486</v>
       </c>
       <c r="I158" s="5"/>
-      <c r="K158" s="5" t="str">
+      <c r="K158" s="32">
         <v>45520</v>
       </c>
       <c r="L158" t="str">
@@ -4530,7 +4739,7 @@
         <v>45486</v>
       </c>
       <c r="I159" s="5"/>
-      <c r="K159" s="5" t="str">
+      <c r="K159" s="32">
         <v>45520</v>
       </c>
       <c r="L159" t="str">
@@ -4542,7 +4751,7 @@
         <v>45486</v>
       </c>
       <c r="I160" s="5"/>
-      <c r="K160" s="5" t="str">
+      <c r="K160" s="32">
         <v>45520</v>
       </c>
       <c r="L160" t="str">
@@ -4554,7 +4763,7 @@
         <v>45486</v>
       </c>
       <c r="I161" s="5"/>
-      <c r="K161" s="5" t="str">
+      <c r="K161" s="32">
         <v>45520</v>
       </c>
       <c r="L161" t="str">
@@ -4566,7 +4775,7 @@
         <v>45486</v>
       </c>
       <c r="I162" s="5"/>
-      <c r="K162" s="5" t="str">
+      <c r="K162" s="32">
         <v>45520</v>
       </c>
       <c r="L162" t="str">
@@ -4578,7 +4787,7 @@
         <v>45486</v>
       </c>
       <c r="I163" s="5"/>
-      <c r="K163" s="5" t="str">
+      <c r="K163" s="32">
         <v>45520</v>
       </c>
       <c r="L163" t="str">
@@ -4590,7 +4799,7 @@
         <v>45486</v>
       </c>
       <c r="I164" s="5"/>
-      <c r="K164" s="5" t="str">
+      <c r="K164" s="32">
         <v>45520</v>
       </c>
       <c r="L164" t="str">
@@ -4602,7 +4811,7 @@
         <v>45486</v>
       </c>
       <c r="I165" s="5"/>
-      <c r="K165" s="5" t="str">
+      <c r="K165" s="32">
         <v>45520</v>
       </c>
       <c r="L165" t="str">
@@ -4614,7 +4823,7 @@
         <v>45486</v>
       </c>
       <c r="I166" s="5"/>
-      <c r="K166" s="5" t="str">
+      <c r="K166" s="32">
         <v>45520</v>
       </c>
       <c r="L166" t="str">
@@ -4626,7 +4835,7 @@
         <v>45486</v>
       </c>
       <c r="I167" s="5"/>
-      <c r="K167" s="5" t="str">
+      <c r="K167" s="32">
         <v>45520</v>
       </c>
       <c r="L167" t="str">
@@ -4638,7 +4847,7 @@
         <v>45486</v>
       </c>
       <c r="I168" s="5"/>
-      <c r="K168" s="5" t="str">
+      <c r="K168" s="32">
         <v>45520</v>
       </c>
       <c r="L168" t="str">
@@ -4650,7 +4859,7 @@
         <v>45486</v>
       </c>
       <c r="I169" s="5"/>
-      <c r="K169" s="5" t="str">
+      <c r="K169" s="32">
         <v>45520</v>
       </c>
       <c r="L169" t="str">
@@ -4662,7 +4871,7 @@
         <v>45486</v>
       </c>
       <c r="I170" s="5"/>
-      <c r="K170" s="5" t="str">
+      <c r="K170" s="32">
         <v>45520</v>
       </c>
       <c r="L170" t="str">
@@ -4674,7 +4883,7 @@
         <v>45486</v>
       </c>
       <c r="I171" s="5"/>
-      <c r="K171" s="5" t="str">
+      <c r="K171" s="32">
         <v>45520</v>
       </c>
       <c r="L171" t="str">
@@ -4686,7 +4895,7 @@
         <v>45486</v>
       </c>
       <c r="I172" s="5"/>
-      <c r="K172" s="5" t="str">
+      <c r="K172" s="32">
         <v>45520</v>
       </c>
       <c r="L172" t="str">
@@ -4698,7 +4907,7 @@
         <v>45486</v>
       </c>
       <c r="I173" s="5"/>
-      <c r="K173" s="5" t="str">
+      <c r="K173" s="32">
         <v>45520</v>
       </c>
       <c r="L173" t="str">
@@ -4710,7 +4919,7 @@
         <v>45486</v>
       </c>
       <c r="I174" s="5"/>
-      <c r="K174" s="5" t="str">
+      <c r="K174" s="32">
         <v>45520</v>
       </c>
       <c r="L174" t="str">
@@ -4722,7 +4931,7 @@
         <v>45502</v>
       </c>
       <c r="I175" s="5"/>
-      <c r="K175" s="5" t="str">
+      <c r="K175" s="32">
         <v>45520</v>
       </c>
       <c r="L175" t="str">
@@ -4734,7 +4943,7 @@
         <v>45502</v>
       </c>
       <c r="I176" s="5"/>
-      <c r="K176" s="5" t="str">
+      <c r="K176" s="32">
         <v>45523</v>
       </c>
       <c r="L176" t="str">
@@ -4746,7 +4955,7 @@
         <v>45502</v>
       </c>
       <c r="I177" s="5"/>
-      <c r="K177" s="5" t="str">
+      <c r="K177" s="32">
         <v>45523</v>
       </c>
       <c r="L177" t="str">
@@ -4758,7 +4967,7 @@
         <v>45502</v>
       </c>
       <c r="I178" s="5"/>
-      <c r="K178" s="5" t="str">
+      <c r="K178" s="32">
         <v>45523</v>
       </c>
       <c r="L178" t="str">
@@ -4770,7 +4979,7 @@
         <v>45502</v>
       </c>
       <c r="I179" s="5"/>
-      <c r="K179" s="5" t="str">
+      <c r="K179" s="32">
         <v>45523</v>
       </c>
       <c r="L179" t="str">
@@ -4782,7 +4991,7 @@
         <v>45502</v>
       </c>
       <c r="I180" s="5"/>
-      <c r="K180" s="5" t="str">
+      <c r="K180" s="32">
         <v>45523</v>
       </c>
       <c r="L180" t="str">
@@ -4794,7 +5003,7 @@
         <v>45502</v>
       </c>
       <c r="I181" s="5"/>
-      <c r="K181" s="5" t="str">
+      <c r="K181" s="32">
         <v>45523</v>
       </c>
       <c r="L181" t="str">
@@ -4806,7 +5015,7 @@
         <v>45502</v>
       </c>
       <c r="I182" s="5"/>
-      <c r="K182" s="5" t="str">
+      <c r="K182" s="32">
         <v>45523</v>
       </c>
       <c r="L182" t="str">
@@ -4818,7 +5027,7 @@
         <v>45502</v>
       </c>
       <c r="I183" s="5"/>
-      <c r="K183" s="5" t="str">
+      <c r="K183" s="32">
         <v>45523</v>
       </c>
       <c r="L183" t="str">
@@ -4830,7 +5039,7 @@
         <v>45502</v>
       </c>
       <c r="I184" s="5"/>
-      <c r="K184" s="5" t="str">
+      <c r="K184" s="32">
         <v>45523</v>
       </c>
       <c r="L184" t="str">
@@ -4842,7 +5051,7 @@
         <v>45502</v>
       </c>
       <c r="I185" s="5"/>
-      <c r="K185" s="5" t="str">
+      <c r="K185" s="32">
         <v>45523</v>
       </c>
       <c r="L185" t="str">
@@ -4854,7 +5063,7 @@
         <v>45502</v>
       </c>
       <c r="I186" s="5"/>
-      <c r="K186" s="5" t="str">
+      <c r="K186" s="32">
         <v>45523</v>
       </c>
       <c r="L186" t="str">
@@ -4866,7 +5075,7 @@
         <v>45502</v>
       </c>
       <c r="I187" s="5"/>
-      <c r="K187" s="5" t="str">
+      <c r="K187" s="32">
         <v>45523</v>
       </c>
       <c r="L187" t="str">
@@ -4878,7 +5087,7 @@
         <v>45502</v>
       </c>
       <c r="I188" s="5"/>
-      <c r="K188" s="5" t="str">
+      <c r="K188" s="32">
         <v>45523</v>
       </c>
       <c r="L188" t="str">
@@ -4890,7 +5099,7 @@
         <v>45502</v>
       </c>
       <c r="I189" s="5"/>
-      <c r="K189" s="5" t="str">
+      <c r="K189" s="32">
         <v>45523</v>
       </c>
       <c r="L189" t="str">
@@ -4902,7 +5111,7 @@
         <v>45502</v>
       </c>
       <c r="I190" s="5"/>
-      <c r="K190" s="5" t="str">
+      <c r="K190" s="32">
         <v>45523</v>
       </c>
       <c r="L190" t="str">
@@ -4914,7 +5123,7 @@
         <v>45502</v>
       </c>
       <c r="I191" s="5"/>
-      <c r="K191" s="5" t="str">
+      <c r="K191" s="32">
         <v>45523</v>
       </c>
       <c r="L191" t="str">
@@ -4926,7 +5135,7 @@
         <v>45502</v>
       </c>
       <c r="I192" s="5"/>
-      <c r="K192" s="5" t="str">
+      <c r="K192" s="32">
         <v>45523</v>
       </c>
       <c r="L192" t="str">
@@ -4938,7 +5147,7 @@
         <v>45502</v>
       </c>
       <c r="I193" s="5"/>
-      <c r="K193" s="5" t="str">
+      <c r="K193" s="32">
         <v>45523</v>
       </c>
       <c r="L193" t="str">
@@ -4950,7 +5159,7 @@
         <v>45502</v>
       </c>
       <c r="I194" s="5"/>
-      <c r="K194" s="5" t="str">
+      <c r="K194" s="32">
         <v>45523</v>
       </c>
       <c r="L194" t="str">
@@ -4962,7 +5171,7 @@
         <v>45502</v>
       </c>
       <c r="I195" s="5"/>
-      <c r="K195" s="5" t="str">
+      <c r="K195" s="32">
         <v>45523</v>
       </c>
       <c r="L195" t="str">
@@ -4974,7 +5183,7 @@
         <v>45502</v>
       </c>
       <c r="I196" s="5"/>
-      <c r="K196" s="5" t="str">
+      <c r="K196" s="32">
         <v>45523</v>
       </c>
       <c r="L196" t="str">
@@ -4986,7 +5195,7 @@
         <v>45502</v>
       </c>
       <c r="I197" s="5"/>
-      <c r="K197" s="5" t="str">
+      <c r="K197" s="32">
         <v>45523</v>
       </c>
       <c r="L197" t="str">
@@ -4998,7 +5207,7 @@
         <v>45502</v>
       </c>
       <c r="I198" s="5"/>
-      <c r="K198" s="5" t="str">
+      <c r="K198" s="32">
         <v>45523</v>
       </c>
       <c r="L198" t="str">

</xml_diff>

<commit_message>
Cleaning up the EDA
</commit_message>
<xml_diff>
--- a/CH-130 FIFO.xlsx
+++ b/CH-130 FIFO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADDFF4AB-EF9E-4E6C-B851-903FF705A80D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B33C13C-14BF-4406-9ED1-643E2670F514}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -485,7 +485,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -584,6 +584,9 @@
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1645,8 +1648,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4C65EB1-3462-4A10-A150-765232CDCA14}">
   <dimension ref="A1:O308"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="K19" sqref="K19"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="M17" sqref="M17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1659,6 +1662,8 @@
     <col min="7" max="7" width="12.3984375" style="5" customWidth="1"/>
     <col min="8" max="8" width="11.5" customWidth="1"/>
     <col min="9" max="9" width="8.8984375" customWidth="1"/>
+    <col min="11" max="11" width="9.59765625" customWidth="1"/>
+    <col min="12" max="12" width="11.296875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" s="6" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1986,6 +1991,9 @@
         <v>23</v>
       </c>
       <c r="E13" s="7"/>
+      <c r="I13" s="39">
+        <v>0</v>
+      </c>
       <c r="L13" s="2"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
@@ -2184,6 +2192,22 @@
       <c r="B23" s="7"/>
       <c r="C23" s="7"/>
       <c r="E23" s="7"/>
+      <c r="G23" s="5">
+        <v>0</v>
+      </c>
+      <c r="J23" s="9" t="str" cm="1">
+        <f t="array" ref="J23:M23">F2:I2</f>
+        <v>Output</v>
+      </c>
+      <c r="K23" s="17" t="str">
+        <v>Registered Date</v>
+      </c>
+      <c r="L23" s="10" t="str">
+        <v>Source Date</v>
+      </c>
+      <c r="M23" s="11" t="str">
+        <v>Quantity</v>
+      </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B24" s="7"/>
@@ -2205,29 +2229,29 @@
         <v>Output A|45457</v>
       </c>
       <c r="F24" s="5" t="str" cm="1">
-        <f t="array" aca="1" ref="F24:G24" ca="1">_xlfn.TEXTSPLIT(E24,"|")</f>
+        <f t="array" aca="1" ref="F24:G24" ca="1">_xlfn.LET(_xlpm.z,_xlfn.TEXTSPLIT(E24,"|"),_xlfn.HSTACK(_xlfn.TAKE(_xlpm.z,,1),_xlfn.TAKE(_xlpm.z,,-1)+0))</f>
         <v>Output A</v>
       </c>
-      <c r="G24" s="5" t="str">
+      <c r="G24" s="5">
         <f ca="1"/>
         <v>45457</v>
       </c>
       <c r="H24">
         <v>45455</v>
       </c>
-      <c r="J24" t="str" cm="1">
-        <f t="array" aca="1" ref="J24:M33" ca="1">_xlfn.GROUPBY(F24:H205,H24:H205,_xleta.COUNTA)</f>
+      <c r="J24" s="12" t="str" cm="1">
+        <f t="array" aca="1" ref="J24:M32" ca="1">_xlfn.GROUPBY(F24:H205,H24:H205,_xleta.COUNTA,,0)</f>
         <v>Output A</v>
       </c>
-      <c r="K24" t="str">
+      <c r="K24" s="18">
         <f ca="1"/>
         <v>45457</v>
       </c>
-      <c r="L24">
-        <f ca="1"/>
-        <v>45455</v>
-      </c>
-      <c r="M24">
+      <c r="L24" s="14">
+        <f ca="1"/>
+        <v>45455</v>
+      </c>
+      <c r="M24" s="22">
         <f ca="1"/>
         <v>27</v>
       </c>
@@ -2243,29 +2267,29 @@
         <v>Output A|45457</v>
       </c>
       <c r="F25" s="5" t="str" cm="1">
-        <f t="array" aca="1" ref="F25:G25" ca="1">_xlfn.TEXTSPLIT(E25,"|")</f>
+        <f t="array" aca="1" ref="F25:G25" ca="1">_xlfn.LET(_xlpm.z,_xlfn.TEXTSPLIT(E25,"|"),_xlfn.HSTACK(_xlfn.TAKE(_xlpm.z,,1),_xlfn.TAKE(_xlpm.z,,-1)+0))</f>
         <v>Output A</v>
       </c>
-      <c r="G25" s="5" t="str">
+      <c r="G25" s="5">
         <f ca="1"/>
         <v>45457</v>
       </c>
       <c r="H25">
         <v>45455</v>
       </c>
-      <c r="J25" t="str">
+      <c r="J25" s="12" t="str">
         <f ca="1"/>
         <v>Output B</v>
       </c>
-      <c r="K25" t="str">
-        <f ca="1"/>
-        <v>45487</v>
-      </c>
-      <c r="L25">
-        <f ca="1"/>
-        <v>45455</v>
-      </c>
-      <c r="M25">
+      <c r="K25" s="18">
+        <f ca="1"/>
+        <v>45487</v>
+      </c>
+      <c r="L25" s="14">
+        <f ca="1"/>
+        <v>45455</v>
+      </c>
+      <c r="M25" s="22">
         <f ca="1"/>
         <v>51</v>
       </c>
@@ -2281,29 +2305,29 @@
         <v>Output A|45457</v>
       </c>
       <c r="F26" s="5" t="str" cm="1">
-        <f t="array" aca="1" ref="F26:G26" ca="1">_xlfn.TEXTSPLIT(E26,"|")</f>
+        <f t="array" aca="1" ref="F26:G26" ca="1">_xlfn.LET(_xlpm.z,_xlfn.TEXTSPLIT(E26,"|"),_xlfn.HSTACK(_xlfn.TAKE(_xlpm.z,,1),_xlfn.TAKE(_xlpm.z,,-1)+0))</f>
         <v>Output A</v>
       </c>
-      <c r="G26" s="5" t="str">
+      <c r="G26" s="5">
         <f ca="1"/>
         <v>45457</v>
       </c>
       <c r="H26">
         <v>45455</v>
       </c>
-      <c r="J26" t="str">
+      <c r="J26" s="12" t="str">
         <f ca="1"/>
         <v>Output B</v>
       </c>
-      <c r="K26" t="str">
-        <f ca="1"/>
-        <v>45487</v>
-      </c>
-      <c r="L26">
+      <c r="K26" s="18">
+        <f ca="1"/>
+        <v>45487</v>
+      </c>
+      <c r="L26" s="19">
         <f ca="1"/>
         <v>45456</v>
       </c>
-      <c r="M26">
+      <c r="M26" s="22">
         <f ca="1"/>
         <v>7</v>
       </c>
@@ -2320,29 +2344,29 @@
         <v>Output A|45457</v>
       </c>
       <c r="F27" s="5" t="str" cm="1">
-        <f t="array" aca="1" ref="F27:G27" ca="1">_xlfn.TEXTSPLIT(E27,"|")</f>
+        <f t="array" aca="1" ref="F27:G27" ca="1">_xlfn.LET(_xlpm.z,_xlfn.TEXTSPLIT(E27,"|"),_xlfn.HSTACK(_xlfn.TAKE(_xlpm.z,,1),_xlfn.TAKE(_xlpm.z,,-1)+0))</f>
         <v>Output A</v>
       </c>
-      <c r="G27" s="5" t="str">
+      <c r="G27" s="5">
         <f ca="1"/>
         <v>45457</v>
       </c>
       <c r="H27">
         <v>45455</v>
       </c>
-      <c r="J27" t="str">
+      <c r="J27" s="12" t="str">
         <f ca="1"/>
         <v>Output C</v>
       </c>
-      <c r="K27" t="str">
+      <c r="K27" s="18">
         <f ca="1"/>
         <v>45489</v>
       </c>
-      <c r="L27">
+      <c r="L27" s="19">
         <f ca="1"/>
         <v>45456</v>
       </c>
-      <c r="M27">
+      <c r="M27" s="22">
         <f ca="1"/>
         <v>20</v>
       </c>
@@ -2359,29 +2383,29 @@
         <v>Output A|45457</v>
       </c>
       <c r="F28" s="5" t="str" cm="1">
-        <f t="array" aca="1" ref="F28:G28" ca="1">_xlfn.TEXTSPLIT(E28,"|")</f>
+        <f t="array" aca="1" ref="F28:G28" ca="1">_xlfn.LET(_xlpm.z,_xlfn.TEXTSPLIT(E28,"|"),_xlfn.HSTACK(_xlfn.TAKE(_xlpm.z,,1),_xlfn.TAKE(_xlpm.z,,-1)+0))</f>
         <v>Output A</v>
       </c>
-      <c r="G28" s="5" t="str">
+      <c r="G28" s="5">
         <f ca="1"/>
         <v>45457</v>
       </c>
       <c r="H28">
         <v>45455</v>
       </c>
-      <c r="J28" t="str">
+      <c r="J28" s="12" t="str">
         <f ca="1"/>
         <v>Output C</v>
       </c>
-      <c r="K28" t="str">
+      <c r="K28" s="18">
         <f ca="1"/>
         <v>45489</v>
       </c>
-      <c r="L28">
+      <c r="L28" s="19">
         <f ca="1"/>
         <v>45464</v>
       </c>
-      <c r="M28">
+      <c r="M28" s="22">
         <f ca="1"/>
         <v>12</v>
       </c>
@@ -2397,29 +2421,29 @@
         <v>Output A|45457</v>
       </c>
       <c r="F29" s="5" t="str" cm="1">
-        <f t="array" aca="1" ref="F29:G29" ca="1">_xlfn.TEXTSPLIT(E29,"|")</f>
+        <f t="array" aca="1" ref="F29:G29" ca="1">_xlfn.LET(_xlpm.z,_xlfn.TEXTSPLIT(E29,"|"),_xlfn.HSTACK(_xlfn.TAKE(_xlpm.z,,1),_xlfn.TAKE(_xlpm.z,,-1)+0))</f>
         <v>Output A</v>
       </c>
-      <c r="G29" s="5" t="str">
+      <c r="G29" s="5">
         <f ca="1"/>
         <v>45457</v>
       </c>
       <c r="H29">
         <v>45455</v>
       </c>
-      <c r="J29" t="str">
+      <c r="J29" s="12" t="str">
         <f ca="1"/>
         <v>Output D</v>
       </c>
-      <c r="K29" t="str">
-        <f ca="1"/>
-        <v>45520</v>
-      </c>
-      <c r="L29">
+      <c r="K29" s="18">
+        <f ca="1"/>
+        <v>45520</v>
+      </c>
+      <c r="L29" s="19">
         <f ca="1"/>
         <v>45464</v>
       </c>
-      <c r="M29">
+      <c r="M29" s="22">
         <f ca="1"/>
         <v>3</v>
       </c>
@@ -2436,29 +2460,29 @@
         <v>Output A|45457</v>
       </c>
       <c r="F30" s="5" t="str" cm="1">
-        <f t="array" aca="1" ref="F30:G30" ca="1">_xlfn.TEXTSPLIT(E30,"|")</f>
+        <f t="array" aca="1" ref="F30:G30" ca="1">_xlfn.LET(_xlpm.z,_xlfn.TEXTSPLIT(E30,"|"),_xlfn.HSTACK(_xlfn.TAKE(_xlpm.z,,1),_xlfn.TAKE(_xlpm.z,,-1)+0))</f>
         <v>Output A</v>
       </c>
-      <c r="G30" s="5" t="str">
+      <c r="G30" s="5">
         <f ca="1"/>
         <v>45457</v>
       </c>
       <c r="H30">
         <v>45455</v>
       </c>
-      <c r="J30" t="str">
+      <c r="J30" s="12" t="str">
         <f ca="1"/>
         <v>Output D</v>
       </c>
-      <c r="K30" t="str">
-        <f ca="1"/>
-        <v>45520</v>
-      </c>
-      <c r="L30">
-        <f ca="1"/>
-        <v>45486</v>
-      </c>
-      <c r="M30">
+      <c r="K30" s="18">
+        <f ca="1"/>
+        <v>45520</v>
+      </c>
+      <c r="L30" s="19">
+        <f ca="1"/>
+        <v>45486</v>
+      </c>
+      <c r="M30" s="25">
         <f ca="1"/>
         <v>38</v>
       </c>
@@ -2475,29 +2499,29 @@
         <v>Output A|45457</v>
       </c>
       <c r="F31" s="5" t="str" cm="1">
-        <f t="array" aca="1" ref="F31:G31" ca="1">_xlfn.TEXTSPLIT(E31,"|")</f>
+        <f t="array" aca="1" ref="F31:G31" ca="1">_xlfn.LET(_xlpm.z,_xlfn.TEXTSPLIT(E31,"|"),_xlfn.HSTACK(_xlfn.TAKE(_xlpm.z,,1),_xlfn.TAKE(_xlpm.z,,-1)+0))</f>
         <v>Output A</v>
       </c>
-      <c r="G31" s="5" t="str">
+      <c r="G31" s="5">
         <f ca="1"/>
         <v>45457</v>
       </c>
       <c r="H31">
         <v>45455</v>
       </c>
-      <c r="J31" t="str">
+      <c r="J31" s="12" t="str">
         <f ca="1"/>
         <v>Output D</v>
       </c>
-      <c r="K31" t="str">
-        <f ca="1"/>
-        <v>45520</v>
-      </c>
-      <c r="L31">
-        <f ca="1"/>
-        <v>45502</v>
-      </c>
-      <c r="M31">
+      <c r="K31" s="18">
+        <f ca="1"/>
+        <v>45520</v>
+      </c>
+      <c r="L31" s="24">
+        <f ca="1"/>
+        <v>45502</v>
+      </c>
+      <c r="M31" s="25">
         <f ca="1"/>
         <v>1</v>
       </c>
@@ -2513,34 +2537,34 @@
         <v>Output A|45457</v>
       </c>
       <c r="F32" s="5" t="str" cm="1">
-        <f t="array" aca="1" ref="F32:G32" ca="1">_xlfn.TEXTSPLIT(E32,"|")</f>
+        <f t="array" aca="1" ref="F32:G32" ca="1">_xlfn.LET(_xlpm.z,_xlfn.TEXTSPLIT(E32,"|"),_xlfn.HSTACK(_xlfn.TAKE(_xlpm.z,,1),_xlfn.TAKE(_xlpm.z,,-1)+0))</f>
         <v>Output A</v>
       </c>
-      <c r="G32" s="5" t="str">
+      <c r="G32" s="5">
         <f ca="1"/>
         <v>45457</v>
       </c>
       <c r="H32">
         <v>45455</v>
       </c>
-      <c r="J32" t="str">
+      <c r="J32" s="13" t="str">
         <f ca="1"/>
         <v>Output E</v>
       </c>
-      <c r="K32" t="str">
+      <c r="K32" s="20">
         <f ca="1"/>
         <v>45523</v>
       </c>
-      <c r="L32">
-        <f ca="1"/>
-        <v>45502</v>
-      </c>
-      <c r="M32">
+      <c r="L32" s="21">
+        <f ca="1"/>
+        <v>45502</v>
+      </c>
+      <c r="M32" s="23">
         <f ca="1"/>
         <v>23</v>
       </c>
     </row>
-    <row r="33" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B33" s="7"/>
       <c r="C33" s="38">
         <f ca="1"/>
@@ -2551,34 +2575,18 @@
         <v>Output A|45457</v>
       </c>
       <c r="F33" s="5" t="str" cm="1">
-        <f t="array" aca="1" ref="F33:G33" ca="1">_xlfn.TEXTSPLIT(E33,"|")</f>
+        <f t="array" aca="1" ref="F33:G33" ca="1">_xlfn.LET(_xlpm.z,_xlfn.TEXTSPLIT(E33,"|"),_xlfn.HSTACK(_xlfn.TAKE(_xlpm.z,,1),_xlfn.TAKE(_xlpm.z,,-1)+0))</f>
         <v>Output A</v>
       </c>
-      <c r="G33" s="5" t="str">
+      <c r="G33" s="5">
         <f ca="1"/>
         <v>45457</v>
       </c>
       <c r="H33">
         <v>45455</v>
       </c>
-      <c r="J33" t="str">
-        <f ca="1"/>
-        <v>Total</v>
-      </c>
-      <c r="K33" t="str">
-        <f ca="1"/>
-        <v/>
-      </c>
-      <c r="L33" t="str">
-        <f ca="1"/>
-        <v/>
-      </c>
-      <c r="M33">
-        <f ca="1"/>
-        <v>182</v>
-      </c>
-    </row>
-    <row r="34" spans="2:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B34" s="7"/>
       <c r="C34" s="38">
         <f ca="1"/>
@@ -2589,10 +2597,10 @@
         <v>Output A|45457</v>
       </c>
       <c r="F34" s="5" t="str" cm="1">
-        <f t="array" aca="1" ref="F34:G34" ca="1">_xlfn.TEXTSPLIT(E34,"|")</f>
+        <f t="array" aca="1" ref="F34:G34" ca="1">_xlfn.LET(_xlpm.z,_xlfn.TEXTSPLIT(E34,"|"),_xlfn.HSTACK(_xlfn.TAKE(_xlpm.z,,1),_xlfn.TAKE(_xlpm.z,,-1)+0))</f>
         <v>Output A</v>
       </c>
-      <c r="G34" s="5" t="str">
+      <c r="G34" s="5">
         <f ca="1"/>
         <v>45457</v>
       </c>
@@ -2600,7 +2608,7 @@
         <v>45455</v>
       </c>
     </row>
-    <row r="35" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B35" s="7"/>
       <c r="C35" s="38">
         <f ca="1"/>
@@ -2611,10 +2619,10 @@
         <v>Output A|45457</v>
       </c>
       <c r="F35" s="5" t="str" cm="1">
-        <f t="array" aca="1" ref="F35:G35" ca="1">_xlfn.TEXTSPLIT(E35,"|")</f>
+        <f t="array" aca="1" ref="F35:G35" ca="1">_xlfn.LET(_xlpm.z,_xlfn.TEXTSPLIT(E35,"|"),_xlfn.HSTACK(_xlfn.TAKE(_xlpm.z,,1),_xlfn.TAKE(_xlpm.z,,-1)+0))</f>
         <v>Output A</v>
       </c>
-      <c r="G35" s="5" t="str">
+      <c r="G35" s="5">
         <f ca="1"/>
         <v>45457</v>
       </c>
@@ -2622,7 +2630,7 @@
         <v>45455</v>
       </c>
     </row>
-    <row r="36" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B36" s="7"/>
       <c r="C36" s="38">
         <f ca="1"/>
@@ -2633,10 +2641,10 @@
         <v>Output A|45457</v>
       </c>
       <c r="F36" s="5" t="str" cm="1">
-        <f t="array" aca="1" ref="F36:G36" ca="1">_xlfn.TEXTSPLIT(E36,"|")</f>
+        <f t="array" aca="1" ref="F36:G36" ca="1">_xlfn.LET(_xlpm.z,_xlfn.TEXTSPLIT(E36,"|"),_xlfn.HSTACK(_xlfn.TAKE(_xlpm.z,,1),_xlfn.TAKE(_xlpm.z,,-1)+0))</f>
         <v>Output A</v>
       </c>
-      <c r="G36" s="5" t="str">
+      <c r="G36" s="5">
         <f ca="1"/>
         <v>45457</v>
       </c>
@@ -2644,7 +2652,7 @@
         <v>45455</v>
       </c>
     </row>
-    <row r="37" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C37" s="38">
         <f ca="1"/>
         <v>45455</v>
@@ -2654,10 +2662,10 @@
         <v>Output A|45457</v>
       </c>
       <c r="F37" s="5" t="str" cm="1">
-        <f t="array" aca="1" ref="F37:G37" ca="1">_xlfn.TEXTSPLIT(E37,"|")</f>
+        <f t="array" aca="1" ref="F37:G37" ca="1">_xlfn.LET(_xlpm.z,_xlfn.TEXTSPLIT(E37,"|"),_xlfn.HSTACK(_xlfn.TAKE(_xlpm.z,,1),_xlfn.TAKE(_xlpm.z,,-1)+0))</f>
         <v>Output A</v>
       </c>
-      <c r="G37" s="5" t="str">
+      <c r="G37" s="5">
         <f ca="1"/>
         <v>45457</v>
       </c>
@@ -2665,7 +2673,7 @@
         <v>45455</v>
       </c>
     </row>
-    <row r="38" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C38" s="38">
         <f ca="1"/>
         <v>45455</v>
@@ -2675,10 +2683,10 @@
         <v>Output A|45457</v>
       </c>
       <c r="F38" s="5" t="str" cm="1">
-        <f t="array" aca="1" ref="F38:G38" ca="1">_xlfn.TEXTSPLIT(E38,"|")</f>
+        <f t="array" aca="1" ref="F38:G38" ca="1">_xlfn.LET(_xlpm.z,_xlfn.TEXTSPLIT(E38,"|"),_xlfn.HSTACK(_xlfn.TAKE(_xlpm.z,,1),_xlfn.TAKE(_xlpm.z,,-1)+0))</f>
         <v>Output A</v>
       </c>
-      <c r="G38" s="5" t="str">
+      <c r="G38" s="5">
         <f ca="1"/>
         <v>45457</v>
       </c>
@@ -2686,7 +2694,7 @@
         <v>45455</v>
       </c>
     </row>
-    <row r="39" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C39" s="38">
         <f ca="1"/>
         <v>45455</v>
@@ -2696,10 +2704,10 @@
         <v>Output A|45457</v>
       </c>
       <c r="F39" s="5" t="str" cm="1">
-        <f t="array" aca="1" ref="F39:G39" ca="1">_xlfn.TEXTSPLIT(E39,"|")</f>
+        <f t="array" aca="1" ref="F39:G39" ca="1">_xlfn.LET(_xlpm.z,_xlfn.TEXTSPLIT(E39,"|"),_xlfn.HSTACK(_xlfn.TAKE(_xlpm.z,,1),_xlfn.TAKE(_xlpm.z,,-1)+0))</f>
         <v>Output A</v>
       </c>
-      <c r="G39" s="5" t="str">
+      <c r="G39" s="5">
         <f ca="1"/>
         <v>45457</v>
       </c>
@@ -2707,7 +2715,7 @@
         <v>45455</v>
       </c>
     </row>
-    <row r="40" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C40" s="38">
         <f ca="1"/>
         <v>45455</v>
@@ -2717,10 +2725,10 @@
         <v>Output A|45457</v>
       </c>
       <c r="F40" s="5" t="str" cm="1">
-        <f t="array" aca="1" ref="F40:G40" ca="1">_xlfn.TEXTSPLIT(E40,"|")</f>
+        <f t="array" aca="1" ref="F40:G40" ca="1">_xlfn.LET(_xlpm.z,_xlfn.TEXTSPLIT(E40,"|"),_xlfn.HSTACK(_xlfn.TAKE(_xlpm.z,,1),_xlfn.TAKE(_xlpm.z,,-1)+0))</f>
         <v>Output A</v>
       </c>
-      <c r="G40" s="5" t="str">
+      <c r="G40" s="5">
         <f ca="1"/>
         <v>45457</v>
       </c>
@@ -2728,7 +2736,7 @@
         <v>45455</v>
       </c>
     </row>
-    <row r="41" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C41" s="38">
         <f ca="1"/>
         <v>45455</v>
@@ -2738,10 +2746,10 @@
         <v>Output A|45457</v>
       </c>
       <c r="F41" s="5" t="str" cm="1">
-        <f t="array" aca="1" ref="F41:G41" ca="1">_xlfn.TEXTSPLIT(E41,"|")</f>
+        <f t="array" aca="1" ref="F41:G41" ca="1">_xlfn.LET(_xlpm.z,_xlfn.TEXTSPLIT(E41,"|"),_xlfn.HSTACK(_xlfn.TAKE(_xlpm.z,,1),_xlfn.TAKE(_xlpm.z,,-1)+0))</f>
         <v>Output A</v>
       </c>
-      <c r="G41" s="5" t="str">
+      <c r="G41" s="5">
         <f ca="1"/>
         <v>45457</v>
       </c>
@@ -2749,7 +2757,7 @@
         <v>45455</v>
       </c>
     </row>
-    <row r="42" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C42" s="38">
         <f ca="1"/>
         <v>45455</v>
@@ -2759,10 +2767,10 @@
         <v>Output A|45457</v>
       </c>
       <c r="F42" s="5" t="str" cm="1">
-        <f t="array" aca="1" ref="F42:G42" ca="1">_xlfn.TEXTSPLIT(E42,"|")</f>
+        <f t="array" aca="1" ref="F42:G42" ca="1">_xlfn.LET(_xlpm.z,_xlfn.TEXTSPLIT(E42,"|"),_xlfn.HSTACK(_xlfn.TAKE(_xlpm.z,,1),_xlfn.TAKE(_xlpm.z,,-1)+0))</f>
         <v>Output A</v>
       </c>
-      <c r="G42" s="5" t="str">
+      <c r="G42" s="5">
         <f ca="1"/>
         <v>45457</v>
       </c>
@@ -2770,7 +2778,7 @@
         <v>45455</v>
       </c>
     </row>
-    <row r="43" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C43" s="38">
         <f ca="1"/>
         <v>45455</v>
@@ -2780,10 +2788,10 @@
         <v>Output A|45457</v>
       </c>
       <c r="F43" s="5" t="str" cm="1">
-        <f t="array" aca="1" ref="F43:G43" ca="1">_xlfn.TEXTSPLIT(E43,"|")</f>
+        <f t="array" aca="1" ref="F43:G43" ca="1">_xlfn.LET(_xlpm.z,_xlfn.TEXTSPLIT(E43,"|"),_xlfn.HSTACK(_xlfn.TAKE(_xlpm.z,,1),_xlfn.TAKE(_xlpm.z,,-1)+0))</f>
         <v>Output A</v>
       </c>
-      <c r="G43" s="5" t="str">
+      <c r="G43" s="5">
         <f ca="1"/>
         <v>45457</v>
       </c>
@@ -2791,7 +2799,7 @@
         <v>45455</v>
       </c>
     </row>
-    <row r="44" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C44" s="38">
         <f ca="1"/>
         <v>45455</v>
@@ -2801,10 +2809,10 @@
         <v>Output A|45457</v>
       </c>
       <c r="F44" s="5" t="str" cm="1">
-        <f t="array" aca="1" ref="F44:G44" ca="1">_xlfn.TEXTSPLIT(E44,"|")</f>
+        <f t="array" aca="1" ref="F44:G44" ca="1">_xlfn.LET(_xlpm.z,_xlfn.TEXTSPLIT(E44,"|"),_xlfn.HSTACK(_xlfn.TAKE(_xlpm.z,,1),_xlfn.TAKE(_xlpm.z,,-1)+0))</f>
         <v>Output A</v>
       </c>
-      <c r="G44" s="5" t="str">
+      <c r="G44" s="5">
         <f ca="1"/>
         <v>45457</v>
       </c>
@@ -2812,7 +2820,7 @@
         <v>45455</v>
       </c>
     </row>
-    <row r="45" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C45" s="38">
         <f ca="1"/>
         <v>45455</v>
@@ -2822,10 +2830,10 @@
         <v>Output A|45457</v>
       </c>
       <c r="F45" s="5" t="str" cm="1">
-        <f t="array" aca="1" ref="F45:G45" ca="1">_xlfn.TEXTSPLIT(E45,"|")</f>
+        <f t="array" aca="1" ref="F45:G45" ca="1">_xlfn.LET(_xlpm.z,_xlfn.TEXTSPLIT(E45,"|"),_xlfn.HSTACK(_xlfn.TAKE(_xlpm.z,,1),_xlfn.TAKE(_xlpm.z,,-1)+0))</f>
         <v>Output A</v>
       </c>
-      <c r="G45" s="5" t="str">
+      <c r="G45" s="5">
         <f ca="1"/>
         <v>45457</v>
       </c>
@@ -2833,7 +2841,7 @@
         <v>45455</v>
       </c>
     </row>
-    <row r="46" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C46" s="38">
         <f ca="1"/>
         <v>45455</v>
@@ -2843,10 +2851,10 @@
         <v>Output A|45457</v>
       </c>
       <c r="F46" s="5" t="str" cm="1">
-        <f t="array" aca="1" ref="F46:G46" ca="1">_xlfn.TEXTSPLIT(E46,"|")</f>
+        <f t="array" aca="1" ref="F46:G46" ca="1">_xlfn.LET(_xlpm.z,_xlfn.TEXTSPLIT(E46,"|"),_xlfn.HSTACK(_xlfn.TAKE(_xlpm.z,,1),_xlfn.TAKE(_xlpm.z,,-1)+0))</f>
         <v>Output A</v>
       </c>
-      <c r="G46" s="5" t="str">
+      <c r="G46" s="5">
         <f ca="1"/>
         <v>45457</v>
       </c>
@@ -2854,7 +2862,7 @@
         <v>45455</v>
       </c>
     </row>
-    <row r="47" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C47" s="38">
         <f ca="1"/>
         <v>45455</v>
@@ -2864,10 +2872,10 @@
         <v>Output A|45457</v>
       </c>
       <c r="F47" s="5" t="str" cm="1">
-        <f t="array" aca="1" ref="F47:G47" ca="1">_xlfn.TEXTSPLIT(E47,"|")</f>
+        <f t="array" aca="1" ref="F47:G47" ca="1">_xlfn.LET(_xlpm.z,_xlfn.TEXTSPLIT(E47,"|"),_xlfn.HSTACK(_xlfn.TAKE(_xlpm.z,,1),_xlfn.TAKE(_xlpm.z,,-1)+0))</f>
         <v>Output A</v>
       </c>
-      <c r="G47" s="5" t="str">
+      <c r="G47" s="5">
         <f ca="1"/>
         <v>45457</v>
       </c>
@@ -2875,7 +2883,7 @@
         <v>45455</v>
       </c>
     </row>
-    <row r="48" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C48" s="38">
         <f ca="1"/>
         <v>45455</v>
@@ -2885,10 +2893,10 @@
         <v>Output A|45457</v>
       </c>
       <c r="F48" s="5" t="str" cm="1">
-        <f t="array" aca="1" ref="F48:G48" ca="1">_xlfn.TEXTSPLIT(E48,"|")</f>
+        <f t="array" aca="1" ref="F48:G48" ca="1">_xlfn.LET(_xlpm.z,_xlfn.TEXTSPLIT(E48,"|"),_xlfn.HSTACK(_xlfn.TAKE(_xlpm.z,,1),_xlfn.TAKE(_xlpm.z,,-1)+0))</f>
         <v>Output A</v>
       </c>
-      <c r="G48" s="5" t="str">
+      <c r="G48" s="5">
         <f ca="1"/>
         <v>45457</v>
       </c>
@@ -2906,10 +2914,10 @@
         <v>Output A|45457</v>
       </c>
       <c r="F49" s="5" t="str" cm="1">
-        <f t="array" aca="1" ref="F49:G49" ca="1">_xlfn.TEXTSPLIT(E49,"|")</f>
+        <f t="array" aca="1" ref="F49:G49" ca="1">_xlfn.LET(_xlpm.z,_xlfn.TEXTSPLIT(E49,"|"),_xlfn.HSTACK(_xlfn.TAKE(_xlpm.z,,1),_xlfn.TAKE(_xlpm.z,,-1)+0))</f>
         <v>Output A</v>
       </c>
-      <c r="G49" s="5" t="str">
+      <c r="G49" s="5">
         <f ca="1"/>
         <v>45457</v>
       </c>
@@ -2927,10 +2935,10 @@
         <v>Output A|45457</v>
       </c>
       <c r="F50" s="5" t="str" cm="1">
-        <f t="array" aca="1" ref="F50:G50" ca="1">_xlfn.TEXTSPLIT(E50,"|")</f>
+        <f t="array" aca="1" ref="F50:G50" ca="1">_xlfn.LET(_xlpm.z,_xlfn.TEXTSPLIT(E50,"|"),_xlfn.HSTACK(_xlfn.TAKE(_xlpm.z,,1),_xlfn.TAKE(_xlpm.z,,-1)+0))</f>
         <v>Output A</v>
       </c>
-      <c r="G50" s="5" t="str">
+      <c r="G50" s="5">
         <f ca="1"/>
         <v>45457</v>
       </c>
@@ -2948,10 +2956,10 @@
         <v>Output B|45487</v>
       </c>
       <c r="F51" s="5" t="str" cm="1">
-        <f t="array" aca="1" ref="F51:G51" ca="1">_xlfn.TEXTSPLIT(E51,"|")</f>
+        <f t="array" aca="1" ref="F51:G51" ca="1">_xlfn.LET(_xlpm.z,_xlfn.TEXTSPLIT(E51,"|"),_xlfn.HSTACK(_xlfn.TAKE(_xlpm.z,,1),_xlfn.TAKE(_xlpm.z,,-1)+0))</f>
         <v>Output B</v>
       </c>
-      <c r="G51" s="5" t="str">
+      <c r="G51" s="5">
         <f ca="1"/>
         <v>45487</v>
       </c>
@@ -2969,10 +2977,10 @@
         <v>Output B|45487</v>
       </c>
       <c r="F52" s="5" t="str" cm="1">
-        <f t="array" aca="1" ref="F52:G52" ca="1">_xlfn.TEXTSPLIT(E52,"|")</f>
+        <f t="array" aca="1" ref="F52:G52" ca="1">_xlfn.LET(_xlpm.z,_xlfn.TEXTSPLIT(E52,"|"),_xlfn.HSTACK(_xlfn.TAKE(_xlpm.z,,1),_xlfn.TAKE(_xlpm.z,,-1)+0))</f>
         <v>Output B</v>
       </c>
-      <c r="G52" s="5" t="str">
+      <c r="G52" s="5">
         <f ca="1"/>
         <v>45487</v>
       </c>
@@ -2990,10 +2998,10 @@
         <v>Output B|45487</v>
       </c>
       <c r="F53" s="5" t="str" cm="1">
-        <f t="array" aca="1" ref="F53:G53" ca="1">_xlfn.TEXTSPLIT(E53,"|")</f>
+        <f t="array" aca="1" ref="F53:G53" ca="1">_xlfn.LET(_xlpm.z,_xlfn.TEXTSPLIT(E53,"|"),_xlfn.HSTACK(_xlfn.TAKE(_xlpm.z,,1),_xlfn.TAKE(_xlpm.z,,-1)+0))</f>
         <v>Output B</v>
       </c>
-      <c r="G53" s="5" t="str">
+      <c r="G53" s="5">
         <f ca="1"/>
         <v>45487</v>
       </c>
@@ -3011,10 +3019,10 @@
         <v>Output B|45487</v>
       </c>
       <c r="F54" s="5" t="str" cm="1">
-        <f t="array" aca="1" ref="F54:G54" ca="1">_xlfn.TEXTSPLIT(E54,"|")</f>
+        <f t="array" aca="1" ref="F54:G54" ca="1">_xlfn.LET(_xlpm.z,_xlfn.TEXTSPLIT(E54,"|"),_xlfn.HSTACK(_xlfn.TAKE(_xlpm.z,,1),_xlfn.TAKE(_xlpm.z,,-1)+0))</f>
         <v>Output B</v>
       </c>
-      <c r="G54" s="5" t="str">
+      <c r="G54" s="5">
         <f ca="1"/>
         <v>45487</v>
       </c>
@@ -3032,10 +3040,10 @@
         <v>Output B|45487</v>
       </c>
       <c r="F55" s="5" t="str" cm="1">
-        <f t="array" aca="1" ref="F55:G55" ca="1">_xlfn.TEXTSPLIT(E55,"|")</f>
+        <f t="array" aca="1" ref="F55:G55" ca="1">_xlfn.LET(_xlpm.z,_xlfn.TEXTSPLIT(E55,"|"),_xlfn.HSTACK(_xlfn.TAKE(_xlpm.z,,1),_xlfn.TAKE(_xlpm.z,,-1)+0))</f>
         <v>Output B</v>
       </c>
-      <c r="G55" s="5" t="str">
+      <c r="G55" s="5">
         <f ca="1"/>
         <v>45487</v>
       </c>
@@ -3053,10 +3061,10 @@
         <v>Output B|45487</v>
       </c>
       <c r="F56" s="5" t="str" cm="1">
-        <f t="array" aca="1" ref="F56:G56" ca="1">_xlfn.TEXTSPLIT(E56,"|")</f>
+        <f t="array" aca="1" ref="F56:G56" ca="1">_xlfn.LET(_xlpm.z,_xlfn.TEXTSPLIT(E56,"|"),_xlfn.HSTACK(_xlfn.TAKE(_xlpm.z,,1),_xlfn.TAKE(_xlpm.z,,-1)+0))</f>
         <v>Output B</v>
       </c>
-      <c r="G56" s="5" t="str">
+      <c r="G56" s="5">
         <f ca="1"/>
         <v>45487</v>
       </c>
@@ -3074,10 +3082,10 @@
         <v>Output B|45487</v>
       </c>
       <c r="F57" s="5" t="str" cm="1">
-        <f t="array" aca="1" ref="F57:G57" ca="1">_xlfn.TEXTSPLIT(E57,"|")</f>
+        <f t="array" aca="1" ref="F57:G57" ca="1">_xlfn.LET(_xlpm.z,_xlfn.TEXTSPLIT(E57,"|"),_xlfn.HSTACK(_xlfn.TAKE(_xlpm.z,,1),_xlfn.TAKE(_xlpm.z,,-1)+0))</f>
         <v>Output B</v>
       </c>
-      <c r="G57" s="5" t="str">
+      <c r="G57" s="5">
         <f ca="1"/>
         <v>45487</v>
       </c>
@@ -3095,10 +3103,10 @@
         <v>Output B|45487</v>
       </c>
       <c r="F58" s="5" t="str" cm="1">
-        <f t="array" aca="1" ref="F58:G58" ca="1">_xlfn.TEXTSPLIT(E58,"|")</f>
+        <f t="array" aca="1" ref="F58:G58" ca="1">_xlfn.LET(_xlpm.z,_xlfn.TEXTSPLIT(E58,"|"),_xlfn.HSTACK(_xlfn.TAKE(_xlpm.z,,1),_xlfn.TAKE(_xlpm.z,,-1)+0))</f>
         <v>Output B</v>
       </c>
-      <c r="G58" s="5" t="str">
+      <c r="G58" s="5">
         <f ca="1"/>
         <v>45487</v>
       </c>
@@ -3116,10 +3124,10 @@
         <v>Output B|45487</v>
       </c>
       <c r="F59" s="5" t="str" cm="1">
-        <f t="array" aca="1" ref="F59:G59" ca="1">_xlfn.TEXTSPLIT(E59,"|")</f>
+        <f t="array" aca="1" ref="F59:G59" ca="1">_xlfn.LET(_xlpm.z,_xlfn.TEXTSPLIT(E59,"|"),_xlfn.HSTACK(_xlfn.TAKE(_xlpm.z,,1),_xlfn.TAKE(_xlpm.z,,-1)+0))</f>
         <v>Output B</v>
       </c>
-      <c r="G59" s="5" t="str">
+      <c r="G59" s="5">
         <f ca="1"/>
         <v>45487</v>
       </c>
@@ -3137,10 +3145,10 @@
         <v>Output B|45487</v>
       </c>
       <c r="F60" s="5" t="str" cm="1">
-        <f t="array" aca="1" ref="F60:G60" ca="1">_xlfn.TEXTSPLIT(E60,"|")</f>
+        <f t="array" aca="1" ref="F60:G60" ca="1">_xlfn.LET(_xlpm.z,_xlfn.TEXTSPLIT(E60,"|"),_xlfn.HSTACK(_xlfn.TAKE(_xlpm.z,,1),_xlfn.TAKE(_xlpm.z,,-1)+0))</f>
         <v>Output B</v>
       </c>
-      <c r="G60" s="5" t="str">
+      <c r="G60" s="5">
         <f ca="1"/>
         <v>45487</v>
       </c>
@@ -3158,10 +3166,10 @@
         <v>Output B|45487</v>
       </c>
       <c r="F61" s="5" t="str" cm="1">
-        <f t="array" aca="1" ref="F61:G61" ca="1">_xlfn.TEXTSPLIT(E61,"|")</f>
+        <f t="array" aca="1" ref="F61:G61" ca="1">_xlfn.LET(_xlpm.z,_xlfn.TEXTSPLIT(E61,"|"),_xlfn.HSTACK(_xlfn.TAKE(_xlpm.z,,1),_xlfn.TAKE(_xlpm.z,,-1)+0))</f>
         <v>Output B</v>
       </c>
-      <c r="G61" s="5" t="str">
+      <c r="G61" s="5">
         <f ca="1"/>
         <v>45487</v>
       </c>
@@ -3179,10 +3187,10 @@
         <v>Output B|45487</v>
       </c>
       <c r="F62" s="5" t="str" cm="1">
-        <f t="array" aca="1" ref="F62:G62" ca="1">_xlfn.TEXTSPLIT(E62,"|")</f>
+        <f t="array" aca="1" ref="F62:G62" ca="1">_xlfn.LET(_xlpm.z,_xlfn.TEXTSPLIT(E62,"|"),_xlfn.HSTACK(_xlfn.TAKE(_xlpm.z,,1),_xlfn.TAKE(_xlpm.z,,-1)+0))</f>
         <v>Output B</v>
       </c>
-      <c r="G62" s="5" t="str">
+      <c r="G62" s="5">
         <f ca="1"/>
         <v>45487</v>
       </c>
@@ -3200,10 +3208,10 @@
         <v>Output B|45487</v>
       </c>
       <c r="F63" s="5" t="str" cm="1">
-        <f t="array" aca="1" ref="F63:G63" ca="1">_xlfn.TEXTSPLIT(E63,"|")</f>
+        <f t="array" aca="1" ref="F63:G63" ca="1">_xlfn.LET(_xlpm.z,_xlfn.TEXTSPLIT(E63,"|"),_xlfn.HSTACK(_xlfn.TAKE(_xlpm.z,,1),_xlfn.TAKE(_xlpm.z,,-1)+0))</f>
         <v>Output B</v>
       </c>
-      <c r="G63" s="5" t="str">
+      <c r="G63" s="5">
         <f ca="1"/>
         <v>45487</v>
       </c>
@@ -3221,10 +3229,10 @@
         <v>Output B|45487</v>
       </c>
       <c r="F64" s="5" t="str" cm="1">
-        <f t="array" aca="1" ref="F64:G64" ca="1">_xlfn.TEXTSPLIT(E64,"|")</f>
+        <f t="array" aca="1" ref="F64:G64" ca="1">_xlfn.LET(_xlpm.z,_xlfn.TEXTSPLIT(E64,"|"),_xlfn.HSTACK(_xlfn.TAKE(_xlpm.z,,1),_xlfn.TAKE(_xlpm.z,,-1)+0))</f>
         <v>Output B</v>
       </c>
-      <c r="G64" s="5" t="str">
+      <c r="G64" s="5">
         <f ca="1"/>
         <v>45487</v>
       </c>
@@ -3242,10 +3250,10 @@
         <v>Output B|45487</v>
       </c>
       <c r="F65" s="5" t="str" cm="1">
-        <f t="array" aca="1" ref="F65:G65" ca="1">_xlfn.TEXTSPLIT(E65,"|")</f>
+        <f t="array" aca="1" ref="F65:G65" ca="1">_xlfn.LET(_xlpm.z,_xlfn.TEXTSPLIT(E65,"|"),_xlfn.HSTACK(_xlfn.TAKE(_xlpm.z,,1),_xlfn.TAKE(_xlpm.z,,-1)+0))</f>
         <v>Output B</v>
       </c>
-      <c r="G65" s="5" t="str">
+      <c r="G65" s="5">
         <f ca="1"/>
         <v>45487</v>
       </c>
@@ -3263,10 +3271,10 @@
         <v>Output B|45487</v>
       </c>
       <c r="F66" s="5" t="str" cm="1">
-        <f t="array" aca="1" ref="F66:G66" ca="1">_xlfn.TEXTSPLIT(E66,"|")</f>
+        <f t="array" aca="1" ref="F66:G66" ca="1">_xlfn.LET(_xlpm.z,_xlfn.TEXTSPLIT(E66,"|"),_xlfn.HSTACK(_xlfn.TAKE(_xlpm.z,,1),_xlfn.TAKE(_xlpm.z,,-1)+0))</f>
         <v>Output B</v>
       </c>
-      <c r="G66" s="5" t="str">
+      <c r="G66" s="5">
         <f ca="1"/>
         <v>45487</v>
       </c>
@@ -3284,10 +3292,10 @@
         <v>Output B|45487</v>
       </c>
       <c r="F67" s="5" t="str" cm="1">
-        <f t="array" aca="1" ref="F67:G67" ca="1">_xlfn.TEXTSPLIT(E67,"|")</f>
+        <f t="array" aca="1" ref="F67:G67" ca="1">_xlfn.LET(_xlpm.z,_xlfn.TEXTSPLIT(E67,"|"),_xlfn.HSTACK(_xlfn.TAKE(_xlpm.z,,1),_xlfn.TAKE(_xlpm.z,,-1)+0))</f>
         <v>Output B</v>
       </c>
-      <c r="G67" s="5" t="str">
+      <c r="G67" s="5">
         <f ca="1"/>
         <v>45487</v>
       </c>
@@ -3305,10 +3313,10 @@
         <v>Output B|45487</v>
       </c>
       <c r="F68" s="5" t="str" cm="1">
-        <f t="array" aca="1" ref="F68:G68" ca="1">_xlfn.TEXTSPLIT(E68,"|")</f>
+        <f t="array" aca="1" ref="F68:G68" ca="1">_xlfn.LET(_xlpm.z,_xlfn.TEXTSPLIT(E68,"|"),_xlfn.HSTACK(_xlfn.TAKE(_xlpm.z,,1),_xlfn.TAKE(_xlpm.z,,-1)+0))</f>
         <v>Output B</v>
       </c>
-      <c r="G68" s="5" t="str">
+      <c r="G68" s="5">
         <f ca="1"/>
         <v>45487</v>
       </c>
@@ -3326,10 +3334,10 @@
         <v>Output B|45487</v>
       </c>
       <c r="F69" s="5" t="str" cm="1">
-        <f t="array" aca="1" ref="F69:G69" ca="1">_xlfn.TEXTSPLIT(E69,"|")</f>
+        <f t="array" aca="1" ref="F69:G69" ca="1">_xlfn.LET(_xlpm.z,_xlfn.TEXTSPLIT(E69,"|"),_xlfn.HSTACK(_xlfn.TAKE(_xlpm.z,,1),_xlfn.TAKE(_xlpm.z,,-1)+0))</f>
         <v>Output B</v>
       </c>
-      <c r="G69" s="5" t="str">
+      <c r="G69" s="5">
         <f ca="1"/>
         <v>45487</v>
       </c>
@@ -3347,10 +3355,10 @@
         <v>Output B|45487</v>
       </c>
       <c r="F70" s="5" t="str" cm="1">
-        <f t="array" aca="1" ref="F70:G70" ca="1">_xlfn.TEXTSPLIT(E70,"|")</f>
+        <f t="array" aca="1" ref="F70:G70" ca="1">_xlfn.LET(_xlpm.z,_xlfn.TEXTSPLIT(E70,"|"),_xlfn.HSTACK(_xlfn.TAKE(_xlpm.z,,1),_xlfn.TAKE(_xlpm.z,,-1)+0))</f>
         <v>Output B</v>
       </c>
-      <c r="G70" s="5" t="str">
+      <c r="G70" s="5">
         <f ca="1"/>
         <v>45487</v>
       </c>
@@ -3368,10 +3376,10 @@
         <v>Output B|45487</v>
       </c>
       <c r="F71" s="5" t="str" cm="1">
-        <f t="array" aca="1" ref="F71:G71" ca="1">_xlfn.TEXTSPLIT(E71,"|")</f>
+        <f t="array" aca="1" ref="F71:G71" ca="1">_xlfn.LET(_xlpm.z,_xlfn.TEXTSPLIT(E71,"|"),_xlfn.HSTACK(_xlfn.TAKE(_xlpm.z,,1),_xlfn.TAKE(_xlpm.z,,-1)+0))</f>
         <v>Output B</v>
       </c>
-      <c r="G71" s="5" t="str">
+      <c r="G71" s="5">
         <f ca="1"/>
         <v>45487</v>
       </c>
@@ -3389,10 +3397,10 @@
         <v>Output B|45487</v>
       </c>
       <c r="F72" s="5" t="str" cm="1">
-        <f t="array" aca="1" ref="F72:G72" ca="1">_xlfn.TEXTSPLIT(E72,"|")</f>
+        <f t="array" aca="1" ref="F72:G72" ca="1">_xlfn.LET(_xlpm.z,_xlfn.TEXTSPLIT(E72,"|"),_xlfn.HSTACK(_xlfn.TAKE(_xlpm.z,,1),_xlfn.TAKE(_xlpm.z,,-1)+0))</f>
         <v>Output B</v>
       </c>
-      <c r="G72" s="5" t="str">
+      <c r="G72" s="5">
         <f ca="1"/>
         <v>45487</v>
       </c>
@@ -3410,10 +3418,10 @@
         <v>Output B|45487</v>
       </c>
       <c r="F73" s="5" t="str" cm="1">
-        <f t="array" aca="1" ref="F73:G73" ca="1">_xlfn.TEXTSPLIT(E73,"|")</f>
+        <f t="array" aca="1" ref="F73:G73" ca="1">_xlfn.LET(_xlpm.z,_xlfn.TEXTSPLIT(E73,"|"),_xlfn.HSTACK(_xlfn.TAKE(_xlpm.z,,1),_xlfn.TAKE(_xlpm.z,,-1)+0))</f>
         <v>Output B</v>
       </c>
-      <c r="G73" s="5" t="str">
+      <c r="G73" s="5">
         <f ca="1"/>
         <v>45487</v>
       </c>
@@ -3431,10 +3439,10 @@
         <v>Output B|45487</v>
       </c>
       <c r="F74" s="5" t="str" cm="1">
-        <f t="array" aca="1" ref="F74:G74" ca="1">_xlfn.TEXTSPLIT(E74,"|")</f>
+        <f t="array" aca="1" ref="F74:G74" ca="1">_xlfn.LET(_xlpm.z,_xlfn.TEXTSPLIT(E74,"|"),_xlfn.HSTACK(_xlfn.TAKE(_xlpm.z,,1),_xlfn.TAKE(_xlpm.z,,-1)+0))</f>
         <v>Output B</v>
       </c>
-      <c r="G74" s="5" t="str">
+      <c r="G74" s="5">
         <f ca="1"/>
         <v>45487</v>
       </c>
@@ -3452,10 +3460,10 @@
         <v>Output B|45487</v>
       </c>
       <c r="F75" s="5" t="str" cm="1">
-        <f t="array" aca="1" ref="F75:G75" ca="1">_xlfn.TEXTSPLIT(E75,"|")</f>
+        <f t="array" aca="1" ref="F75:G75" ca="1">_xlfn.LET(_xlpm.z,_xlfn.TEXTSPLIT(E75,"|"),_xlfn.HSTACK(_xlfn.TAKE(_xlpm.z,,1),_xlfn.TAKE(_xlpm.z,,-1)+0))</f>
         <v>Output B</v>
       </c>
-      <c r="G75" s="5" t="str">
+      <c r="G75" s="5">
         <f ca="1"/>
         <v>45487</v>
       </c>
@@ -3473,10 +3481,10 @@
         <v>Output B|45487</v>
       </c>
       <c r="F76" s="5" t="str" cm="1">
-        <f t="array" aca="1" ref="F76:G76" ca="1">_xlfn.TEXTSPLIT(E76,"|")</f>
+        <f t="array" aca="1" ref="F76:G76" ca="1">_xlfn.LET(_xlpm.z,_xlfn.TEXTSPLIT(E76,"|"),_xlfn.HSTACK(_xlfn.TAKE(_xlpm.z,,1),_xlfn.TAKE(_xlpm.z,,-1)+0))</f>
         <v>Output B</v>
       </c>
-      <c r="G76" s="5" t="str">
+      <c r="G76" s="5">
         <f ca="1"/>
         <v>45487</v>
       </c>
@@ -3494,10 +3502,10 @@
         <v>Output B|45487</v>
       </c>
       <c r="F77" s="5" t="str" cm="1">
-        <f t="array" aca="1" ref="F77:G77" ca="1">_xlfn.TEXTSPLIT(E77,"|")</f>
+        <f t="array" aca="1" ref="F77:G77" ca="1">_xlfn.LET(_xlpm.z,_xlfn.TEXTSPLIT(E77,"|"),_xlfn.HSTACK(_xlfn.TAKE(_xlpm.z,,1),_xlfn.TAKE(_xlpm.z,,-1)+0))</f>
         <v>Output B</v>
       </c>
-      <c r="G77" s="5" t="str">
+      <c r="G77" s="5">
         <f ca="1"/>
         <v>45487</v>
       </c>
@@ -3515,10 +3523,10 @@
         <v>Output B|45487</v>
       </c>
       <c r="F78" s="5" t="str" cm="1">
-        <f t="array" aca="1" ref="F78:G78" ca="1">_xlfn.TEXTSPLIT(E78,"|")</f>
+        <f t="array" aca="1" ref="F78:G78" ca="1">_xlfn.LET(_xlpm.z,_xlfn.TEXTSPLIT(E78,"|"),_xlfn.HSTACK(_xlfn.TAKE(_xlpm.z,,1),_xlfn.TAKE(_xlpm.z,,-1)+0))</f>
         <v>Output B</v>
       </c>
-      <c r="G78" s="5" t="str">
+      <c r="G78" s="5">
         <f ca="1"/>
         <v>45487</v>
       </c>
@@ -3536,10 +3544,10 @@
         <v>Output B|45487</v>
       </c>
       <c r="F79" s="5" t="str" cm="1">
-        <f t="array" aca="1" ref="F79:G79" ca="1">_xlfn.TEXTSPLIT(E79,"|")</f>
+        <f t="array" aca="1" ref="F79:G79" ca="1">_xlfn.LET(_xlpm.z,_xlfn.TEXTSPLIT(E79,"|"),_xlfn.HSTACK(_xlfn.TAKE(_xlpm.z,,1),_xlfn.TAKE(_xlpm.z,,-1)+0))</f>
         <v>Output B</v>
       </c>
-      <c r="G79" s="5" t="str">
+      <c r="G79" s="5">
         <f ca="1"/>
         <v>45487</v>
       </c>
@@ -3557,10 +3565,10 @@
         <v>Output B|45487</v>
       </c>
       <c r="F80" s="5" t="str" cm="1">
-        <f t="array" aca="1" ref="F80:G80" ca="1">_xlfn.TEXTSPLIT(E80,"|")</f>
+        <f t="array" aca="1" ref="F80:G80" ca="1">_xlfn.LET(_xlpm.z,_xlfn.TEXTSPLIT(E80,"|"),_xlfn.HSTACK(_xlfn.TAKE(_xlpm.z,,1),_xlfn.TAKE(_xlpm.z,,-1)+0))</f>
         <v>Output B</v>
       </c>
-      <c r="G80" s="5" t="str">
+      <c r="G80" s="5">
         <f ca="1"/>
         <v>45487</v>
       </c>
@@ -3578,10 +3586,10 @@
         <v>Output B|45487</v>
       </c>
       <c r="F81" s="5" t="str" cm="1">
-        <f t="array" aca="1" ref="F81:G81" ca="1">_xlfn.TEXTSPLIT(E81,"|")</f>
+        <f t="array" aca="1" ref="F81:G81" ca="1">_xlfn.LET(_xlpm.z,_xlfn.TEXTSPLIT(E81,"|"),_xlfn.HSTACK(_xlfn.TAKE(_xlpm.z,,1),_xlfn.TAKE(_xlpm.z,,-1)+0))</f>
         <v>Output B</v>
       </c>
-      <c r="G81" s="5" t="str">
+      <c r="G81" s="5">
         <f ca="1"/>
         <v>45487</v>
       </c>
@@ -3599,10 +3607,10 @@
         <v>Output B|45487</v>
       </c>
       <c r="F82" s="5" t="str" cm="1">
-        <f t="array" aca="1" ref="F82:G82" ca="1">_xlfn.TEXTSPLIT(E82,"|")</f>
+        <f t="array" aca="1" ref="F82:G82" ca="1">_xlfn.LET(_xlpm.z,_xlfn.TEXTSPLIT(E82,"|"),_xlfn.HSTACK(_xlfn.TAKE(_xlpm.z,,1),_xlfn.TAKE(_xlpm.z,,-1)+0))</f>
         <v>Output B</v>
       </c>
-      <c r="G82" s="5" t="str">
+      <c r="G82" s="5">
         <f ca="1"/>
         <v>45487</v>
       </c>
@@ -3620,10 +3628,10 @@
         <v>Output B|45487</v>
       </c>
       <c r="F83" s="5" t="str" cm="1">
-        <f t="array" aca="1" ref="F83:G83" ca="1">_xlfn.TEXTSPLIT(E83,"|")</f>
+        <f t="array" aca="1" ref="F83:G83" ca="1">_xlfn.LET(_xlpm.z,_xlfn.TEXTSPLIT(E83,"|"),_xlfn.HSTACK(_xlfn.TAKE(_xlpm.z,,1),_xlfn.TAKE(_xlpm.z,,-1)+0))</f>
         <v>Output B</v>
       </c>
-      <c r="G83" s="5" t="str">
+      <c r="G83" s="5">
         <f ca="1"/>
         <v>45487</v>
       </c>
@@ -3641,10 +3649,10 @@
         <v>Output B|45487</v>
       </c>
       <c r="F84" s="5" t="str" cm="1">
-        <f t="array" aca="1" ref="F84:G84" ca="1">_xlfn.TEXTSPLIT(E84,"|")</f>
+        <f t="array" aca="1" ref="F84:G84" ca="1">_xlfn.LET(_xlpm.z,_xlfn.TEXTSPLIT(E84,"|"),_xlfn.HSTACK(_xlfn.TAKE(_xlpm.z,,1),_xlfn.TAKE(_xlpm.z,,-1)+0))</f>
         <v>Output B</v>
       </c>
-      <c r="G84" s="5" t="str">
+      <c r="G84" s="5">
         <f ca="1"/>
         <v>45487</v>
       </c>
@@ -3662,10 +3670,10 @@
         <v>Output B|45487</v>
       </c>
       <c r="F85" s="5" t="str" cm="1">
-        <f t="array" aca="1" ref="F85:G85" ca="1">_xlfn.TEXTSPLIT(E85,"|")</f>
+        <f t="array" aca="1" ref="F85:G85" ca="1">_xlfn.LET(_xlpm.z,_xlfn.TEXTSPLIT(E85,"|"),_xlfn.HSTACK(_xlfn.TAKE(_xlpm.z,,1),_xlfn.TAKE(_xlpm.z,,-1)+0))</f>
         <v>Output B</v>
       </c>
-      <c r="G85" s="5" t="str">
+      <c r="G85" s="5">
         <f ca="1"/>
         <v>45487</v>
       </c>
@@ -3683,10 +3691,10 @@
         <v>Output B|45487</v>
       </c>
       <c r="F86" s="5" t="str" cm="1">
-        <f t="array" aca="1" ref="F86:G86" ca="1">_xlfn.TEXTSPLIT(E86,"|")</f>
+        <f t="array" aca="1" ref="F86:G86" ca="1">_xlfn.LET(_xlpm.z,_xlfn.TEXTSPLIT(E86,"|"),_xlfn.HSTACK(_xlfn.TAKE(_xlpm.z,,1),_xlfn.TAKE(_xlpm.z,,-1)+0))</f>
         <v>Output B</v>
       </c>
-      <c r="G86" s="5" t="str">
+      <c r="G86" s="5">
         <f ca="1"/>
         <v>45487</v>
       </c>
@@ -3704,10 +3712,10 @@
         <v>Output B|45487</v>
       </c>
       <c r="F87" s="5" t="str" cm="1">
-        <f t="array" aca="1" ref="F87:G87" ca="1">_xlfn.TEXTSPLIT(E87,"|")</f>
+        <f t="array" aca="1" ref="F87:G87" ca="1">_xlfn.LET(_xlpm.z,_xlfn.TEXTSPLIT(E87,"|"),_xlfn.HSTACK(_xlfn.TAKE(_xlpm.z,,1),_xlfn.TAKE(_xlpm.z,,-1)+0))</f>
         <v>Output B</v>
       </c>
-      <c r="G87" s="5" t="str">
+      <c r="G87" s="5">
         <f ca="1"/>
         <v>45487</v>
       </c>
@@ -3725,10 +3733,10 @@
         <v>Output B|45487</v>
       </c>
       <c r="F88" s="5" t="str" cm="1">
-        <f t="array" aca="1" ref="F88:G88" ca="1">_xlfn.TEXTSPLIT(E88,"|")</f>
+        <f t="array" aca="1" ref="F88:G88" ca="1">_xlfn.LET(_xlpm.z,_xlfn.TEXTSPLIT(E88,"|"),_xlfn.HSTACK(_xlfn.TAKE(_xlpm.z,,1),_xlfn.TAKE(_xlpm.z,,-1)+0))</f>
         <v>Output B</v>
       </c>
-      <c r="G88" s="5" t="str">
+      <c r="G88" s="5">
         <f ca="1"/>
         <v>45487</v>
       </c>
@@ -3746,10 +3754,10 @@
         <v>Output B|45487</v>
       </c>
       <c r="F89" s="5" t="str" cm="1">
-        <f t="array" aca="1" ref="F89:G89" ca="1">_xlfn.TEXTSPLIT(E89,"|")</f>
+        <f t="array" aca="1" ref="F89:G89" ca="1">_xlfn.LET(_xlpm.z,_xlfn.TEXTSPLIT(E89,"|"),_xlfn.HSTACK(_xlfn.TAKE(_xlpm.z,,1),_xlfn.TAKE(_xlpm.z,,-1)+0))</f>
         <v>Output B</v>
       </c>
-      <c r="G89" s="5" t="str">
+      <c r="G89" s="5">
         <f ca="1"/>
         <v>45487</v>
       </c>
@@ -3767,10 +3775,10 @@
         <v>Output B|45487</v>
       </c>
       <c r="F90" s="5" t="str" cm="1">
-        <f t="array" aca="1" ref="F90:G90" ca="1">_xlfn.TEXTSPLIT(E90,"|")</f>
+        <f t="array" aca="1" ref="F90:G90" ca="1">_xlfn.LET(_xlpm.z,_xlfn.TEXTSPLIT(E90,"|"),_xlfn.HSTACK(_xlfn.TAKE(_xlpm.z,,1),_xlfn.TAKE(_xlpm.z,,-1)+0))</f>
         <v>Output B</v>
       </c>
-      <c r="G90" s="5" t="str">
+      <c r="G90" s="5">
         <f ca="1"/>
         <v>45487</v>
       </c>
@@ -3788,10 +3796,10 @@
         <v>Output B|45487</v>
       </c>
       <c r="F91" s="5" t="str" cm="1">
-        <f t="array" aca="1" ref="F91:G91" ca="1">_xlfn.TEXTSPLIT(E91,"|")</f>
+        <f t="array" aca="1" ref="F91:G91" ca="1">_xlfn.LET(_xlpm.z,_xlfn.TEXTSPLIT(E91,"|"),_xlfn.HSTACK(_xlfn.TAKE(_xlpm.z,,1),_xlfn.TAKE(_xlpm.z,,-1)+0))</f>
         <v>Output B</v>
       </c>
-      <c r="G91" s="5" t="str">
+      <c r="G91" s="5">
         <f ca="1"/>
         <v>45487</v>
       </c>
@@ -3809,10 +3817,10 @@
         <v>Output B|45487</v>
       </c>
       <c r="F92" s="5" t="str" cm="1">
-        <f t="array" aca="1" ref="F92:G92" ca="1">_xlfn.TEXTSPLIT(E92,"|")</f>
+        <f t="array" aca="1" ref="F92:G92" ca="1">_xlfn.LET(_xlpm.z,_xlfn.TEXTSPLIT(E92,"|"),_xlfn.HSTACK(_xlfn.TAKE(_xlpm.z,,1),_xlfn.TAKE(_xlpm.z,,-1)+0))</f>
         <v>Output B</v>
       </c>
-      <c r="G92" s="5" t="str">
+      <c r="G92" s="5">
         <f ca="1"/>
         <v>45487</v>
       </c>
@@ -3830,10 +3838,10 @@
         <v>Output B|45487</v>
       </c>
       <c r="F93" s="5" t="str" cm="1">
-        <f t="array" aca="1" ref="F93:G93" ca="1">_xlfn.TEXTSPLIT(E93,"|")</f>
+        <f t="array" aca="1" ref="F93:G93" ca="1">_xlfn.LET(_xlpm.z,_xlfn.TEXTSPLIT(E93,"|"),_xlfn.HSTACK(_xlfn.TAKE(_xlpm.z,,1),_xlfn.TAKE(_xlpm.z,,-1)+0))</f>
         <v>Output B</v>
       </c>
-      <c r="G93" s="5" t="str">
+      <c r="G93" s="5">
         <f ca="1"/>
         <v>45487</v>
       </c>
@@ -3851,10 +3859,10 @@
         <v>Output B|45487</v>
       </c>
       <c r="F94" s="5" t="str" cm="1">
-        <f t="array" aca="1" ref="F94:G94" ca="1">_xlfn.TEXTSPLIT(E94,"|")</f>
+        <f t="array" aca="1" ref="F94:G94" ca="1">_xlfn.LET(_xlpm.z,_xlfn.TEXTSPLIT(E94,"|"),_xlfn.HSTACK(_xlfn.TAKE(_xlpm.z,,1),_xlfn.TAKE(_xlpm.z,,-1)+0))</f>
         <v>Output B</v>
       </c>
-      <c r="G94" s="5" t="str">
+      <c r="G94" s="5">
         <f ca="1"/>
         <v>45487</v>
       </c>
@@ -3872,10 +3880,10 @@
         <v>Output B|45487</v>
       </c>
       <c r="F95" s="5" t="str" cm="1">
-        <f t="array" aca="1" ref="F95:G95" ca="1">_xlfn.TEXTSPLIT(E95,"|")</f>
+        <f t="array" aca="1" ref="F95:G95" ca="1">_xlfn.LET(_xlpm.z,_xlfn.TEXTSPLIT(E95,"|"),_xlfn.HSTACK(_xlfn.TAKE(_xlpm.z,,1),_xlfn.TAKE(_xlpm.z,,-1)+0))</f>
         <v>Output B</v>
       </c>
-      <c r="G95" s="5" t="str">
+      <c r="G95" s="5">
         <f ca="1"/>
         <v>45487</v>
       </c>
@@ -3893,10 +3901,10 @@
         <v>Output B|45487</v>
       </c>
       <c r="F96" s="5" t="str" cm="1">
-        <f t="array" aca="1" ref="F96:G96" ca="1">_xlfn.TEXTSPLIT(E96,"|")</f>
+        <f t="array" aca="1" ref="F96:G96" ca="1">_xlfn.LET(_xlpm.z,_xlfn.TEXTSPLIT(E96,"|"),_xlfn.HSTACK(_xlfn.TAKE(_xlpm.z,,1),_xlfn.TAKE(_xlpm.z,,-1)+0))</f>
         <v>Output B</v>
       </c>
-      <c r="G96" s="5" t="str">
+      <c r="G96" s="5">
         <f ca="1"/>
         <v>45487</v>
       </c>
@@ -3914,10 +3922,10 @@
         <v>Output B|45487</v>
       </c>
       <c r="F97" s="5" t="str" cm="1">
-        <f t="array" aca="1" ref="F97:G97" ca="1">_xlfn.TEXTSPLIT(E97,"|")</f>
+        <f t="array" aca="1" ref="F97:G97" ca="1">_xlfn.LET(_xlpm.z,_xlfn.TEXTSPLIT(E97,"|"),_xlfn.HSTACK(_xlfn.TAKE(_xlpm.z,,1),_xlfn.TAKE(_xlpm.z,,-1)+0))</f>
         <v>Output B</v>
       </c>
-      <c r="G97" s="5" t="str">
+      <c r="G97" s="5">
         <f ca="1"/>
         <v>45487</v>
       </c>
@@ -3935,10 +3943,10 @@
         <v>Output B|45487</v>
       </c>
       <c r="F98" s="5" t="str" cm="1">
-        <f t="array" aca="1" ref="F98:G98" ca="1">_xlfn.TEXTSPLIT(E98,"|")</f>
+        <f t="array" aca="1" ref="F98:G98" ca="1">_xlfn.LET(_xlpm.z,_xlfn.TEXTSPLIT(E98,"|"),_xlfn.HSTACK(_xlfn.TAKE(_xlpm.z,,1),_xlfn.TAKE(_xlpm.z,,-1)+0))</f>
         <v>Output B</v>
       </c>
-      <c r="G98" s="5" t="str">
+      <c r="G98" s="5">
         <f ca="1"/>
         <v>45487</v>
       </c>
@@ -3956,10 +3964,10 @@
         <v>Output B|45487</v>
       </c>
       <c r="F99" s="5" t="str" cm="1">
-        <f t="array" aca="1" ref="F99:G99" ca="1">_xlfn.TEXTSPLIT(E99,"|")</f>
+        <f t="array" aca="1" ref="F99:G99" ca="1">_xlfn.LET(_xlpm.z,_xlfn.TEXTSPLIT(E99,"|"),_xlfn.HSTACK(_xlfn.TAKE(_xlpm.z,,1),_xlfn.TAKE(_xlpm.z,,-1)+0))</f>
         <v>Output B</v>
       </c>
-      <c r="G99" s="5" t="str">
+      <c r="G99" s="5">
         <f ca="1"/>
         <v>45487</v>
       </c>
@@ -3977,10 +3985,10 @@
         <v>Output B|45487</v>
       </c>
       <c r="F100" s="5" t="str" cm="1">
-        <f t="array" aca="1" ref="F100:G100" ca="1">_xlfn.TEXTSPLIT(E100,"|")</f>
+        <f t="array" aca="1" ref="F100:G100" ca="1">_xlfn.LET(_xlpm.z,_xlfn.TEXTSPLIT(E100,"|"),_xlfn.HSTACK(_xlfn.TAKE(_xlpm.z,,1),_xlfn.TAKE(_xlpm.z,,-1)+0))</f>
         <v>Output B</v>
       </c>
-      <c r="G100" s="5" t="str">
+      <c r="G100" s="5">
         <f ca="1"/>
         <v>45487</v>
       </c>
@@ -3998,10 +4006,10 @@
         <v>Output B|45487</v>
       </c>
       <c r="F101" s="5" t="str" cm="1">
-        <f t="array" aca="1" ref="F101:G101" ca="1">_xlfn.TEXTSPLIT(E101,"|")</f>
+        <f t="array" aca="1" ref="F101:G101" ca="1">_xlfn.LET(_xlpm.z,_xlfn.TEXTSPLIT(E101,"|"),_xlfn.HSTACK(_xlfn.TAKE(_xlpm.z,,1),_xlfn.TAKE(_xlpm.z,,-1)+0))</f>
         <v>Output B</v>
       </c>
-      <c r="G101" s="5" t="str">
+      <c r="G101" s="5">
         <f ca="1"/>
         <v>45487</v>
       </c>
@@ -4019,10 +4027,10 @@
         <v>Output B|45487</v>
       </c>
       <c r="F102" s="5" t="str" cm="1">
-        <f t="array" aca="1" ref="F102:G102" ca="1">_xlfn.TEXTSPLIT(E102,"|")</f>
+        <f t="array" aca="1" ref="F102:G102" ca="1">_xlfn.LET(_xlpm.z,_xlfn.TEXTSPLIT(E102,"|"),_xlfn.HSTACK(_xlfn.TAKE(_xlpm.z,,1),_xlfn.TAKE(_xlpm.z,,-1)+0))</f>
         <v>Output B</v>
       </c>
-      <c r="G102" s="5" t="str">
+      <c r="G102" s="5">
         <f ca="1"/>
         <v>45487</v>
       </c>
@@ -4040,10 +4048,10 @@
         <v>Output B|45487</v>
       </c>
       <c r="F103" s="5" t="str" cm="1">
-        <f t="array" aca="1" ref="F103:G103" ca="1">_xlfn.TEXTSPLIT(E103,"|")</f>
+        <f t="array" aca="1" ref="F103:G103" ca="1">_xlfn.LET(_xlpm.z,_xlfn.TEXTSPLIT(E103,"|"),_xlfn.HSTACK(_xlfn.TAKE(_xlpm.z,,1),_xlfn.TAKE(_xlpm.z,,-1)+0))</f>
         <v>Output B</v>
       </c>
-      <c r="G103" s="5" t="str">
+      <c r="G103" s="5">
         <f ca="1"/>
         <v>45487</v>
       </c>
@@ -4061,10 +4069,10 @@
         <v>Output B|45487</v>
       </c>
       <c r="F104" s="5" t="str" cm="1">
-        <f t="array" aca="1" ref="F104:G104" ca="1">_xlfn.TEXTSPLIT(E104,"|")</f>
+        <f t="array" aca="1" ref="F104:G104" ca="1">_xlfn.LET(_xlpm.z,_xlfn.TEXTSPLIT(E104,"|"),_xlfn.HSTACK(_xlfn.TAKE(_xlpm.z,,1),_xlfn.TAKE(_xlpm.z,,-1)+0))</f>
         <v>Output B</v>
       </c>
-      <c r="G104" s="5" t="str">
+      <c r="G104" s="5">
         <f ca="1"/>
         <v>45487</v>
       </c>
@@ -4082,10 +4090,10 @@
         <v>Output B|45487</v>
       </c>
       <c r="F105" s="5" t="str" cm="1">
-        <f t="array" aca="1" ref="F105:G105" ca="1">_xlfn.TEXTSPLIT(E105,"|")</f>
+        <f t="array" aca="1" ref="F105:G105" ca="1">_xlfn.LET(_xlpm.z,_xlfn.TEXTSPLIT(E105,"|"),_xlfn.HSTACK(_xlfn.TAKE(_xlpm.z,,1),_xlfn.TAKE(_xlpm.z,,-1)+0))</f>
         <v>Output B</v>
       </c>
-      <c r="G105" s="5" t="str">
+      <c r="G105" s="5">
         <f ca="1"/>
         <v>45487</v>
       </c>
@@ -4103,10 +4111,10 @@
         <v>Output B|45487</v>
       </c>
       <c r="F106" s="5" t="str" cm="1">
-        <f t="array" aca="1" ref="F106:G106" ca="1">_xlfn.TEXTSPLIT(E106,"|")</f>
+        <f t="array" aca="1" ref="F106:G106" ca="1">_xlfn.LET(_xlpm.z,_xlfn.TEXTSPLIT(E106,"|"),_xlfn.HSTACK(_xlfn.TAKE(_xlpm.z,,1),_xlfn.TAKE(_xlpm.z,,-1)+0))</f>
         <v>Output B</v>
       </c>
-      <c r="G106" s="5" t="str">
+      <c r="G106" s="5">
         <f ca="1"/>
         <v>45487</v>
       </c>
@@ -4124,10 +4132,10 @@
         <v>Output B|45487</v>
       </c>
       <c r="F107" s="5" t="str" cm="1">
-        <f t="array" aca="1" ref="F107:G107" ca="1">_xlfn.TEXTSPLIT(E107,"|")</f>
+        <f t="array" aca="1" ref="F107:G107" ca="1">_xlfn.LET(_xlpm.z,_xlfn.TEXTSPLIT(E107,"|"),_xlfn.HSTACK(_xlfn.TAKE(_xlpm.z,,1),_xlfn.TAKE(_xlpm.z,,-1)+0))</f>
         <v>Output B</v>
       </c>
-      <c r="G107" s="5" t="str">
+      <c r="G107" s="5">
         <f ca="1"/>
         <v>45487</v>
       </c>
@@ -4145,10 +4153,10 @@
         <v>Output B|45487</v>
       </c>
       <c r="F108" s="5" t="str" cm="1">
-        <f t="array" aca="1" ref="F108:G108" ca="1">_xlfn.TEXTSPLIT(E108,"|")</f>
+        <f t="array" aca="1" ref="F108:G108" ca="1">_xlfn.LET(_xlpm.z,_xlfn.TEXTSPLIT(E108,"|"),_xlfn.HSTACK(_xlfn.TAKE(_xlpm.z,,1),_xlfn.TAKE(_xlpm.z,,-1)+0))</f>
         <v>Output B</v>
       </c>
-      <c r="G108" s="5" t="str">
+      <c r="G108" s="5">
         <f ca="1"/>
         <v>45487</v>
       </c>
@@ -4166,10 +4174,10 @@
         <v>Output C|45489</v>
       </c>
       <c r="F109" s="5" t="str" cm="1">
-        <f t="array" aca="1" ref="F109:G109" ca="1">_xlfn.TEXTSPLIT(E109,"|")</f>
+        <f t="array" aca="1" ref="F109:G109" ca="1">_xlfn.LET(_xlpm.z,_xlfn.TEXTSPLIT(E109,"|"),_xlfn.HSTACK(_xlfn.TAKE(_xlpm.z,,1),_xlfn.TAKE(_xlpm.z,,-1)+0))</f>
         <v>Output C</v>
       </c>
-      <c r="G109" s="5" t="str">
+      <c r="G109" s="5">
         <f ca="1"/>
         <v>45489</v>
       </c>
@@ -4187,10 +4195,10 @@
         <v>Output C|45489</v>
       </c>
       <c r="F110" s="5" t="str" cm="1">
-        <f t="array" aca="1" ref="F110:G110" ca="1">_xlfn.TEXTSPLIT(E110,"|")</f>
+        <f t="array" aca="1" ref="F110:G110" ca="1">_xlfn.LET(_xlpm.z,_xlfn.TEXTSPLIT(E110,"|"),_xlfn.HSTACK(_xlfn.TAKE(_xlpm.z,,1),_xlfn.TAKE(_xlpm.z,,-1)+0))</f>
         <v>Output C</v>
       </c>
-      <c r="G110" s="5" t="str">
+      <c r="G110" s="5">
         <f ca="1"/>
         <v>45489</v>
       </c>
@@ -4208,10 +4216,10 @@
         <v>Output C|45489</v>
       </c>
       <c r="F111" s="5" t="str" cm="1">
-        <f t="array" aca="1" ref="F111:G111" ca="1">_xlfn.TEXTSPLIT(E111,"|")</f>
+        <f t="array" aca="1" ref="F111:G111" ca="1">_xlfn.LET(_xlpm.z,_xlfn.TEXTSPLIT(E111,"|"),_xlfn.HSTACK(_xlfn.TAKE(_xlpm.z,,1),_xlfn.TAKE(_xlpm.z,,-1)+0))</f>
         <v>Output C</v>
       </c>
-      <c r="G111" s="5" t="str">
+      <c r="G111" s="5">
         <f ca="1"/>
         <v>45489</v>
       </c>
@@ -4229,10 +4237,10 @@
         <v>Output C|45489</v>
       </c>
       <c r="F112" s="5" t="str" cm="1">
-        <f t="array" aca="1" ref="F112:G112" ca="1">_xlfn.TEXTSPLIT(E112,"|")</f>
+        <f t="array" aca="1" ref="F112:G112" ca="1">_xlfn.LET(_xlpm.z,_xlfn.TEXTSPLIT(E112,"|"),_xlfn.HSTACK(_xlfn.TAKE(_xlpm.z,,1),_xlfn.TAKE(_xlpm.z,,-1)+0))</f>
         <v>Output C</v>
       </c>
-      <c r="G112" s="5" t="str">
+      <c r="G112" s="5">
         <f ca="1"/>
         <v>45489</v>
       </c>
@@ -4250,10 +4258,10 @@
         <v>Output C|45489</v>
       </c>
       <c r="F113" s="5" t="str" cm="1">
-        <f t="array" aca="1" ref="F113:G113" ca="1">_xlfn.TEXTSPLIT(E113,"|")</f>
+        <f t="array" aca="1" ref="F113:G113" ca="1">_xlfn.LET(_xlpm.z,_xlfn.TEXTSPLIT(E113,"|"),_xlfn.HSTACK(_xlfn.TAKE(_xlpm.z,,1),_xlfn.TAKE(_xlpm.z,,-1)+0))</f>
         <v>Output C</v>
       </c>
-      <c r="G113" s="5" t="str">
+      <c r="G113" s="5">
         <f ca="1"/>
         <v>45489</v>
       </c>
@@ -4271,10 +4279,10 @@
         <v>Output C|45489</v>
       </c>
       <c r="F114" s="5" t="str" cm="1">
-        <f t="array" aca="1" ref="F114:G114" ca="1">_xlfn.TEXTSPLIT(E114,"|")</f>
+        <f t="array" aca="1" ref="F114:G114" ca="1">_xlfn.LET(_xlpm.z,_xlfn.TEXTSPLIT(E114,"|"),_xlfn.HSTACK(_xlfn.TAKE(_xlpm.z,,1),_xlfn.TAKE(_xlpm.z,,-1)+0))</f>
         <v>Output C</v>
       </c>
-      <c r="G114" s="5" t="str">
+      <c r="G114" s="5">
         <f ca="1"/>
         <v>45489</v>
       </c>
@@ -4292,10 +4300,10 @@
         <v>Output C|45489</v>
       </c>
       <c r="F115" s="5" t="str" cm="1">
-        <f t="array" aca="1" ref="F115:G115" ca="1">_xlfn.TEXTSPLIT(E115,"|")</f>
+        <f t="array" aca="1" ref="F115:G115" ca="1">_xlfn.LET(_xlpm.z,_xlfn.TEXTSPLIT(E115,"|"),_xlfn.HSTACK(_xlfn.TAKE(_xlpm.z,,1),_xlfn.TAKE(_xlpm.z,,-1)+0))</f>
         <v>Output C</v>
       </c>
-      <c r="G115" s="5" t="str">
+      <c r="G115" s="5">
         <f ca="1"/>
         <v>45489</v>
       </c>
@@ -4313,10 +4321,10 @@
         <v>Output C|45489</v>
       </c>
       <c r="F116" s="5" t="str" cm="1">
-        <f t="array" aca="1" ref="F116:G116" ca="1">_xlfn.TEXTSPLIT(E116,"|")</f>
+        <f t="array" aca="1" ref="F116:G116" ca="1">_xlfn.LET(_xlpm.z,_xlfn.TEXTSPLIT(E116,"|"),_xlfn.HSTACK(_xlfn.TAKE(_xlpm.z,,1),_xlfn.TAKE(_xlpm.z,,-1)+0))</f>
         <v>Output C</v>
       </c>
-      <c r="G116" s="5" t="str">
+      <c r="G116" s="5">
         <f ca="1"/>
         <v>45489</v>
       </c>
@@ -4334,10 +4342,10 @@
         <v>Output C|45489</v>
       </c>
       <c r="F117" s="5" t="str" cm="1">
-        <f t="array" aca="1" ref="F117:G117" ca="1">_xlfn.TEXTSPLIT(E117,"|")</f>
+        <f t="array" aca="1" ref="F117:G117" ca="1">_xlfn.LET(_xlpm.z,_xlfn.TEXTSPLIT(E117,"|"),_xlfn.HSTACK(_xlfn.TAKE(_xlpm.z,,1),_xlfn.TAKE(_xlpm.z,,-1)+0))</f>
         <v>Output C</v>
       </c>
-      <c r="G117" s="5" t="str">
+      <c r="G117" s="5">
         <f ca="1"/>
         <v>45489</v>
       </c>
@@ -4355,10 +4363,10 @@
         <v>Output C|45489</v>
       </c>
       <c r="F118" s="5" t="str" cm="1">
-        <f t="array" aca="1" ref="F118:G118" ca="1">_xlfn.TEXTSPLIT(E118,"|")</f>
+        <f t="array" aca="1" ref="F118:G118" ca="1">_xlfn.LET(_xlpm.z,_xlfn.TEXTSPLIT(E118,"|"),_xlfn.HSTACK(_xlfn.TAKE(_xlpm.z,,1),_xlfn.TAKE(_xlpm.z,,-1)+0))</f>
         <v>Output C</v>
       </c>
-      <c r="G118" s="5" t="str">
+      <c r="G118" s="5">
         <f ca="1"/>
         <v>45489</v>
       </c>
@@ -4376,10 +4384,10 @@
         <v>Output C|45489</v>
       </c>
       <c r="F119" s="5" t="str" cm="1">
-        <f t="array" aca="1" ref="F119:G119" ca="1">_xlfn.TEXTSPLIT(E119,"|")</f>
+        <f t="array" aca="1" ref="F119:G119" ca="1">_xlfn.LET(_xlpm.z,_xlfn.TEXTSPLIT(E119,"|"),_xlfn.HSTACK(_xlfn.TAKE(_xlpm.z,,1),_xlfn.TAKE(_xlpm.z,,-1)+0))</f>
         <v>Output C</v>
       </c>
-      <c r="G119" s="5" t="str">
+      <c r="G119" s="5">
         <f ca="1"/>
         <v>45489</v>
       </c>
@@ -4397,10 +4405,10 @@
         <v>Output C|45489</v>
       </c>
       <c r="F120" s="5" t="str" cm="1">
-        <f t="array" aca="1" ref="F120:G120" ca="1">_xlfn.TEXTSPLIT(E120,"|")</f>
+        <f t="array" aca="1" ref="F120:G120" ca="1">_xlfn.LET(_xlpm.z,_xlfn.TEXTSPLIT(E120,"|"),_xlfn.HSTACK(_xlfn.TAKE(_xlpm.z,,1),_xlfn.TAKE(_xlpm.z,,-1)+0))</f>
         <v>Output C</v>
       </c>
-      <c r="G120" s="5" t="str">
+      <c r="G120" s="5">
         <f ca="1"/>
         <v>45489</v>
       </c>
@@ -4418,10 +4426,10 @@
         <v>Output C|45489</v>
       </c>
       <c r="F121" s="5" t="str" cm="1">
-        <f t="array" aca="1" ref="F121:G121" ca="1">_xlfn.TEXTSPLIT(E121,"|")</f>
+        <f t="array" aca="1" ref="F121:G121" ca="1">_xlfn.LET(_xlpm.z,_xlfn.TEXTSPLIT(E121,"|"),_xlfn.HSTACK(_xlfn.TAKE(_xlpm.z,,1),_xlfn.TAKE(_xlpm.z,,-1)+0))</f>
         <v>Output C</v>
       </c>
-      <c r="G121" s="5" t="str">
+      <c r="G121" s="5">
         <f ca="1"/>
         <v>45489</v>
       </c>
@@ -4439,10 +4447,10 @@
         <v>Output C|45489</v>
       </c>
       <c r="F122" s="5" t="str" cm="1">
-        <f t="array" aca="1" ref="F122:G122" ca="1">_xlfn.TEXTSPLIT(E122,"|")</f>
+        <f t="array" aca="1" ref="F122:G122" ca="1">_xlfn.LET(_xlpm.z,_xlfn.TEXTSPLIT(E122,"|"),_xlfn.HSTACK(_xlfn.TAKE(_xlpm.z,,1),_xlfn.TAKE(_xlpm.z,,-1)+0))</f>
         <v>Output C</v>
       </c>
-      <c r="G122" s="5" t="str">
+      <c r="G122" s="5">
         <f ca="1"/>
         <v>45489</v>
       </c>
@@ -4460,10 +4468,10 @@
         <v>Output C|45489</v>
       </c>
       <c r="F123" s="5" t="str" cm="1">
-        <f t="array" aca="1" ref="F123:G123" ca="1">_xlfn.TEXTSPLIT(E123,"|")</f>
+        <f t="array" aca="1" ref="F123:G123" ca="1">_xlfn.LET(_xlpm.z,_xlfn.TEXTSPLIT(E123,"|"),_xlfn.HSTACK(_xlfn.TAKE(_xlpm.z,,1),_xlfn.TAKE(_xlpm.z,,-1)+0))</f>
         <v>Output C</v>
       </c>
-      <c r="G123" s="5" t="str">
+      <c r="G123" s="5">
         <f ca="1"/>
         <v>45489</v>
       </c>
@@ -4481,10 +4489,10 @@
         <v>Output C|45489</v>
       </c>
       <c r="F124" s="5" t="str" cm="1">
-        <f t="array" aca="1" ref="F124:G124" ca="1">_xlfn.TEXTSPLIT(E124,"|")</f>
+        <f t="array" aca="1" ref="F124:G124" ca="1">_xlfn.LET(_xlpm.z,_xlfn.TEXTSPLIT(E124,"|"),_xlfn.HSTACK(_xlfn.TAKE(_xlpm.z,,1),_xlfn.TAKE(_xlpm.z,,-1)+0))</f>
         <v>Output C</v>
       </c>
-      <c r="G124" s="5" t="str">
+      <c r="G124" s="5">
         <f ca="1"/>
         <v>45489</v>
       </c>
@@ -4502,10 +4510,10 @@
         <v>Output C|45489</v>
       </c>
       <c r="F125" s="5" t="str" cm="1">
-        <f t="array" aca="1" ref="F125:G125" ca="1">_xlfn.TEXTSPLIT(E125,"|")</f>
+        <f t="array" aca="1" ref="F125:G125" ca="1">_xlfn.LET(_xlpm.z,_xlfn.TEXTSPLIT(E125,"|"),_xlfn.HSTACK(_xlfn.TAKE(_xlpm.z,,1),_xlfn.TAKE(_xlpm.z,,-1)+0))</f>
         <v>Output C</v>
       </c>
-      <c r="G125" s="5" t="str">
+      <c r="G125" s="5">
         <f ca="1"/>
         <v>45489</v>
       </c>
@@ -4523,10 +4531,10 @@
         <v>Output C|45489</v>
       </c>
       <c r="F126" s="5" t="str" cm="1">
-        <f t="array" aca="1" ref="F126:G126" ca="1">_xlfn.TEXTSPLIT(E126,"|")</f>
+        <f t="array" aca="1" ref="F126:G126" ca="1">_xlfn.LET(_xlpm.z,_xlfn.TEXTSPLIT(E126,"|"),_xlfn.HSTACK(_xlfn.TAKE(_xlpm.z,,1),_xlfn.TAKE(_xlpm.z,,-1)+0))</f>
         <v>Output C</v>
       </c>
-      <c r="G126" s="5" t="str">
+      <c r="G126" s="5">
         <f ca="1"/>
         <v>45489</v>
       </c>
@@ -4544,10 +4552,10 @@
         <v>Output C|45489</v>
       </c>
       <c r="F127" s="5" t="str" cm="1">
-        <f t="array" aca="1" ref="F127:G127" ca="1">_xlfn.TEXTSPLIT(E127,"|")</f>
+        <f t="array" aca="1" ref="F127:G127" ca="1">_xlfn.LET(_xlpm.z,_xlfn.TEXTSPLIT(E127,"|"),_xlfn.HSTACK(_xlfn.TAKE(_xlpm.z,,1),_xlfn.TAKE(_xlpm.z,,-1)+0))</f>
         <v>Output C</v>
       </c>
-      <c r="G127" s="5" t="str">
+      <c r="G127" s="5">
         <f ca="1"/>
         <v>45489</v>
       </c>
@@ -4565,10 +4573,10 @@
         <v>Output C|45489</v>
       </c>
       <c r="F128" s="5" t="str" cm="1">
-        <f t="array" aca="1" ref="F128:G128" ca="1">_xlfn.TEXTSPLIT(E128,"|")</f>
+        <f t="array" aca="1" ref="F128:G128" ca="1">_xlfn.LET(_xlpm.z,_xlfn.TEXTSPLIT(E128,"|"),_xlfn.HSTACK(_xlfn.TAKE(_xlpm.z,,1),_xlfn.TAKE(_xlpm.z,,-1)+0))</f>
         <v>Output C</v>
       </c>
-      <c r="G128" s="5" t="str">
+      <c r="G128" s="5">
         <f ca="1"/>
         <v>45489</v>
       </c>
@@ -4586,10 +4594,10 @@
         <v>Output C|45489</v>
       </c>
       <c r="F129" s="5" t="str" cm="1">
-        <f t="array" aca="1" ref="F129:G129" ca="1">_xlfn.TEXTSPLIT(E129,"|")</f>
+        <f t="array" aca="1" ref="F129:G129" ca="1">_xlfn.LET(_xlpm.z,_xlfn.TEXTSPLIT(E129,"|"),_xlfn.HSTACK(_xlfn.TAKE(_xlpm.z,,1),_xlfn.TAKE(_xlpm.z,,-1)+0))</f>
         <v>Output C</v>
       </c>
-      <c r="G129" s="5" t="str">
+      <c r="G129" s="5">
         <f ca="1"/>
         <v>45489</v>
       </c>
@@ -4607,10 +4615,10 @@
         <v>Output C|45489</v>
       </c>
       <c r="F130" s="5" t="str" cm="1">
-        <f t="array" aca="1" ref="F130:G130" ca="1">_xlfn.TEXTSPLIT(E130,"|")</f>
+        <f t="array" aca="1" ref="F130:G130" ca="1">_xlfn.LET(_xlpm.z,_xlfn.TEXTSPLIT(E130,"|"),_xlfn.HSTACK(_xlfn.TAKE(_xlpm.z,,1),_xlfn.TAKE(_xlpm.z,,-1)+0))</f>
         <v>Output C</v>
       </c>
-      <c r="G130" s="5" t="str">
+      <c r="G130" s="5">
         <f ca="1"/>
         <v>45489</v>
       </c>
@@ -4628,10 +4636,10 @@
         <v>Output C|45489</v>
       </c>
       <c r="F131" s="5" t="str" cm="1">
-        <f t="array" aca="1" ref="F131:G131" ca="1">_xlfn.TEXTSPLIT(E131,"|")</f>
+        <f t="array" aca="1" ref="F131:G131" ca="1">_xlfn.LET(_xlpm.z,_xlfn.TEXTSPLIT(E131,"|"),_xlfn.HSTACK(_xlfn.TAKE(_xlpm.z,,1),_xlfn.TAKE(_xlpm.z,,-1)+0))</f>
         <v>Output C</v>
       </c>
-      <c r="G131" s="5" t="str">
+      <c r="G131" s="5">
         <f ca="1"/>
         <v>45489</v>
       </c>
@@ -4649,10 +4657,10 @@
         <v>Output C|45489</v>
       </c>
       <c r="F132" s="5" t="str" cm="1">
-        <f t="array" aca="1" ref="F132:G132" ca="1">_xlfn.TEXTSPLIT(E132,"|")</f>
+        <f t="array" aca="1" ref="F132:G132" ca="1">_xlfn.LET(_xlpm.z,_xlfn.TEXTSPLIT(E132,"|"),_xlfn.HSTACK(_xlfn.TAKE(_xlpm.z,,1),_xlfn.TAKE(_xlpm.z,,-1)+0))</f>
         <v>Output C</v>
       </c>
-      <c r="G132" s="5" t="str">
+      <c r="G132" s="5">
         <f ca="1"/>
         <v>45489</v>
       </c>
@@ -4670,10 +4678,10 @@
         <v>Output C|45489</v>
       </c>
       <c r="F133" s="5" t="str" cm="1">
-        <f t="array" aca="1" ref="F133:G133" ca="1">_xlfn.TEXTSPLIT(E133,"|")</f>
+        <f t="array" aca="1" ref="F133:G133" ca="1">_xlfn.LET(_xlpm.z,_xlfn.TEXTSPLIT(E133,"|"),_xlfn.HSTACK(_xlfn.TAKE(_xlpm.z,,1),_xlfn.TAKE(_xlpm.z,,-1)+0))</f>
         <v>Output C</v>
       </c>
-      <c r="G133" s="5" t="str">
+      <c r="G133" s="5">
         <f ca="1"/>
         <v>45489</v>
       </c>
@@ -4691,10 +4699,10 @@
         <v>Output C|45489</v>
       </c>
       <c r="F134" s="5" t="str" cm="1">
-        <f t="array" aca="1" ref="F134:G134" ca="1">_xlfn.TEXTSPLIT(E134,"|")</f>
+        <f t="array" aca="1" ref="F134:G134" ca="1">_xlfn.LET(_xlpm.z,_xlfn.TEXTSPLIT(E134,"|"),_xlfn.HSTACK(_xlfn.TAKE(_xlpm.z,,1),_xlfn.TAKE(_xlpm.z,,-1)+0))</f>
         <v>Output C</v>
       </c>
-      <c r="G134" s="5" t="str">
+      <c r="G134" s="5">
         <f ca="1"/>
         <v>45489</v>
       </c>
@@ -4712,10 +4720,10 @@
         <v>Output C|45489</v>
       </c>
       <c r="F135" s="5" t="str" cm="1">
-        <f t="array" aca="1" ref="F135:G135" ca="1">_xlfn.TEXTSPLIT(E135,"|")</f>
+        <f t="array" aca="1" ref="F135:G135" ca="1">_xlfn.LET(_xlpm.z,_xlfn.TEXTSPLIT(E135,"|"),_xlfn.HSTACK(_xlfn.TAKE(_xlpm.z,,1),_xlfn.TAKE(_xlpm.z,,-1)+0))</f>
         <v>Output C</v>
       </c>
-      <c r="G135" s="5" t="str">
+      <c r="G135" s="5">
         <f ca="1"/>
         <v>45489</v>
       </c>
@@ -4733,10 +4741,10 @@
         <v>Output C|45489</v>
       </c>
       <c r="F136" s="5" t="str" cm="1">
-        <f t="array" aca="1" ref="F136:G136" ca="1">_xlfn.TEXTSPLIT(E136,"|")</f>
+        <f t="array" aca="1" ref="F136:G136" ca="1">_xlfn.LET(_xlpm.z,_xlfn.TEXTSPLIT(E136,"|"),_xlfn.HSTACK(_xlfn.TAKE(_xlpm.z,,1),_xlfn.TAKE(_xlpm.z,,-1)+0))</f>
         <v>Output C</v>
       </c>
-      <c r="G136" s="5" t="str">
+      <c r="G136" s="5">
         <f ca="1"/>
         <v>45489</v>
       </c>
@@ -4754,10 +4762,10 @@
         <v>Output C|45489</v>
       </c>
       <c r="F137" s="5" t="str" cm="1">
-        <f t="array" aca="1" ref="F137:G137" ca="1">_xlfn.TEXTSPLIT(E137,"|")</f>
+        <f t="array" aca="1" ref="F137:G137" ca="1">_xlfn.LET(_xlpm.z,_xlfn.TEXTSPLIT(E137,"|"),_xlfn.HSTACK(_xlfn.TAKE(_xlpm.z,,1),_xlfn.TAKE(_xlpm.z,,-1)+0))</f>
         <v>Output C</v>
       </c>
-      <c r="G137" s="5" t="str">
+      <c r="G137" s="5">
         <f ca="1"/>
         <v>45489</v>
       </c>
@@ -4775,10 +4783,10 @@
         <v>Output C|45489</v>
       </c>
       <c r="F138" s="5" t="str" cm="1">
-        <f t="array" aca="1" ref="F138:G138" ca="1">_xlfn.TEXTSPLIT(E138,"|")</f>
+        <f t="array" aca="1" ref="F138:G138" ca="1">_xlfn.LET(_xlpm.z,_xlfn.TEXTSPLIT(E138,"|"),_xlfn.HSTACK(_xlfn.TAKE(_xlpm.z,,1),_xlfn.TAKE(_xlpm.z,,-1)+0))</f>
         <v>Output C</v>
       </c>
-      <c r="G138" s="5" t="str">
+      <c r="G138" s="5">
         <f ca="1"/>
         <v>45489</v>
       </c>
@@ -4796,10 +4804,10 @@
         <v>Output C|45489</v>
       </c>
       <c r="F139" s="5" t="str" cm="1">
-        <f t="array" aca="1" ref="F139:G139" ca="1">_xlfn.TEXTSPLIT(E139,"|")</f>
+        <f t="array" aca="1" ref="F139:G139" ca="1">_xlfn.LET(_xlpm.z,_xlfn.TEXTSPLIT(E139,"|"),_xlfn.HSTACK(_xlfn.TAKE(_xlpm.z,,1),_xlfn.TAKE(_xlpm.z,,-1)+0))</f>
         <v>Output C</v>
       </c>
-      <c r="G139" s="5" t="str">
+      <c r="G139" s="5">
         <f ca="1"/>
         <v>45489</v>
       </c>
@@ -4817,10 +4825,10 @@
         <v>Output C|45489</v>
       </c>
       <c r="F140" s="5" t="str" cm="1">
-        <f t="array" aca="1" ref="F140:G140" ca="1">_xlfn.TEXTSPLIT(E140,"|")</f>
+        <f t="array" aca="1" ref="F140:G140" ca="1">_xlfn.LET(_xlpm.z,_xlfn.TEXTSPLIT(E140,"|"),_xlfn.HSTACK(_xlfn.TAKE(_xlpm.z,,1),_xlfn.TAKE(_xlpm.z,,-1)+0))</f>
         <v>Output C</v>
       </c>
-      <c r="G140" s="5" t="str">
+      <c r="G140" s="5">
         <f ca="1"/>
         <v>45489</v>
       </c>
@@ -4838,10 +4846,10 @@
         <v>Output D|45520</v>
       </c>
       <c r="F141" s="5" t="str" cm="1">
-        <f t="array" aca="1" ref="F141:G141" ca="1">_xlfn.TEXTSPLIT(E141,"|")</f>
+        <f t="array" aca="1" ref="F141:G141" ca="1">_xlfn.LET(_xlpm.z,_xlfn.TEXTSPLIT(E141,"|"),_xlfn.HSTACK(_xlfn.TAKE(_xlpm.z,,1),_xlfn.TAKE(_xlpm.z,,-1)+0))</f>
         <v>Output D</v>
       </c>
-      <c r="G141" s="5" t="str">
+      <c r="G141" s="5">
         <f ca="1"/>
         <v>45520</v>
       </c>
@@ -4859,10 +4867,10 @@
         <v>Output D|45520</v>
       </c>
       <c r="F142" s="5" t="str" cm="1">
-        <f t="array" aca="1" ref="F142:G142" ca="1">_xlfn.TEXTSPLIT(E142,"|")</f>
+        <f t="array" aca="1" ref="F142:G142" ca="1">_xlfn.LET(_xlpm.z,_xlfn.TEXTSPLIT(E142,"|"),_xlfn.HSTACK(_xlfn.TAKE(_xlpm.z,,1),_xlfn.TAKE(_xlpm.z,,-1)+0))</f>
         <v>Output D</v>
       </c>
-      <c r="G142" s="5" t="str">
+      <c r="G142" s="5">
         <f ca="1"/>
         <v>45520</v>
       </c>
@@ -4880,10 +4888,10 @@
         <v>Output D|45520</v>
       </c>
       <c r="F143" s="5" t="str" cm="1">
-        <f t="array" aca="1" ref="F143:G143" ca="1">_xlfn.TEXTSPLIT(E143,"|")</f>
+        <f t="array" aca="1" ref="F143:G143" ca="1">_xlfn.LET(_xlpm.z,_xlfn.TEXTSPLIT(E143,"|"),_xlfn.HSTACK(_xlfn.TAKE(_xlpm.z,,1),_xlfn.TAKE(_xlpm.z,,-1)+0))</f>
         <v>Output D</v>
       </c>
-      <c r="G143" s="5" t="str">
+      <c r="G143" s="5">
         <f ca="1"/>
         <v>45520</v>
       </c>
@@ -4901,10 +4909,10 @@
         <v>Output D|45520</v>
       </c>
       <c r="F144" s="5" t="str" cm="1">
-        <f t="array" aca="1" ref="F144:G144" ca="1">_xlfn.TEXTSPLIT(E144,"|")</f>
+        <f t="array" aca="1" ref="F144:G144" ca="1">_xlfn.LET(_xlpm.z,_xlfn.TEXTSPLIT(E144,"|"),_xlfn.HSTACK(_xlfn.TAKE(_xlpm.z,,1),_xlfn.TAKE(_xlpm.z,,-1)+0))</f>
         <v>Output D</v>
       </c>
-      <c r="G144" s="5" t="str">
+      <c r="G144" s="5">
         <f ca="1"/>
         <v>45520</v>
       </c>
@@ -4922,10 +4930,10 @@
         <v>Output D|45520</v>
       </c>
       <c r="F145" s="5" t="str" cm="1">
-        <f t="array" aca="1" ref="F145:G145" ca="1">_xlfn.TEXTSPLIT(E145,"|")</f>
+        <f t="array" aca="1" ref="F145:G145" ca="1">_xlfn.LET(_xlpm.z,_xlfn.TEXTSPLIT(E145,"|"),_xlfn.HSTACK(_xlfn.TAKE(_xlpm.z,,1),_xlfn.TAKE(_xlpm.z,,-1)+0))</f>
         <v>Output D</v>
       </c>
-      <c r="G145" s="5" t="str">
+      <c r="G145" s="5">
         <f ca="1"/>
         <v>45520</v>
       </c>
@@ -4943,10 +4951,10 @@
         <v>Output D|45520</v>
       </c>
       <c r="F146" s="5" t="str" cm="1">
-        <f t="array" aca="1" ref="F146:G146" ca="1">_xlfn.TEXTSPLIT(E146,"|")</f>
+        <f t="array" aca="1" ref="F146:G146" ca="1">_xlfn.LET(_xlpm.z,_xlfn.TEXTSPLIT(E146,"|"),_xlfn.HSTACK(_xlfn.TAKE(_xlpm.z,,1),_xlfn.TAKE(_xlpm.z,,-1)+0))</f>
         <v>Output D</v>
       </c>
-      <c r="G146" s="5" t="str">
+      <c r="G146" s="5">
         <f ca="1"/>
         <v>45520</v>
       </c>
@@ -4964,10 +4972,10 @@
         <v>Output D|45520</v>
       </c>
       <c r="F147" s="5" t="str" cm="1">
-        <f t="array" aca="1" ref="F147:G147" ca="1">_xlfn.TEXTSPLIT(E147,"|")</f>
+        <f t="array" aca="1" ref="F147:G147" ca="1">_xlfn.LET(_xlpm.z,_xlfn.TEXTSPLIT(E147,"|"),_xlfn.HSTACK(_xlfn.TAKE(_xlpm.z,,1),_xlfn.TAKE(_xlpm.z,,-1)+0))</f>
         <v>Output D</v>
       </c>
-      <c r="G147" s="5" t="str">
+      <c r="G147" s="5">
         <f ca="1"/>
         <v>45520</v>
       </c>
@@ -4985,10 +4993,10 @@
         <v>Output D|45520</v>
       </c>
       <c r="F148" s="5" t="str" cm="1">
-        <f t="array" aca="1" ref="F148:G148" ca="1">_xlfn.TEXTSPLIT(E148,"|")</f>
+        <f t="array" aca="1" ref="F148:G148" ca="1">_xlfn.LET(_xlpm.z,_xlfn.TEXTSPLIT(E148,"|"),_xlfn.HSTACK(_xlfn.TAKE(_xlpm.z,,1),_xlfn.TAKE(_xlpm.z,,-1)+0))</f>
         <v>Output D</v>
       </c>
-      <c r="G148" s="5" t="str">
+      <c r="G148" s="5">
         <f ca="1"/>
         <v>45520</v>
       </c>
@@ -5006,10 +5014,10 @@
         <v>Output D|45520</v>
       </c>
       <c r="F149" s="5" t="str" cm="1">
-        <f t="array" aca="1" ref="F149:G149" ca="1">_xlfn.TEXTSPLIT(E149,"|")</f>
+        <f t="array" aca="1" ref="F149:G149" ca="1">_xlfn.LET(_xlpm.z,_xlfn.TEXTSPLIT(E149,"|"),_xlfn.HSTACK(_xlfn.TAKE(_xlpm.z,,1),_xlfn.TAKE(_xlpm.z,,-1)+0))</f>
         <v>Output D</v>
       </c>
-      <c r="G149" s="5" t="str">
+      <c r="G149" s="5">
         <f ca="1"/>
         <v>45520</v>
       </c>
@@ -5027,10 +5035,10 @@
         <v>Output D|45520</v>
       </c>
       <c r="F150" s="5" t="str" cm="1">
-        <f t="array" aca="1" ref="F150:G150" ca="1">_xlfn.TEXTSPLIT(E150,"|")</f>
+        <f t="array" aca="1" ref="F150:G150" ca="1">_xlfn.LET(_xlpm.z,_xlfn.TEXTSPLIT(E150,"|"),_xlfn.HSTACK(_xlfn.TAKE(_xlpm.z,,1),_xlfn.TAKE(_xlpm.z,,-1)+0))</f>
         <v>Output D</v>
       </c>
-      <c r="G150" s="5" t="str">
+      <c r="G150" s="5">
         <f ca="1"/>
         <v>45520</v>
       </c>
@@ -5048,10 +5056,10 @@
         <v>Output D|45520</v>
       </c>
       <c r="F151" s="5" t="str" cm="1">
-        <f t="array" aca="1" ref="F151:G151" ca="1">_xlfn.TEXTSPLIT(E151,"|")</f>
+        <f t="array" aca="1" ref="F151:G151" ca="1">_xlfn.LET(_xlpm.z,_xlfn.TEXTSPLIT(E151,"|"),_xlfn.HSTACK(_xlfn.TAKE(_xlpm.z,,1),_xlfn.TAKE(_xlpm.z,,-1)+0))</f>
         <v>Output D</v>
       </c>
-      <c r="G151" s="5" t="str">
+      <c r="G151" s="5">
         <f ca="1"/>
         <v>45520</v>
       </c>
@@ -5069,10 +5077,10 @@
         <v>Output D|45520</v>
       </c>
       <c r="F152" s="5" t="str" cm="1">
-        <f t="array" aca="1" ref="F152:G152" ca="1">_xlfn.TEXTSPLIT(E152,"|")</f>
+        <f t="array" aca="1" ref="F152:G152" ca="1">_xlfn.LET(_xlpm.z,_xlfn.TEXTSPLIT(E152,"|"),_xlfn.HSTACK(_xlfn.TAKE(_xlpm.z,,1),_xlfn.TAKE(_xlpm.z,,-1)+0))</f>
         <v>Output D</v>
       </c>
-      <c r="G152" s="5" t="str">
+      <c r="G152" s="5">
         <f ca="1"/>
         <v>45520</v>
       </c>
@@ -5090,10 +5098,10 @@
         <v>Output D|45520</v>
       </c>
       <c r="F153" s="5" t="str" cm="1">
-        <f t="array" aca="1" ref="F153:G153" ca="1">_xlfn.TEXTSPLIT(E153,"|")</f>
+        <f t="array" aca="1" ref="F153:G153" ca="1">_xlfn.LET(_xlpm.z,_xlfn.TEXTSPLIT(E153,"|"),_xlfn.HSTACK(_xlfn.TAKE(_xlpm.z,,1),_xlfn.TAKE(_xlpm.z,,-1)+0))</f>
         <v>Output D</v>
       </c>
-      <c r="G153" s="5" t="str">
+      <c r="G153" s="5">
         <f ca="1"/>
         <v>45520</v>
       </c>
@@ -5111,10 +5119,10 @@
         <v>Output D|45520</v>
       </c>
       <c r="F154" s="5" t="str" cm="1">
-        <f t="array" aca="1" ref="F154:G154" ca="1">_xlfn.TEXTSPLIT(E154,"|")</f>
+        <f t="array" aca="1" ref="F154:G154" ca="1">_xlfn.LET(_xlpm.z,_xlfn.TEXTSPLIT(E154,"|"),_xlfn.HSTACK(_xlfn.TAKE(_xlpm.z,,1),_xlfn.TAKE(_xlpm.z,,-1)+0))</f>
         <v>Output D</v>
       </c>
-      <c r="G154" s="5" t="str">
+      <c r="G154" s="5">
         <f ca="1"/>
         <v>45520</v>
       </c>
@@ -5132,10 +5140,10 @@
         <v>Output D|45520</v>
       </c>
       <c r="F155" s="5" t="str" cm="1">
-        <f t="array" aca="1" ref="F155:G155" ca="1">_xlfn.TEXTSPLIT(E155,"|")</f>
+        <f t="array" aca="1" ref="F155:G155" ca="1">_xlfn.LET(_xlpm.z,_xlfn.TEXTSPLIT(E155,"|"),_xlfn.HSTACK(_xlfn.TAKE(_xlpm.z,,1),_xlfn.TAKE(_xlpm.z,,-1)+0))</f>
         <v>Output D</v>
       </c>
-      <c r="G155" s="5" t="str">
+      <c r="G155" s="5">
         <f ca="1"/>
         <v>45520</v>
       </c>
@@ -5153,10 +5161,10 @@
         <v>Output D|45520</v>
       </c>
       <c r="F156" s="5" t="str" cm="1">
-        <f t="array" aca="1" ref="F156:G156" ca="1">_xlfn.TEXTSPLIT(E156,"|")</f>
+        <f t="array" aca="1" ref="F156:G156" ca="1">_xlfn.LET(_xlpm.z,_xlfn.TEXTSPLIT(E156,"|"),_xlfn.HSTACK(_xlfn.TAKE(_xlpm.z,,1),_xlfn.TAKE(_xlpm.z,,-1)+0))</f>
         <v>Output D</v>
       </c>
-      <c r="G156" s="5" t="str">
+      <c r="G156" s="5">
         <f ca="1"/>
         <v>45520</v>
       </c>
@@ -5174,10 +5182,10 @@
         <v>Output D|45520</v>
       </c>
       <c r="F157" s="5" t="str" cm="1">
-        <f t="array" aca="1" ref="F157:G157" ca="1">_xlfn.TEXTSPLIT(E157,"|")</f>
+        <f t="array" aca="1" ref="F157:G157" ca="1">_xlfn.LET(_xlpm.z,_xlfn.TEXTSPLIT(E157,"|"),_xlfn.HSTACK(_xlfn.TAKE(_xlpm.z,,1),_xlfn.TAKE(_xlpm.z,,-1)+0))</f>
         <v>Output D</v>
       </c>
-      <c r="G157" s="5" t="str">
+      <c r="G157" s="5">
         <f ca="1"/>
         <v>45520</v>
       </c>
@@ -5195,10 +5203,10 @@
         <v>Output D|45520</v>
       </c>
       <c r="F158" s="5" t="str" cm="1">
-        <f t="array" aca="1" ref="F158:G158" ca="1">_xlfn.TEXTSPLIT(E158,"|")</f>
+        <f t="array" aca="1" ref="F158:G158" ca="1">_xlfn.LET(_xlpm.z,_xlfn.TEXTSPLIT(E158,"|"),_xlfn.HSTACK(_xlfn.TAKE(_xlpm.z,,1),_xlfn.TAKE(_xlpm.z,,-1)+0))</f>
         <v>Output D</v>
       </c>
-      <c r="G158" s="5" t="str">
+      <c r="G158" s="5">
         <f ca="1"/>
         <v>45520</v>
       </c>
@@ -5216,10 +5224,10 @@
         <v>Output D|45520</v>
       </c>
       <c r="F159" s="5" t="str" cm="1">
-        <f t="array" aca="1" ref="F159:G159" ca="1">_xlfn.TEXTSPLIT(E159,"|")</f>
+        <f t="array" aca="1" ref="F159:G159" ca="1">_xlfn.LET(_xlpm.z,_xlfn.TEXTSPLIT(E159,"|"),_xlfn.HSTACK(_xlfn.TAKE(_xlpm.z,,1),_xlfn.TAKE(_xlpm.z,,-1)+0))</f>
         <v>Output D</v>
       </c>
-      <c r="G159" s="5" t="str">
+      <c r="G159" s="5">
         <f ca="1"/>
         <v>45520</v>
       </c>
@@ -5237,10 +5245,10 @@
         <v>Output D|45520</v>
       </c>
       <c r="F160" s="5" t="str" cm="1">
-        <f t="array" aca="1" ref="F160:G160" ca="1">_xlfn.TEXTSPLIT(E160,"|")</f>
+        <f t="array" aca="1" ref="F160:G160" ca="1">_xlfn.LET(_xlpm.z,_xlfn.TEXTSPLIT(E160,"|"),_xlfn.HSTACK(_xlfn.TAKE(_xlpm.z,,1),_xlfn.TAKE(_xlpm.z,,-1)+0))</f>
         <v>Output D</v>
       </c>
-      <c r="G160" s="5" t="str">
+      <c r="G160" s="5">
         <f ca="1"/>
         <v>45520</v>
       </c>
@@ -5258,10 +5266,10 @@
         <v>Output D|45520</v>
       </c>
       <c r="F161" s="5" t="str" cm="1">
-        <f t="array" aca="1" ref="F161:G161" ca="1">_xlfn.TEXTSPLIT(E161,"|")</f>
+        <f t="array" aca="1" ref="F161:G161" ca="1">_xlfn.LET(_xlpm.z,_xlfn.TEXTSPLIT(E161,"|"),_xlfn.HSTACK(_xlfn.TAKE(_xlpm.z,,1),_xlfn.TAKE(_xlpm.z,,-1)+0))</f>
         <v>Output D</v>
       </c>
-      <c r="G161" s="5" t="str">
+      <c r="G161" s="5">
         <f ca="1"/>
         <v>45520</v>
       </c>
@@ -5279,10 +5287,10 @@
         <v>Output D|45520</v>
       </c>
       <c r="F162" s="5" t="str" cm="1">
-        <f t="array" aca="1" ref="F162:G162" ca="1">_xlfn.TEXTSPLIT(E162,"|")</f>
+        <f t="array" aca="1" ref="F162:G162" ca="1">_xlfn.LET(_xlpm.z,_xlfn.TEXTSPLIT(E162,"|"),_xlfn.HSTACK(_xlfn.TAKE(_xlpm.z,,1),_xlfn.TAKE(_xlpm.z,,-1)+0))</f>
         <v>Output D</v>
       </c>
-      <c r="G162" s="5" t="str">
+      <c r="G162" s="5">
         <f ca="1"/>
         <v>45520</v>
       </c>
@@ -5300,10 +5308,10 @@
         <v>Output D|45520</v>
       </c>
       <c r="F163" s="5" t="str" cm="1">
-        <f t="array" aca="1" ref="F163:G163" ca="1">_xlfn.TEXTSPLIT(E163,"|")</f>
+        <f t="array" aca="1" ref="F163:G163" ca="1">_xlfn.LET(_xlpm.z,_xlfn.TEXTSPLIT(E163,"|"),_xlfn.HSTACK(_xlfn.TAKE(_xlpm.z,,1),_xlfn.TAKE(_xlpm.z,,-1)+0))</f>
         <v>Output D</v>
       </c>
-      <c r="G163" s="5" t="str">
+      <c r="G163" s="5">
         <f ca="1"/>
         <v>45520</v>
       </c>
@@ -5321,10 +5329,10 @@
         <v>Output D|45520</v>
       </c>
       <c r="F164" s="5" t="str" cm="1">
-        <f t="array" aca="1" ref="F164:G164" ca="1">_xlfn.TEXTSPLIT(E164,"|")</f>
+        <f t="array" aca="1" ref="F164:G164" ca="1">_xlfn.LET(_xlpm.z,_xlfn.TEXTSPLIT(E164,"|"),_xlfn.HSTACK(_xlfn.TAKE(_xlpm.z,,1),_xlfn.TAKE(_xlpm.z,,-1)+0))</f>
         <v>Output D</v>
       </c>
-      <c r="G164" s="5" t="str">
+      <c r="G164" s="5">
         <f ca="1"/>
         <v>45520</v>
       </c>
@@ -5342,10 +5350,10 @@
         <v>Output D|45520</v>
       </c>
       <c r="F165" s="5" t="str" cm="1">
-        <f t="array" aca="1" ref="F165:G165" ca="1">_xlfn.TEXTSPLIT(E165,"|")</f>
+        <f t="array" aca="1" ref="F165:G165" ca="1">_xlfn.LET(_xlpm.z,_xlfn.TEXTSPLIT(E165,"|"),_xlfn.HSTACK(_xlfn.TAKE(_xlpm.z,,1),_xlfn.TAKE(_xlpm.z,,-1)+0))</f>
         <v>Output D</v>
       </c>
-      <c r="G165" s="5" t="str">
+      <c r="G165" s="5">
         <f ca="1"/>
         <v>45520</v>
       </c>
@@ -5363,10 +5371,10 @@
         <v>Output D|45520</v>
       </c>
       <c r="F166" s="5" t="str" cm="1">
-        <f t="array" aca="1" ref="F166:G166" ca="1">_xlfn.TEXTSPLIT(E166,"|")</f>
+        <f t="array" aca="1" ref="F166:G166" ca="1">_xlfn.LET(_xlpm.z,_xlfn.TEXTSPLIT(E166,"|"),_xlfn.HSTACK(_xlfn.TAKE(_xlpm.z,,1),_xlfn.TAKE(_xlpm.z,,-1)+0))</f>
         <v>Output D</v>
       </c>
-      <c r="G166" s="5" t="str">
+      <c r="G166" s="5">
         <f ca="1"/>
         <v>45520</v>
       </c>
@@ -5384,10 +5392,10 @@
         <v>Output D|45520</v>
       </c>
       <c r="F167" s="5" t="str" cm="1">
-        <f t="array" aca="1" ref="F167:G167" ca="1">_xlfn.TEXTSPLIT(E167,"|")</f>
+        <f t="array" aca="1" ref="F167:G167" ca="1">_xlfn.LET(_xlpm.z,_xlfn.TEXTSPLIT(E167,"|"),_xlfn.HSTACK(_xlfn.TAKE(_xlpm.z,,1),_xlfn.TAKE(_xlpm.z,,-1)+0))</f>
         <v>Output D</v>
       </c>
-      <c r="G167" s="5" t="str">
+      <c r="G167" s="5">
         <f ca="1"/>
         <v>45520</v>
       </c>
@@ -5405,10 +5413,10 @@
         <v>Output D|45520</v>
       </c>
       <c r="F168" s="5" t="str" cm="1">
-        <f t="array" aca="1" ref="F168:G168" ca="1">_xlfn.TEXTSPLIT(E168,"|")</f>
+        <f t="array" aca="1" ref="F168:G168" ca="1">_xlfn.LET(_xlpm.z,_xlfn.TEXTSPLIT(E168,"|"),_xlfn.HSTACK(_xlfn.TAKE(_xlpm.z,,1),_xlfn.TAKE(_xlpm.z,,-1)+0))</f>
         <v>Output D</v>
       </c>
-      <c r="G168" s="5" t="str">
+      <c r="G168" s="5">
         <f ca="1"/>
         <v>45520</v>
       </c>
@@ -5426,10 +5434,10 @@
         <v>Output D|45520</v>
       </c>
       <c r="F169" s="5" t="str" cm="1">
-        <f t="array" aca="1" ref="F169:G169" ca="1">_xlfn.TEXTSPLIT(E169,"|")</f>
+        <f t="array" aca="1" ref="F169:G169" ca="1">_xlfn.LET(_xlpm.z,_xlfn.TEXTSPLIT(E169,"|"),_xlfn.HSTACK(_xlfn.TAKE(_xlpm.z,,1),_xlfn.TAKE(_xlpm.z,,-1)+0))</f>
         <v>Output D</v>
       </c>
-      <c r="G169" s="5" t="str">
+      <c r="G169" s="5">
         <f ca="1"/>
         <v>45520</v>
       </c>
@@ -5447,10 +5455,10 @@
         <v>Output D|45520</v>
       </c>
       <c r="F170" s="5" t="str" cm="1">
-        <f t="array" aca="1" ref="F170:G170" ca="1">_xlfn.TEXTSPLIT(E170,"|")</f>
+        <f t="array" aca="1" ref="F170:G170" ca="1">_xlfn.LET(_xlpm.z,_xlfn.TEXTSPLIT(E170,"|"),_xlfn.HSTACK(_xlfn.TAKE(_xlpm.z,,1),_xlfn.TAKE(_xlpm.z,,-1)+0))</f>
         <v>Output D</v>
       </c>
-      <c r="G170" s="5" t="str">
+      <c r="G170" s="5">
         <f ca="1"/>
         <v>45520</v>
       </c>
@@ -5468,10 +5476,10 @@
         <v>Output D|45520</v>
       </c>
       <c r="F171" s="5" t="str" cm="1">
-        <f t="array" aca="1" ref="F171:G171" ca="1">_xlfn.TEXTSPLIT(E171,"|")</f>
+        <f t="array" aca="1" ref="F171:G171" ca="1">_xlfn.LET(_xlpm.z,_xlfn.TEXTSPLIT(E171,"|"),_xlfn.HSTACK(_xlfn.TAKE(_xlpm.z,,1),_xlfn.TAKE(_xlpm.z,,-1)+0))</f>
         <v>Output D</v>
       </c>
-      <c r="G171" s="5" t="str">
+      <c r="G171" s="5">
         <f ca="1"/>
         <v>45520</v>
       </c>
@@ -5489,10 +5497,10 @@
         <v>Output D|45520</v>
       </c>
       <c r="F172" s="5" t="str" cm="1">
-        <f t="array" aca="1" ref="F172:G172" ca="1">_xlfn.TEXTSPLIT(E172,"|")</f>
+        <f t="array" aca="1" ref="F172:G172" ca="1">_xlfn.LET(_xlpm.z,_xlfn.TEXTSPLIT(E172,"|"),_xlfn.HSTACK(_xlfn.TAKE(_xlpm.z,,1),_xlfn.TAKE(_xlpm.z,,-1)+0))</f>
         <v>Output D</v>
       </c>
-      <c r="G172" s="5" t="str">
+      <c r="G172" s="5">
         <f ca="1"/>
         <v>45520</v>
       </c>
@@ -5510,10 +5518,10 @@
         <v>Output D|45520</v>
       </c>
       <c r="F173" s="5" t="str" cm="1">
-        <f t="array" aca="1" ref="F173:G173" ca="1">_xlfn.TEXTSPLIT(E173,"|")</f>
+        <f t="array" aca="1" ref="F173:G173" ca="1">_xlfn.LET(_xlpm.z,_xlfn.TEXTSPLIT(E173,"|"),_xlfn.HSTACK(_xlfn.TAKE(_xlpm.z,,1),_xlfn.TAKE(_xlpm.z,,-1)+0))</f>
         <v>Output D</v>
       </c>
-      <c r="G173" s="5" t="str">
+      <c r="G173" s="5">
         <f ca="1"/>
         <v>45520</v>
       </c>
@@ -5531,10 +5539,10 @@
         <v>Output D|45520</v>
       </c>
       <c r="F174" s="5" t="str" cm="1">
-        <f t="array" aca="1" ref="F174:G174" ca="1">_xlfn.TEXTSPLIT(E174,"|")</f>
+        <f t="array" aca="1" ref="F174:G174" ca="1">_xlfn.LET(_xlpm.z,_xlfn.TEXTSPLIT(E174,"|"),_xlfn.HSTACK(_xlfn.TAKE(_xlpm.z,,1),_xlfn.TAKE(_xlpm.z,,-1)+0))</f>
         <v>Output D</v>
       </c>
-      <c r="G174" s="5" t="str">
+      <c r="G174" s="5">
         <f ca="1"/>
         <v>45520</v>
       </c>
@@ -5552,10 +5560,10 @@
         <v>Output D|45520</v>
       </c>
       <c r="F175" s="5" t="str" cm="1">
-        <f t="array" aca="1" ref="F175:G175" ca="1">_xlfn.TEXTSPLIT(E175,"|")</f>
+        <f t="array" aca="1" ref="F175:G175" ca="1">_xlfn.LET(_xlpm.z,_xlfn.TEXTSPLIT(E175,"|"),_xlfn.HSTACK(_xlfn.TAKE(_xlpm.z,,1),_xlfn.TAKE(_xlpm.z,,-1)+0))</f>
         <v>Output D</v>
       </c>
-      <c r="G175" s="5" t="str">
+      <c r="G175" s="5">
         <f ca="1"/>
         <v>45520</v>
       </c>
@@ -5573,10 +5581,10 @@
         <v>Output D|45520</v>
       </c>
       <c r="F176" s="5" t="str" cm="1">
-        <f t="array" aca="1" ref="F176:G176" ca="1">_xlfn.TEXTSPLIT(E176,"|")</f>
+        <f t="array" aca="1" ref="F176:G176" ca="1">_xlfn.LET(_xlpm.z,_xlfn.TEXTSPLIT(E176,"|"),_xlfn.HSTACK(_xlfn.TAKE(_xlpm.z,,1),_xlfn.TAKE(_xlpm.z,,-1)+0))</f>
         <v>Output D</v>
       </c>
-      <c r="G176" s="5" t="str">
+      <c r="G176" s="5">
         <f ca="1"/>
         <v>45520</v>
       </c>
@@ -5594,10 +5602,10 @@
         <v>Output D|45520</v>
       </c>
       <c r="F177" s="5" t="str" cm="1">
-        <f t="array" aca="1" ref="F177:G177" ca="1">_xlfn.TEXTSPLIT(E177,"|")</f>
+        <f t="array" aca="1" ref="F177:G177" ca="1">_xlfn.LET(_xlpm.z,_xlfn.TEXTSPLIT(E177,"|"),_xlfn.HSTACK(_xlfn.TAKE(_xlpm.z,,1),_xlfn.TAKE(_xlpm.z,,-1)+0))</f>
         <v>Output D</v>
       </c>
-      <c r="G177" s="5" t="str">
+      <c r="G177" s="5">
         <f ca="1"/>
         <v>45520</v>
       </c>
@@ -5615,10 +5623,10 @@
         <v>Output D|45520</v>
       </c>
       <c r="F178" s="5" t="str" cm="1">
-        <f t="array" aca="1" ref="F178:G178" ca="1">_xlfn.TEXTSPLIT(E178,"|")</f>
+        <f t="array" aca="1" ref="F178:G178" ca="1">_xlfn.LET(_xlpm.z,_xlfn.TEXTSPLIT(E178,"|"),_xlfn.HSTACK(_xlfn.TAKE(_xlpm.z,,1),_xlfn.TAKE(_xlpm.z,,-1)+0))</f>
         <v>Output D</v>
       </c>
-      <c r="G178" s="5" t="str">
+      <c r="G178" s="5">
         <f ca="1"/>
         <v>45520</v>
       </c>
@@ -5636,10 +5644,10 @@
         <v>Output D|45520</v>
       </c>
       <c r="F179" s="5" t="str" cm="1">
-        <f t="array" aca="1" ref="F179:G179" ca="1">_xlfn.TEXTSPLIT(E179,"|")</f>
+        <f t="array" aca="1" ref="F179:G179" ca="1">_xlfn.LET(_xlpm.z,_xlfn.TEXTSPLIT(E179,"|"),_xlfn.HSTACK(_xlfn.TAKE(_xlpm.z,,1),_xlfn.TAKE(_xlpm.z,,-1)+0))</f>
         <v>Output D</v>
       </c>
-      <c r="G179" s="5" t="str">
+      <c r="G179" s="5">
         <f ca="1"/>
         <v>45520</v>
       </c>
@@ -5657,10 +5665,10 @@
         <v>Output D|45520</v>
       </c>
       <c r="F180" s="5" t="str" cm="1">
-        <f t="array" aca="1" ref="F180:G180" ca="1">_xlfn.TEXTSPLIT(E180,"|")</f>
+        <f t="array" aca="1" ref="F180:G180" ca="1">_xlfn.LET(_xlpm.z,_xlfn.TEXTSPLIT(E180,"|"),_xlfn.HSTACK(_xlfn.TAKE(_xlpm.z,,1),_xlfn.TAKE(_xlpm.z,,-1)+0))</f>
         <v>Output D</v>
       </c>
-      <c r="G180" s="5" t="str">
+      <c r="G180" s="5">
         <f ca="1"/>
         <v>45520</v>
       </c>
@@ -5678,10 +5686,10 @@
         <v>Output D|45520</v>
       </c>
       <c r="F181" s="5" t="str" cm="1">
-        <f t="array" aca="1" ref="F181:G181" ca="1">_xlfn.TEXTSPLIT(E181,"|")</f>
+        <f t="array" aca="1" ref="F181:G181" ca="1">_xlfn.LET(_xlpm.z,_xlfn.TEXTSPLIT(E181,"|"),_xlfn.HSTACK(_xlfn.TAKE(_xlpm.z,,1),_xlfn.TAKE(_xlpm.z,,-1)+0))</f>
         <v>Output D</v>
       </c>
-      <c r="G181" s="5" t="str">
+      <c r="G181" s="5">
         <f ca="1"/>
         <v>45520</v>
       </c>
@@ -5699,10 +5707,10 @@
         <v>Output D|45520</v>
       </c>
       <c r="F182" s="5" t="str" cm="1">
-        <f t="array" aca="1" ref="F182:G182" ca="1">_xlfn.TEXTSPLIT(E182,"|")</f>
+        <f t="array" aca="1" ref="F182:G182" ca="1">_xlfn.LET(_xlpm.z,_xlfn.TEXTSPLIT(E182,"|"),_xlfn.HSTACK(_xlfn.TAKE(_xlpm.z,,1),_xlfn.TAKE(_xlpm.z,,-1)+0))</f>
         <v>Output D</v>
       </c>
-      <c r="G182" s="5" t="str">
+      <c r="G182" s="5">
         <f ca="1"/>
         <v>45520</v>
       </c>
@@ -5720,10 +5728,10 @@
         <v>Output E|45523</v>
       </c>
       <c r="F183" s="5" t="str" cm="1">
-        <f t="array" aca="1" ref="F183:G183" ca="1">_xlfn.TEXTSPLIT(E183,"|")</f>
+        <f t="array" aca="1" ref="F183:G183" ca="1">_xlfn.LET(_xlpm.z,_xlfn.TEXTSPLIT(E183,"|"),_xlfn.HSTACK(_xlfn.TAKE(_xlpm.z,,1),_xlfn.TAKE(_xlpm.z,,-1)+0))</f>
         <v>Output E</v>
       </c>
-      <c r="G183" s="5" t="str">
+      <c r="G183" s="5">
         <f ca="1"/>
         <v>45523</v>
       </c>
@@ -5741,10 +5749,10 @@
         <v>Output E|45523</v>
       </c>
       <c r="F184" s="5" t="str" cm="1">
-        <f t="array" aca="1" ref="F184:G184" ca="1">_xlfn.TEXTSPLIT(E184,"|")</f>
+        <f t="array" aca="1" ref="F184:G184" ca="1">_xlfn.LET(_xlpm.z,_xlfn.TEXTSPLIT(E184,"|"),_xlfn.HSTACK(_xlfn.TAKE(_xlpm.z,,1),_xlfn.TAKE(_xlpm.z,,-1)+0))</f>
         <v>Output E</v>
       </c>
-      <c r="G184" s="5" t="str">
+      <c r="G184" s="5">
         <f ca="1"/>
         <v>45523</v>
       </c>
@@ -5762,10 +5770,10 @@
         <v>Output E|45523</v>
       </c>
       <c r="F185" s="5" t="str" cm="1">
-        <f t="array" aca="1" ref="F185:G185" ca="1">_xlfn.TEXTSPLIT(E185,"|")</f>
+        <f t="array" aca="1" ref="F185:G185" ca="1">_xlfn.LET(_xlpm.z,_xlfn.TEXTSPLIT(E185,"|"),_xlfn.HSTACK(_xlfn.TAKE(_xlpm.z,,1),_xlfn.TAKE(_xlpm.z,,-1)+0))</f>
         <v>Output E</v>
       </c>
-      <c r="G185" s="5" t="str">
+      <c r="G185" s="5">
         <f ca="1"/>
         <v>45523</v>
       </c>
@@ -5783,10 +5791,10 @@
         <v>Output E|45523</v>
       </c>
       <c r="F186" s="5" t="str" cm="1">
-        <f t="array" aca="1" ref="F186:G186" ca="1">_xlfn.TEXTSPLIT(E186,"|")</f>
+        <f t="array" aca="1" ref="F186:G186" ca="1">_xlfn.LET(_xlpm.z,_xlfn.TEXTSPLIT(E186,"|"),_xlfn.HSTACK(_xlfn.TAKE(_xlpm.z,,1),_xlfn.TAKE(_xlpm.z,,-1)+0))</f>
         <v>Output E</v>
       </c>
-      <c r="G186" s="5" t="str">
+      <c r="G186" s="5">
         <f ca="1"/>
         <v>45523</v>
       </c>
@@ -5804,10 +5812,10 @@
         <v>Output E|45523</v>
       </c>
       <c r="F187" s="5" t="str" cm="1">
-        <f t="array" aca="1" ref="F187:G187" ca="1">_xlfn.TEXTSPLIT(E187,"|")</f>
+        <f t="array" aca="1" ref="F187:G187" ca="1">_xlfn.LET(_xlpm.z,_xlfn.TEXTSPLIT(E187,"|"),_xlfn.HSTACK(_xlfn.TAKE(_xlpm.z,,1),_xlfn.TAKE(_xlpm.z,,-1)+0))</f>
         <v>Output E</v>
       </c>
-      <c r="G187" s="5" t="str">
+      <c r="G187" s="5">
         <f ca="1"/>
         <v>45523</v>
       </c>
@@ -5825,10 +5833,10 @@
         <v>Output E|45523</v>
       </c>
       <c r="F188" s="5" t="str" cm="1">
-        <f t="array" aca="1" ref="F188:G188" ca="1">_xlfn.TEXTSPLIT(E188,"|")</f>
+        <f t="array" aca="1" ref="F188:G188" ca="1">_xlfn.LET(_xlpm.z,_xlfn.TEXTSPLIT(E188,"|"),_xlfn.HSTACK(_xlfn.TAKE(_xlpm.z,,1),_xlfn.TAKE(_xlpm.z,,-1)+0))</f>
         <v>Output E</v>
       </c>
-      <c r="G188" s="5" t="str">
+      <c r="G188" s="5">
         <f ca="1"/>
         <v>45523</v>
       </c>
@@ -5846,10 +5854,10 @@
         <v>Output E|45523</v>
       </c>
       <c r="F189" s="5" t="str" cm="1">
-        <f t="array" aca="1" ref="F189:G189" ca="1">_xlfn.TEXTSPLIT(E189,"|")</f>
+        <f t="array" aca="1" ref="F189:G189" ca="1">_xlfn.LET(_xlpm.z,_xlfn.TEXTSPLIT(E189,"|"),_xlfn.HSTACK(_xlfn.TAKE(_xlpm.z,,1),_xlfn.TAKE(_xlpm.z,,-1)+0))</f>
         <v>Output E</v>
       </c>
-      <c r="G189" s="5" t="str">
+      <c r="G189" s="5">
         <f ca="1"/>
         <v>45523</v>
       </c>
@@ -5867,10 +5875,10 @@
         <v>Output E|45523</v>
       </c>
       <c r="F190" s="5" t="str" cm="1">
-        <f t="array" aca="1" ref="F190:G190" ca="1">_xlfn.TEXTSPLIT(E190,"|")</f>
+        <f t="array" aca="1" ref="F190:G190" ca="1">_xlfn.LET(_xlpm.z,_xlfn.TEXTSPLIT(E190,"|"),_xlfn.HSTACK(_xlfn.TAKE(_xlpm.z,,1),_xlfn.TAKE(_xlpm.z,,-1)+0))</f>
         <v>Output E</v>
       </c>
-      <c r="G190" s="5" t="str">
+      <c r="G190" s="5">
         <f ca="1"/>
         <v>45523</v>
       </c>
@@ -5888,10 +5896,10 @@
         <v>Output E|45523</v>
       </c>
       <c r="F191" s="5" t="str" cm="1">
-        <f t="array" aca="1" ref="F191:G191" ca="1">_xlfn.TEXTSPLIT(E191,"|")</f>
+        <f t="array" aca="1" ref="F191:G191" ca="1">_xlfn.LET(_xlpm.z,_xlfn.TEXTSPLIT(E191,"|"),_xlfn.HSTACK(_xlfn.TAKE(_xlpm.z,,1),_xlfn.TAKE(_xlpm.z,,-1)+0))</f>
         <v>Output E</v>
       </c>
-      <c r="G191" s="5" t="str">
+      <c r="G191" s="5">
         <f ca="1"/>
         <v>45523</v>
       </c>
@@ -5909,10 +5917,10 @@
         <v>Output E|45523</v>
       </c>
       <c r="F192" s="5" t="str" cm="1">
-        <f t="array" aca="1" ref="F192:G192" ca="1">_xlfn.TEXTSPLIT(E192,"|")</f>
+        <f t="array" aca="1" ref="F192:G192" ca="1">_xlfn.LET(_xlpm.z,_xlfn.TEXTSPLIT(E192,"|"),_xlfn.HSTACK(_xlfn.TAKE(_xlpm.z,,1),_xlfn.TAKE(_xlpm.z,,-1)+0))</f>
         <v>Output E</v>
       </c>
-      <c r="G192" s="5" t="str">
+      <c r="G192" s="5">
         <f ca="1"/>
         <v>45523</v>
       </c>
@@ -5930,10 +5938,10 @@
         <v>Output E|45523</v>
       </c>
       <c r="F193" s="5" t="str" cm="1">
-        <f t="array" aca="1" ref="F193:G193" ca="1">_xlfn.TEXTSPLIT(E193,"|")</f>
+        <f t="array" aca="1" ref="F193:G193" ca="1">_xlfn.LET(_xlpm.z,_xlfn.TEXTSPLIT(E193,"|"),_xlfn.HSTACK(_xlfn.TAKE(_xlpm.z,,1),_xlfn.TAKE(_xlpm.z,,-1)+0))</f>
         <v>Output E</v>
       </c>
-      <c r="G193" s="5" t="str">
+      <c r="G193" s="5">
         <f ca="1"/>
         <v>45523</v>
       </c>
@@ -5951,10 +5959,10 @@
         <v>Output E|45523</v>
       </c>
       <c r="F194" s="5" t="str" cm="1">
-        <f t="array" aca="1" ref="F194:G194" ca="1">_xlfn.TEXTSPLIT(E194,"|")</f>
+        <f t="array" aca="1" ref="F194:G194" ca="1">_xlfn.LET(_xlpm.z,_xlfn.TEXTSPLIT(E194,"|"),_xlfn.HSTACK(_xlfn.TAKE(_xlpm.z,,1),_xlfn.TAKE(_xlpm.z,,-1)+0))</f>
         <v>Output E</v>
       </c>
-      <c r="G194" s="5" t="str">
+      <c r="G194" s="5">
         <f ca="1"/>
         <v>45523</v>
       </c>
@@ -5972,10 +5980,10 @@
         <v>Output E|45523</v>
       </c>
       <c r="F195" s="5" t="str" cm="1">
-        <f t="array" aca="1" ref="F195:G195" ca="1">_xlfn.TEXTSPLIT(E195,"|")</f>
+        <f t="array" aca="1" ref="F195:G195" ca="1">_xlfn.LET(_xlpm.z,_xlfn.TEXTSPLIT(E195,"|"),_xlfn.HSTACK(_xlfn.TAKE(_xlpm.z,,1),_xlfn.TAKE(_xlpm.z,,-1)+0))</f>
         <v>Output E</v>
       </c>
-      <c r="G195" s="5" t="str">
+      <c r="G195" s="5">
         <f ca="1"/>
         <v>45523</v>
       </c>
@@ -5993,10 +6001,10 @@
         <v>Output E|45523</v>
       </c>
       <c r="F196" s="5" t="str" cm="1">
-        <f t="array" aca="1" ref="F196:G196" ca="1">_xlfn.TEXTSPLIT(E196,"|")</f>
+        <f t="array" aca="1" ref="F196:G196" ca="1">_xlfn.LET(_xlpm.z,_xlfn.TEXTSPLIT(E196,"|"),_xlfn.HSTACK(_xlfn.TAKE(_xlpm.z,,1),_xlfn.TAKE(_xlpm.z,,-1)+0))</f>
         <v>Output E</v>
       </c>
-      <c r="G196" s="5" t="str">
+      <c r="G196" s="5">
         <f ca="1"/>
         <v>45523</v>
       </c>
@@ -6014,10 +6022,10 @@
         <v>Output E|45523</v>
       </c>
       <c r="F197" s="5" t="str" cm="1">
-        <f t="array" aca="1" ref="F197:G197" ca="1">_xlfn.TEXTSPLIT(E197,"|")</f>
+        <f t="array" aca="1" ref="F197:G197" ca="1">_xlfn.LET(_xlpm.z,_xlfn.TEXTSPLIT(E197,"|"),_xlfn.HSTACK(_xlfn.TAKE(_xlpm.z,,1),_xlfn.TAKE(_xlpm.z,,-1)+0))</f>
         <v>Output E</v>
       </c>
-      <c r="G197" s="5" t="str">
+      <c r="G197" s="5">
         <f ca="1"/>
         <v>45523</v>
       </c>
@@ -6035,10 +6043,10 @@
         <v>Output E|45523</v>
       </c>
       <c r="F198" s="5" t="str" cm="1">
-        <f t="array" aca="1" ref="F198:G198" ca="1">_xlfn.TEXTSPLIT(E198,"|")</f>
+        <f t="array" aca="1" ref="F198:G198" ca="1">_xlfn.LET(_xlpm.z,_xlfn.TEXTSPLIT(E198,"|"),_xlfn.HSTACK(_xlfn.TAKE(_xlpm.z,,1),_xlfn.TAKE(_xlpm.z,,-1)+0))</f>
         <v>Output E</v>
       </c>
-      <c r="G198" s="5" t="str">
+      <c r="G198" s="5">
         <f ca="1"/>
         <v>45523</v>
       </c>
@@ -6056,10 +6064,10 @@
         <v>Output E|45523</v>
       </c>
       <c r="F199" s="5" t="str" cm="1">
-        <f t="array" aca="1" ref="F199:G199" ca="1">_xlfn.TEXTSPLIT(E199,"|")</f>
+        <f t="array" aca="1" ref="F199:G199" ca="1">_xlfn.LET(_xlpm.z,_xlfn.TEXTSPLIT(E199,"|"),_xlfn.HSTACK(_xlfn.TAKE(_xlpm.z,,1),_xlfn.TAKE(_xlpm.z,,-1)+0))</f>
         <v>Output E</v>
       </c>
-      <c r="G199" s="5" t="str">
+      <c r="G199" s="5">
         <f ca="1"/>
         <v>45523</v>
       </c>
@@ -6077,10 +6085,10 @@
         <v>Output E|45523</v>
       </c>
       <c r="F200" s="5" t="str" cm="1">
-        <f t="array" aca="1" ref="F200:G200" ca="1">_xlfn.TEXTSPLIT(E200,"|")</f>
+        <f t="array" aca="1" ref="F200:G200" ca="1">_xlfn.LET(_xlpm.z,_xlfn.TEXTSPLIT(E200,"|"),_xlfn.HSTACK(_xlfn.TAKE(_xlpm.z,,1),_xlfn.TAKE(_xlpm.z,,-1)+0))</f>
         <v>Output E</v>
       </c>
-      <c r="G200" s="5" t="str">
+      <c r="G200" s="5">
         <f ca="1"/>
         <v>45523</v>
       </c>
@@ -6098,10 +6106,10 @@
         <v>Output E|45523</v>
       </c>
       <c r="F201" s="5" t="str" cm="1">
-        <f t="array" aca="1" ref="F201:G201" ca="1">_xlfn.TEXTSPLIT(E201,"|")</f>
+        <f t="array" aca="1" ref="F201:G201" ca="1">_xlfn.LET(_xlpm.z,_xlfn.TEXTSPLIT(E201,"|"),_xlfn.HSTACK(_xlfn.TAKE(_xlpm.z,,1),_xlfn.TAKE(_xlpm.z,,-1)+0))</f>
         <v>Output E</v>
       </c>
-      <c r="G201" s="5" t="str">
+      <c r="G201" s="5">
         <f ca="1"/>
         <v>45523</v>
       </c>
@@ -6119,10 +6127,10 @@
         <v>Output E|45523</v>
       </c>
       <c r="F202" s="5" t="str" cm="1">
-        <f t="array" aca="1" ref="F202:G202" ca="1">_xlfn.TEXTSPLIT(E202,"|")</f>
+        <f t="array" aca="1" ref="F202:G202" ca="1">_xlfn.LET(_xlpm.z,_xlfn.TEXTSPLIT(E202,"|"),_xlfn.HSTACK(_xlfn.TAKE(_xlpm.z,,1),_xlfn.TAKE(_xlpm.z,,-1)+0))</f>
         <v>Output E</v>
       </c>
-      <c r="G202" s="5" t="str">
+      <c r="G202" s="5">
         <f ca="1"/>
         <v>45523</v>
       </c>
@@ -6140,10 +6148,10 @@
         <v>Output E|45523</v>
       </c>
       <c r="F203" s="5" t="str" cm="1">
-        <f t="array" aca="1" ref="F203:G203" ca="1">_xlfn.TEXTSPLIT(E203,"|")</f>
+        <f t="array" aca="1" ref="F203:G203" ca="1">_xlfn.LET(_xlpm.z,_xlfn.TEXTSPLIT(E203,"|"),_xlfn.HSTACK(_xlfn.TAKE(_xlpm.z,,1),_xlfn.TAKE(_xlpm.z,,-1)+0))</f>
         <v>Output E</v>
       </c>
-      <c r="G203" s="5" t="str">
+      <c r="G203" s="5">
         <f ca="1"/>
         <v>45523</v>
       </c>
@@ -6161,10 +6169,10 @@
         <v>Output E|45523</v>
       </c>
       <c r="F204" s="5" t="str" cm="1">
-        <f t="array" aca="1" ref="F204:G204" ca="1">_xlfn.TEXTSPLIT(E204,"|")</f>
+        <f t="array" aca="1" ref="F204:G204" ca="1">_xlfn.LET(_xlpm.z,_xlfn.TEXTSPLIT(E204,"|"),_xlfn.HSTACK(_xlfn.TAKE(_xlpm.z,,1),_xlfn.TAKE(_xlpm.z,,-1)+0))</f>
         <v>Output E</v>
       </c>
-      <c r="G204" s="5" t="str">
+      <c r="G204" s="5">
         <f ca="1"/>
         <v>45523</v>
       </c>
@@ -6182,10 +6190,10 @@
         <v>Output E|45523</v>
       </c>
       <c r="F205" s="5" t="str" cm="1">
-        <f t="array" aca="1" ref="F205:G205" ca="1">_xlfn.TEXTSPLIT(E205,"|")</f>
+        <f t="array" aca="1" ref="F205:G205" ca="1">_xlfn.LET(_xlpm.z,_xlfn.TEXTSPLIT(E205,"|"),_xlfn.HSTACK(_xlfn.TAKE(_xlpm.z,,1),_xlfn.TAKE(_xlpm.z,,-1)+0))</f>
         <v>Output E</v>
       </c>
-      <c r="G205" s="5" t="str">
+      <c r="G205" s="5">
         <f ca="1"/>
         <v>45523</v>
       </c>

</xml_diff>